<commit_message>
Refactored to map variable names form different investegators to match DataModel
</commit_message>
<xml_diff>
--- a/config/SFN_NHP_Coordinates_All.xlsx
+++ b/config/SFN_NHP_Coordinates_All.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="460" windowWidth="23000" windowHeight="14760" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="1100" yWindow="460" windowWidth="23000" windowHeight="14760" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Br" sheetId="2" r:id="rId1"/>
@@ -1357,8 +1357,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="189">
+  <cellStyleXfs count="193">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1669,7 +1673,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="189">
+  <cellStyles count="193">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1764,6 +1768,8 @@
     <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1858,6 +1864,8 @@
     <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2138,7 +2146,7 @@
   </sheetPr>
   <dimension ref="A1:Z23"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="H1" workbookViewId="0">
       <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
@@ -4088,8 +4096,8 @@
   </sheetPr>
   <dimension ref="A1:Z20"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M29" sqref="M29"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5770,8 +5778,8 @@
   </sheetPr>
   <dimension ref="A1:AA89"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8562,7 +8570,7 @@
     <col min="8" max="8" width="29.1640625" customWidth="1"/>
     <col min="9" max="9" width="72.6640625" customWidth="1"/>
     <col min="10" max="10" width="42.6640625" customWidth="1"/>
-    <col min="11" max="11" width="27.83203125" customWidth="1"/>
+    <col min="11" max="11" width="24.33203125" customWidth="1"/>
     <col min="12" max="12" width="48.33203125" customWidth="1"/>
     <col min="13" max="13" width="14" customWidth="1"/>
     <col min="22" max="24" width="30" customWidth="1"/>
@@ -10740,7 +10748,7 @@
   </sheetPr>
   <dimension ref="A1:AB37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+    <sheetView topLeftCell="J1" workbookViewId="0">
       <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added probeNo to excel for Da_K, uodated outout file name
</commit_message>
<xml_diff>
--- a/config/SFN_NHP_Coordinates_All.xlsx
+++ b/config/SFN_NHP_Coordinates_All.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27011"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elseyjg/temp/schalllab-spatial/config/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/subravcr/Projects/lab-schall/schalllab-spatial/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="24500" windowHeight="19940" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="1400" yWindow="1260" windowWidth="50860" windowHeight="25500" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Br" sheetId="2" r:id="rId1"/>
     <sheet name="Jo" sheetId="1" r:id="rId2"/>
     <sheet name="Da_WJ" sheetId="6" r:id="rId3"/>
     <sheet name="Da_K" sheetId="7" r:id="rId4"/>
-    <sheet name="Ga" sheetId="4" r:id="rId5"/>
-    <sheet name="He" sheetId="5" r:id="rId6"/>
+    <sheet name="TestDarwin" sheetId="8" r:id="rId5"/>
+    <sheet name="Ga" sheetId="4" r:id="rId6"/>
+    <sheet name="He" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1584" uniqueCount="393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1676" uniqueCount="394">
   <si>
     <t>a3</t>
   </si>
@@ -1211,6 +1212,9 @@
   </si>
   <si>
     <t>Users/Kaleb/dataProcessed/Init_SetUp-161005-134520/Channel*/chan*.mat</t>
+  </si>
+  <si>
+    <t>probeNo</t>
   </si>
 </sst>
 </file>
@@ -1333,8 +1337,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="191">
+  <cellStyleXfs count="193">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1647,7 +1653,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="191">
+  <cellStyles count="193">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1743,6 +1749,7 @@
     <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1838,6 +1845,7 @@
     <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -8401,27 +8409,30 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA53"/>
+  <dimension ref="A1:AB53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="8" max="8" width="29.1640625" customWidth="1"/>
     <col min="9" max="9" width="72.6640625" customWidth="1"/>
-    <col min="10" max="10" width="42.6640625" customWidth="1"/>
-    <col min="11" max="11" width="27.83203125" customWidth="1"/>
-    <col min="12" max="12" width="14" customWidth="1"/>
-    <col min="14" max="14" width="18.83203125" customWidth="1"/>
-    <col min="21" max="23" width="30" customWidth="1"/>
-    <col min="24" max="24" width="19" customWidth="1"/>
-    <col min="25" max="25" width="105.5" customWidth="1"/>
-    <col min="26" max="27" width="30" customWidth="1"/>
+    <col min="10" max="10" width="13.83203125" customWidth="1"/>
+    <col min="11" max="11" width="42.6640625" customWidth="1"/>
+    <col min="12" max="12" width="22.83203125" customWidth="1"/>
+    <col min="13" max="13" width="14" customWidth="1"/>
+    <col min="15" max="15" width="18.83203125" customWidth="1"/>
+    <col min="22" max="22" width="20.5" customWidth="1"/>
+    <col min="23" max="23" width="17.1640625" customWidth="1"/>
+    <col min="24" max="24" width="19.1640625" customWidth="1"/>
+    <col min="25" max="25" width="16.1640625" customWidth="1"/>
+    <col min="26" max="26" width="105.5" customWidth="1"/>
+    <col min="27" max="28" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:28" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>74</v>
       </c>
@@ -8450,61 +8461,64 @@
         <v>94</v>
       </c>
       <c r="J1" s="6" t="s">
+        <v>393</v>
+      </c>
+      <c r="K1" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="M1" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="O1" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="P1" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="Q1" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="R1" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="S1" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="S1" s="6" t="s">
+      <c r="T1" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="T1" s="6" t="s">
+      <c r="U1" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="U1" s="6" t="s">
+      <c r="V1" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="V1" s="6" t="s">
+      <c r="W1" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="W1" s="6" t="s">
+      <c r="X1" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="X1" s="6" t="s">
+      <c r="Y1" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="Y1" s="6" t="s">
+      <c r="Z1" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="Z1" s="6" t="s">
+      <c r="AA1" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="AA1" s="6" t="s">
+      <c r="AB1" s="6" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>111</v>
       </c>
@@ -8532,63 +8546,66 @@
       <c r="I2" s="7" t="s">
         <v>378</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="7">
+        <v>1</v>
+      </c>
+      <c r="K2" s="7" t="s">
         <v>291</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="L2" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="M2" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="M2" s="7" t="s">
+      <c r="N2" s="7" t="s">
         <v>87</v>
-      </c>
-      <c r="N2" s="7" t="s">
-        <v>3</v>
       </c>
       <c r="O2" s="7" t="s">
         <v>3</v>
       </c>
       <c r="P2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q2" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="Q2" s="27" t="s">
+      <c r="R2" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="R2" s="27" t="s">
+      <c r="S2" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="S2" s="31">
+      <c r="T2" s="31">
         <v>3</v>
       </c>
-      <c r="T2" s="31">
+      <c r="U2" s="31">
         <v>-2</v>
       </c>
-      <c r="U2" s="35">
+      <c r="V2" s="35">
         <v>17200</v>
       </c>
-      <c r="V2" s="35">
+      <c r="W2" s="35">
         <v>21000</v>
       </c>
-      <c r="W2" s="36">
-        <f>V2-U2</f>
+      <c r="X2" s="36">
+        <f>W2-V2</f>
         <v>3800</v>
       </c>
-      <c r="X2" s="27">
+      <c r="Y2" s="27">
         <v>150</v>
       </c>
-      <c r="Y2" s="33" t="s">
+      <c r="Z2" s="33" t="s">
         <v>114</v>
       </c>
-      <c r="Z2" s="7">
+      <c r="AA2" s="7">
         <v>1</v>
       </c>
-      <c r="AA2" s="27">
+      <c r="AB2" s="27">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>111</v>
       </c>
@@ -8616,63 +8633,66 @@
       <c r="I3" s="7" t="s">
         <v>375</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="J3" s="7">
+        <v>1</v>
+      </c>
+      <c r="K3" s="7" t="s">
         <v>292</v>
       </c>
-      <c r="K3" s="7" t="s">
+      <c r="L3" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="L3" s="7" t="s">
+      <c r="M3" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="M3" s="7" t="s">
+      <c r="N3" s="7" t="s">
         <v>87</v>
-      </c>
-      <c r="N3" s="7" t="s">
-        <v>3</v>
       </c>
       <c r="O3" s="7" t="s">
         <v>3</v>
       </c>
       <c r="P3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q3" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="Q3" s="27" t="s">
+      <c r="R3" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="R3" s="27" t="s">
+      <c r="S3" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="S3" s="31">
+      <c r="T3" s="31">
         <v>3</v>
       </c>
-      <c r="T3" s="31">
+      <c r="U3" s="31">
         <v>-2</v>
       </c>
-      <c r="U3" s="35">
+      <c r="V3" s="35">
         <v>17200</v>
       </c>
-      <c r="V3" s="35">
+      <c r="W3" s="35">
         <v>21000</v>
       </c>
-      <c r="W3" s="36">
-        <f t="shared" ref="W3:W24" si="0">V3-U3</f>
+      <c r="X3" s="36">
+        <f t="shared" ref="X3:X24" si="0">W3-V3</f>
         <v>3800</v>
       </c>
-      <c r="X3" s="27">
+      <c r="Y3" s="27">
         <v>150</v>
       </c>
-      <c r="Y3" s="33" t="s">
+      <c r="Z3" s="33" t="s">
         <v>114</v>
       </c>
-      <c r="Z3" s="7">
+      <c r="AA3" s="7">
         <v>1</v>
       </c>
-      <c r="AA3" s="27">
+      <c r="AB3" s="27">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>111</v>
       </c>
@@ -8700,63 +8720,66 @@
       <c r="I4" s="7" t="s">
         <v>376</v>
       </c>
-      <c r="J4" s="7" t="s">
+      <c r="J4" s="7">
+        <v>1</v>
+      </c>
+      <c r="K4" s="7" t="s">
         <v>293</v>
       </c>
-      <c r="K4" s="7" t="s">
+      <c r="L4" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="L4" s="7" t="s">
+      <c r="M4" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="M4" s="7" t="s">
+      <c r="N4" s="7" t="s">
         <v>87</v>
-      </c>
-      <c r="N4" s="7" t="s">
-        <v>3</v>
       </c>
       <c r="O4" s="7" t="s">
         <v>3</v>
       </c>
       <c r="P4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q4" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="Q4" s="27" t="s">
+      <c r="R4" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="R4" s="27" t="s">
+      <c r="S4" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="S4" s="31">
+      <c r="T4" s="31">
         <v>3</v>
       </c>
-      <c r="T4" s="31">
+      <c r="U4" s="31">
         <v>-1</v>
       </c>
-      <c r="U4" s="35">
+      <c r="V4" s="35">
         <v>17200</v>
       </c>
-      <c r="V4" s="35">
+      <c r="W4" s="35">
         <v>21500</v>
       </c>
-      <c r="W4" s="36">
+      <c r="X4" s="36">
         <f t="shared" si="0"/>
         <v>4300</v>
       </c>
-      <c r="X4" s="27">
+      <c r="Y4" s="27">
         <v>150</v>
       </c>
-      <c r="Y4" s="33" t="s">
+      <c r="Z4" s="33" t="s">
         <v>114</v>
       </c>
-      <c r="Z4" s="7">
+      <c r="AA4" s="7">
         <v>1</v>
       </c>
-      <c r="AA4" s="27">
+      <c r="AB4" s="27">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>111</v>
       </c>
@@ -8784,63 +8807,66 @@
       <c r="I5" s="7" t="s">
         <v>377</v>
       </c>
-      <c r="J5" s="7" t="s">
+      <c r="J5" s="7">
+        <v>1</v>
+      </c>
+      <c r="K5" s="7" t="s">
         <v>294</v>
       </c>
-      <c r="K5" s="7" t="s">
+      <c r="L5" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="L5" s="7" t="s">
+      <c r="M5" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="M5" s="7" t="s">
+      <c r="N5" s="7" t="s">
         <v>87</v>
-      </c>
-      <c r="N5" s="7" t="s">
-        <v>3</v>
       </c>
       <c r="O5" s="7" t="s">
         <v>3</v>
       </c>
       <c r="P5" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q5" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="Q5" s="27" t="s">
+      <c r="R5" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="R5" s="27" t="s">
+      <c r="S5" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="S5" s="31">
+      <c r="T5" s="31">
         <v>2</v>
       </c>
-      <c r="T5" s="31">
+      <c r="U5" s="31">
         <v>-2</v>
       </c>
-      <c r="U5" s="35">
+      <c r="V5" s="35">
         <v>18000</v>
       </c>
-      <c r="V5" s="35">
+      <c r="W5" s="35">
         <v>22000</v>
       </c>
-      <c r="W5" s="36">
+      <c r="X5" s="36">
         <f t="shared" si="0"/>
         <v>4000</v>
       </c>
-      <c r="X5" s="27">
+      <c r="Y5" s="27">
         <v>150</v>
       </c>
-      <c r="Y5" s="33" t="s">
+      <c r="Z5" s="33" t="s">
         <v>114</v>
       </c>
-      <c r="Z5" s="7">
+      <c r="AA5" s="7">
         <v>1</v>
       </c>
-      <c r="AA5" s="27">
+      <c r="AB5" s="27">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>111</v>
       </c>
@@ -8868,63 +8894,66 @@
       <c r="I6" s="7" t="s">
         <v>379</v>
       </c>
-      <c r="J6" s="7" t="s">
+      <c r="J6" s="7">
+        <v>1</v>
+      </c>
+      <c r="K6" s="7" t="s">
         <v>295</v>
       </c>
-      <c r="K6" s="7" t="s">
+      <c r="L6" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="L6" s="7" t="s">
+      <c r="M6" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="M6" s="7" t="s">
+      <c r="N6" s="7" t="s">
         <v>87</v>
-      </c>
-      <c r="N6" s="7" t="s">
-        <v>3</v>
       </c>
       <c r="O6" s="7" t="s">
         <v>3</v>
       </c>
       <c r="P6" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q6" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="Q6" s="27" t="s">
+      <c r="R6" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="R6" s="27" t="s">
+      <c r="S6" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="S6" s="31">
+      <c r="T6" s="31">
         <v>2</v>
       </c>
-      <c r="T6" s="34">
+      <c r="U6" s="34">
         <v>-2</v>
       </c>
-      <c r="U6" s="36">
+      <c r="V6" s="36">
         <v>18000</v>
       </c>
-      <c r="V6" s="36">
+      <c r="W6" s="36">
         <v>25000</v>
       </c>
-      <c r="W6" s="36">
+      <c r="X6" s="36">
         <f t="shared" si="0"/>
         <v>7000</v>
       </c>
-      <c r="X6" s="27">
+      <c r="Y6" s="27">
         <v>150</v>
       </c>
-      <c r="Y6" s="33" t="s">
+      <c r="Z6" s="33" t="s">
         <v>114</v>
       </c>
-      <c r="Z6" s="7">
+      <c r="AA6" s="7">
         <v>1</v>
       </c>
-      <c r="AA6" s="27">
+      <c r="AB6" s="27">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>111</v>
       </c>
@@ -8952,63 +8981,66 @@
       <c r="I7" s="7" t="s">
         <v>380</v>
       </c>
-      <c r="J7" s="7" t="s">
+      <c r="J7" s="7">
+        <v>1</v>
+      </c>
+      <c r="K7" s="7" t="s">
         <v>296</v>
       </c>
-      <c r="K7" s="7" t="s">
+      <c r="L7" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="L7" s="7" t="s">
+      <c r="M7" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="M7" s="7" t="s">
+      <c r="N7" s="7" t="s">
         <v>87</v>
-      </c>
-      <c r="N7" s="7" t="s">
-        <v>3</v>
       </c>
       <c r="O7" s="7" t="s">
         <v>3</v>
       </c>
       <c r="P7" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q7" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="Q7" s="27" t="s">
+      <c r="R7" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="R7" s="27" t="s">
+      <c r="S7" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="S7" s="31">
+      <c r="T7" s="31">
         <v>3</v>
       </c>
-      <c r="T7" s="31">
+      <c r="U7" s="31">
         <v>-2</v>
       </c>
-      <c r="U7" s="35">
+      <c r="V7" s="35">
         <v>18000</v>
       </c>
-      <c r="V7" s="35">
+      <c r="W7" s="35">
         <v>22000</v>
       </c>
-      <c r="W7" s="36">
+      <c r="X7" s="36">
         <f t="shared" si="0"/>
         <v>4000</v>
       </c>
-      <c r="X7" s="27">
+      <c r="Y7" s="27">
         <v>150</v>
       </c>
-      <c r="Y7" s="33" t="s">
+      <c r="Z7" s="33" t="s">
         <v>114</v>
       </c>
-      <c r="Z7" s="7">
+      <c r="AA7" s="7">
         <v>1</v>
       </c>
-      <c r="AA7" s="27">
+      <c r="AB7" s="27">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>111</v>
       </c>
@@ -9036,63 +9068,66 @@
       <c r="I8" s="7" t="s">
         <v>381</v>
       </c>
-      <c r="J8" s="7" t="s">
+      <c r="J8" s="7">
+        <v>1</v>
+      </c>
+      <c r="K8" s="7" t="s">
         <v>297</v>
       </c>
-      <c r="K8" s="7" t="s">
+      <c r="L8" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="L8" s="7" t="s">
+      <c r="M8" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="M8" s="7" t="s">
+      <c r="N8" s="7" t="s">
         <v>87</v>
-      </c>
-      <c r="N8" s="7" t="s">
-        <v>3</v>
       </c>
       <c r="O8" s="7" t="s">
         <v>3</v>
       </c>
       <c r="P8" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q8" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="Q8" s="27" t="s">
+      <c r="R8" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="R8" s="27" t="s">
+      <c r="S8" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="S8" s="31">
+      <c r="T8" s="31">
         <v>4</v>
       </c>
-      <c r="T8" s="31">
+      <c r="U8" s="31">
         <v>-2</v>
       </c>
-      <c r="U8" s="35">
+      <c r="V8" s="35">
         <v>18000</v>
       </c>
-      <c r="V8" s="35">
+      <c r="W8" s="35">
         <v>25000</v>
       </c>
-      <c r="W8" s="36">
+      <c r="X8" s="36">
         <f t="shared" si="0"/>
         <v>7000</v>
       </c>
-      <c r="X8" s="27">
+      <c r="Y8" s="27">
         <v>150</v>
       </c>
-      <c r="Y8" s="33" t="s">
+      <c r="Z8" s="33" t="s">
         <v>114</v>
       </c>
-      <c r="Z8" s="7">
+      <c r="AA8" s="7">
         <v>1</v>
       </c>
-      <c r="AA8" s="27">
+      <c r="AB8" s="27">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>111</v>
       </c>
@@ -9120,63 +9155,66 @@
       <c r="I9" s="7" t="s">
         <v>382</v>
       </c>
-      <c r="J9" s="7" t="s">
+      <c r="J9" s="7">
+        <v>1</v>
+      </c>
+      <c r="K9" s="7" t="s">
         <v>298</v>
       </c>
-      <c r="K9" s="7" t="s">
+      <c r="L9" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="L9" s="7" t="s">
+      <c r="M9" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="M9" s="7" t="s">
+      <c r="N9" s="7" t="s">
         <v>87</v>
-      </c>
-      <c r="N9" s="7" t="s">
-        <v>3</v>
       </c>
       <c r="O9" s="7" t="s">
         <v>3</v>
       </c>
       <c r="P9" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q9" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="Q9" s="27" t="s">
+      <c r="R9" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="R9" s="27" t="s">
+      <c r="S9" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="S9" s="31">
+      <c r="T9" s="31">
         <v>4</v>
       </c>
-      <c r="T9" s="31">
+      <c r="U9" s="31">
         <v>-1</v>
       </c>
-      <c r="U9" s="35">
+      <c r="V9" s="35">
         <v>18000</v>
       </c>
-      <c r="V9" s="35">
+      <c r="W9" s="35">
         <v>25000</v>
       </c>
-      <c r="W9" s="36">
+      <c r="X9" s="36">
         <f t="shared" si="0"/>
         <v>7000</v>
       </c>
-      <c r="X9" s="27">
+      <c r="Y9" s="27">
         <v>150</v>
       </c>
-      <c r="Y9" s="33" t="s">
+      <c r="Z9" s="33" t="s">
         <v>114</v>
       </c>
-      <c r="Z9" s="7">
+      <c r="AA9" s="7">
         <v>1</v>
       </c>
-      <c r="AA9" s="27">
+      <c r="AB9" s="27">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>111</v>
       </c>
@@ -9204,63 +9242,66 @@
       <c r="I10" s="7" t="s">
         <v>383</v>
       </c>
-      <c r="J10" s="7" t="s">
+      <c r="J10" s="7">
+        <v>1</v>
+      </c>
+      <c r="K10" s="7" t="s">
         <v>299</v>
       </c>
-      <c r="K10" s="7" t="s">
+      <c r="L10" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="L10" s="7" t="s">
+      <c r="M10" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="M10" s="7" t="s">
+      <c r="N10" s="7" t="s">
         <v>87</v>
-      </c>
-      <c r="N10" s="7" t="s">
-        <v>3</v>
       </c>
       <c r="O10" s="7" t="s">
         <v>3</v>
       </c>
       <c r="P10" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q10" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="Q10" s="27" t="s">
+      <c r="R10" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="R10" s="27" t="s">
+      <c r="S10" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="S10" s="31">
+      <c r="T10" s="31">
         <v>4</v>
       </c>
-      <c r="T10" s="31">
+      <c r="U10" s="31">
         <v>-1</v>
       </c>
-      <c r="U10" s="35">
+      <c r="V10" s="35">
         <v>18000</v>
       </c>
-      <c r="V10" s="35">
+      <c r="W10" s="35">
         <v>23800</v>
       </c>
-      <c r="W10" s="36">
+      <c r="X10" s="36">
         <f t="shared" si="0"/>
         <v>5800</v>
       </c>
-      <c r="X10" s="27">
+      <c r="Y10" s="27">
         <v>150</v>
       </c>
-      <c r="Y10" s="33" t="s">
+      <c r="Z10" s="33" t="s">
         <v>114</v>
       </c>
-      <c r="Z10" s="7">
+      <c r="AA10" s="7">
         <v>1</v>
       </c>
-      <c r="AA10" s="27">
+      <c r="AB10" s="27">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>111</v>
       </c>
@@ -9288,63 +9329,66 @@
       <c r="I11" s="7" t="s">
         <v>384</v>
       </c>
-      <c r="J11" s="7" t="s">
+      <c r="J11" s="7">
+        <v>1</v>
+      </c>
+      <c r="K11" s="7" t="s">
         <v>300</v>
       </c>
-      <c r="K11" s="7" t="s">
+      <c r="L11" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="L11" s="7" t="s">
+      <c r="M11" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="M11" s="7" t="s">
+      <c r="N11" s="7" t="s">
         <v>87</v>
-      </c>
-      <c r="N11" s="7" t="s">
-        <v>3</v>
       </c>
       <c r="O11" s="7" t="s">
         <v>3</v>
       </c>
       <c r="P11" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q11" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="Q11" s="27" t="s">
+      <c r="R11" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="R11" s="27" t="s">
+      <c r="S11" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="S11" s="31">
+      <c r="T11" s="31">
         <v>4</v>
       </c>
-      <c r="T11" s="31">
+      <c r="U11" s="31">
         <v>-1</v>
       </c>
-      <c r="U11" s="35">
+      <c r="V11" s="35">
         <v>18000</v>
       </c>
-      <c r="V11" s="35">
+      <c r="W11" s="35">
         <v>26000</v>
       </c>
-      <c r="W11" s="36">
+      <c r="X11" s="36">
         <f t="shared" si="0"/>
         <v>8000</v>
       </c>
-      <c r="X11" s="27">
+      <c r="Y11" s="27">
         <v>150</v>
       </c>
-      <c r="Y11" s="33" t="s">
+      <c r="Z11" s="33" t="s">
         <v>114</v>
       </c>
-      <c r="Z11" s="7">
+      <c r="AA11" s="7">
         <v>1</v>
       </c>
-      <c r="AA11" s="27">
+      <c r="AB11" s="27">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>111</v>
       </c>
@@ -9372,63 +9416,66 @@
       <c r="I12" s="7" t="s">
         <v>385</v>
       </c>
-      <c r="J12" s="7" t="s">
+      <c r="J12" s="7">
+        <v>1</v>
+      </c>
+      <c r="K12" s="7" t="s">
         <v>301</v>
       </c>
-      <c r="K12" s="7" t="s">
+      <c r="L12" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="L12" s="7" t="s">
+      <c r="M12" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="M12" s="7" t="s">
+      <c r="N12" s="7" t="s">
         <v>87</v>
-      </c>
-      <c r="N12" s="7" t="s">
-        <v>3</v>
       </c>
       <c r="O12" s="7" t="s">
         <v>3</v>
       </c>
       <c r="P12" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q12" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="Q12" s="27" t="s">
+      <c r="R12" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="R12" s="27" t="s">
+      <c r="S12" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="S12" s="31">
+      <c r="T12" s="31">
         <v>4</v>
       </c>
-      <c r="T12" s="31">
+      <c r="U12" s="31">
         <v>3</v>
       </c>
-      <c r="U12" s="35">
+      <c r="V12" s="35">
         <v>18000</v>
       </c>
-      <c r="V12" s="35">
+      <c r="W12" s="35">
         <v>22000</v>
       </c>
-      <c r="W12" s="36">
+      <c r="X12" s="36">
         <f t="shared" si="0"/>
         <v>4000</v>
       </c>
-      <c r="X12" s="27">
+      <c r="Y12" s="27">
         <v>150</v>
       </c>
-      <c r="Y12" s="33" t="s">
+      <c r="Z12" s="33" t="s">
         <v>114</v>
       </c>
-      <c r="Z12" s="7">
+      <c r="AA12" s="7">
         <v>1</v>
       </c>
-      <c r="AA12" s="27">
+      <c r="AB12" s="27">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>111</v>
       </c>
@@ -9456,63 +9503,66 @@
       <c r="I13" s="7" t="s">
         <v>386</v>
       </c>
-      <c r="J13" s="7" t="s">
+      <c r="J13" s="7">
+        <v>1</v>
+      </c>
+      <c r="K13" s="7" t="s">
         <v>302</v>
       </c>
-      <c r="K13" s="7" t="s">
+      <c r="L13" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="L13" s="7" t="s">
+      <c r="M13" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="M13" s="7" t="s">
+      <c r="N13" s="7" t="s">
         <v>87</v>
-      </c>
-      <c r="N13" s="7" t="s">
-        <v>3</v>
       </c>
       <c r="O13" s="7" t="s">
         <v>3</v>
       </c>
       <c r="P13" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q13" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="Q13" s="27" t="s">
+      <c r="R13" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="R13" s="27" t="s">
+      <c r="S13" s="27" t="s">
         <v>9</v>
-      </c>
-      <c r="S13" s="31">
-        <v>2</v>
       </c>
       <c r="T13" s="31">
         <v>2</v>
       </c>
-      <c r="U13" s="35">
+      <c r="U13" s="31">
+        <v>2</v>
+      </c>
+      <c r="V13" s="35">
         <v>18000</v>
       </c>
-      <c r="V13" s="35">
+      <c r="W13" s="35">
         <v>23500</v>
       </c>
-      <c r="W13" s="36">
+      <c r="X13" s="36">
         <f t="shared" si="0"/>
         <v>5500</v>
       </c>
-      <c r="X13" s="27">
+      <c r="Y13" s="27">
         <v>150</v>
       </c>
-      <c r="Y13" s="33" t="s">
+      <c r="Z13" s="33" t="s">
         <v>114</v>
       </c>
-      <c r="Z13" s="7">
+      <c r="AA13" s="7">
         <v>1</v>
       </c>
-      <c r="AA13" s="27">
+      <c r="AB13" s="27">
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>111</v>
       </c>
@@ -9540,63 +9590,66 @@
       <c r="I14" s="7" t="s">
         <v>386</v>
       </c>
-      <c r="J14" s="7" t="s">
+      <c r="J14" s="7">
+        <v>2</v>
+      </c>
+      <c r="K14" s="7" t="s">
         <v>302</v>
       </c>
-      <c r="K14" s="7" t="s">
+      <c r="L14" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="L14" s="7" t="s">
+      <c r="M14" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="M14" s="7" t="s">
+      <c r="N14" s="7" t="s">
         <v>87</v>
-      </c>
-      <c r="N14" s="7" t="s">
-        <v>3</v>
       </c>
       <c r="O14" s="7" t="s">
         <v>3</v>
       </c>
       <c r="P14" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q14" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="Q14" s="27" t="s">
+      <c r="R14" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="R14" s="27" t="s">
+      <c r="S14" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="S14" s="31">
+      <c r="T14" s="31">
         <v>2</v>
       </c>
-      <c r="T14" s="31">
+      <c r="U14" s="31">
         <v>-1</v>
       </c>
-      <c r="U14" s="35">
+      <c r="V14" s="35">
         <v>15650</v>
       </c>
-      <c r="V14" s="35">
+      <c r="W14" s="35">
         <v>21500</v>
       </c>
-      <c r="W14" s="36">
+      <c r="X14" s="36">
         <f t="shared" si="0"/>
         <v>5850</v>
       </c>
-      <c r="X14" s="27">
+      <c r="Y14" s="27">
         <v>150</v>
       </c>
-      <c r="Y14" s="7" t="s">
+      <c r="Z14" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="Z14" s="7">
+      <c r="AA14" s="7">
         <v>33</v>
       </c>
-      <c r="AA14" s="27">
+      <c r="AB14" s="27">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
         <v>111</v>
       </c>
@@ -9624,63 +9677,66 @@
       <c r="I15" s="7" t="s">
         <v>387</v>
       </c>
-      <c r="J15" s="7" t="s">
+      <c r="J15" s="7">
+        <v>1</v>
+      </c>
+      <c r="K15" s="7" t="s">
         <v>303</v>
       </c>
-      <c r="K15" s="7" t="s">
+      <c r="L15" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="L15" s="7" t="s">
+      <c r="M15" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="M15" s="7" t="s">
+      <c r="N15" s="7" t="s">
         <v>87</v>
-      </c>
-      <c r="N15" s="7" t="s">
-        <v>3</v>
       </c>
       <c r="O15" s="7" t="s">
         <v>3</v>
       </c>
       <c r="P15" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q15" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="Q15" s="27" t="s">
+      <c r="R15" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="R15" s="27" t="s">
+      <c r="S15" s="27" t="s">
         <v>9</v>
-      </c>
-      <c r="S15" s="31">
-        <v>2</v>
       </c>
       <c r="T15" s="31">
         <v>2</v>
       </c>
-      <c r="U15" s="35">
+      <c r="U15" s="31">
+        <v>2</v>
+      </c>
+      <c r="V15" s="35">
         <v>18000</v>
       </c>
-      <c r="V15" s="35">
+      <c r="W15" s="35">
         <v>25500</v>
       </c>
-      <c r="W15" s="36">
+      <c r="X15" s="36">
         <f t="shared" si="0"/>
         <v>7500</v>
       </c>
-      <c r="X15" s="27">
+      <c r="Y15" s="27">
         <v>150</v>
       </c>
-      <c r="Y15" s="33" t="s">
+      <c r="Z15" s="33" t="s">
         <v>114</v>
       </c>
-      <c r="Z15" s="7">
+      <c r="AA15" s="7">
         <v>1</v>
       </c>
-      <c r="AA15" s="27">
+      <c r="AB15" s="27">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
         <v>111</v>
       </c>
@@ -9708,63 +9764,66 @@
       <c r="I16" s="7" t="s">
         <v>387</v>
       </c>
-      <c r="J16" s="7" t="s">
+      <c r="J16" s="7">
+        <v>2</v>
+      </c>
+      <c r="K16" s="7" t="s">
         <v>303</v>
       </c>
-      <c r="K16" s="7" t="s">
+      <c r="L16" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="L16" s="7" t="s">
+      <c r="M16" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="M16" s="7" t="s">
+      <c r="N16" s="7" t="s">
         <v>87</v>
-      </c>
-      <c r="N16" s="7" t="s">
-        <v>3</v>
       </c>
       <c r="O16" s="7" t="s">
         <v>3</v>
       </c>
       <c r="P16" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q16" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="Q16" s="27" t="s">
+      <c r="R16" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="R16" s="27" t="s">
+      <c r="S16" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="S16" s="31">
+      <c r="T16" s="31">
         <v>2</v>
       </c>
-      <c r="T16" s="31">
+      <c r="U16" s="31">
         <v>-1</v>
       </c>
-      <c r="U16" s="35">
+      <c r="V16" s="35">
         <v>15650</v>
       </c>
-      <c r="V16" s="35">
+      <c r="W16" s="35">
         <v>21500</v>
       </c>
-      <c r="W16" s="36">
+      <c r="X16" s="36">
         <f t="shared" si="0"/>
         <v>5850</v>
       </c>
-      <c r="X16" s="27">
+      <c r="Y16" s="27">
         <v>150</v>
       </c>
-      <c r="Y16" s="7" t="s">
+      <c r="Z16" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="Z16" s="7">
+      <c r="AA16" s="7">
         <v>33</v>
       </c>
-      <c r="AA16" s="27">
+      <c r="AB16" s="27">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>111</v>
       </c>
@@ -9792,63 +9851,66 @@
       <c r="I17" s="7" t="s">
         <v>388</v>
       </c>
-      <c r="J17" s="7" t="s">
+      <c r="J17" s="7">
+        <v>1</v>
+      </c>
+      <c r="K17" s="7" t="s">
         <v>304</v>
       </c>
-      <c r="K17" s="7" t="s">
+      <c r="L17" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="L17" s="7" t="s">
+      <c r="M17" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="M17" s="7" t="s">
+      <c r="N17" s="7" t="s">
         <v>87</v>
-      </c>
-      <c r="N17" s="7" t="s">
-        <v>3</v>
       </c>
       <c r="O17" s="7" t="s">
         <v>3</v>
       </c>
       <c r="P17" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q17" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="Q17" s="27" t="s">
+      <c r="R17" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="R17" s="27" t="s">
+      <c r="S17" s="27" t="s">
         <v>10</v>
-      </c>
-      <c r="S17" s="31">
-        <v>0</v>
       </c>
       <c r="T17" s="31">
         <v>0</v>
       </c>
-      <c r="U17" s="35">
+      <c r="U17" s="31">
+        <v>0</v>
+      </c>
+      <c r="V17" s="35">
         <v>18000</v>
       </c>
-      <c r="V17" s="35">
+      <c r="W17" s="35">
         <v>19500</v>
       </c>
-      <c r="W17" s="36">
+      <c r="X17" s="36">
         <f t="shared" si="0"/>
         <v>1500</v>
       </c>
-      <c r="X17" s="27">
+      <c r="Y17" s="27">
         <v>150</v>
       </c>
-      <c r="Y17" s="33" t="s">
+      <c r="Z17" s="33" t="s">
         <v>114</v>
       </c>
-      <c r="Z17" s="7">
+      <c r="AA17" s="7">
         <v>1</v>
       </c>
-      <c r="AA17" s="27">
+      <c r="AB17" s="27">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>111</v>
       </c>
@@ -9876,63 +9938,66 @@
       <c r="I18" s="7" t="s">
         <v>388</v>
       </c>
-      <c r="J18" s="7" t="s">
+      <c r="J18" s="7">
+        <v>2</v>
+      </c>
+      <c r="K18" s="7" t="s">
         <v>304</v>
       </c>
-      <c r="K18" s="7" t="s">
+      <c r="L18" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="L18" s="7" t="s">
+      <c r="M18" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="M18" s="7" t="s">
+      <c r="N18" s="7" t="s">
         <v>87</v>
-      </c>
-      <c r="N18" s="7" t="s">
-        <v>3</v>
       </c>
       <c r="O18" s="7" t="s">
         <v>3</v>
       </c>
       <c r="P18" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q18" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="Q18" s="27" t="s">
+      <c r="R18" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="R18" s="27" t="s">
+      <c r="S18" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="S18" s="31">
+      <c r="T18" s="31">
         <v>2</v>
       </c>
-      <c r="T18" s="31">
+      <c r="U18" s="31">
         <v>-1</v>
       </c>
-      <c r="U18" s="35">
+      <c r="V18" s="35">
         <v>15650</v>
       </c>
-      <c r="V18" s="35">
+      <c r="W18" s="35">
         <v>24000</v>
       </c>
-      <c r="W18" s="36">
+      <c r="X18" s="36">
         <f t="shared" si="0"/>
         <v>8350</v>
       </c>
-      <c r="X18" s="27">
+      <c r="Y18" s="27">
         <v>150</v>
       </c>
-      <c r="Y18" s="7" t="s">
+      <c r="Z18" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="Z18" s="7">
+      <c r="AA18" s="7">
         <v>33</v>
       </c>
-      <c r="AA18" s="27">
+      <c r="AB18" s="27">
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>111</v>
       </c>
@@ -9960,63 +10025,66 @@
       <c r="I19" s="7" t="s">
         <v>389</v>
       </c>
-      <c r="J19" s="7" t="s">
+      <c r="J19" s="7">
+        <v>1</v>
+      </c>
+      <c r="K19" s="7" t="s">
         <v>305</v>
       </c>
-      <c r="K19" s="7" t="s">
+      <c r="L19" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="L19" s="7" t="s">
+      <c r="M19" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="M19" s="7" t="s">
+      <c r="N19" s="7" t="s">
         <v>87</v>
-      </c>
-      <c r="N19" s="7" t="s">
-        <v>3</v>
       </c>
       <c r="O19" s="7" t="s">
         <v>3</v>
       </c>
       <c r="P19" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q19" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="Q19" s="27" t="s">
+      <c r="R19" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="R19" s="27" t="s">
+      <c r="S19" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="S19" s="31">
+      <c r="T19" s="31">
         <v>0</v>
       </c>
-      <c r="T19" s="31">
+      <c r="U19" s="31">
         <v>-2</v>
       </c>
-      <c r="U19" s="35">
+      <c r="V19" s="35">
         <v>18000</v>
       </c>
-      <c r="V19" s="35">
+      <c r="W19" s="35">
         <v>18500</v>
       </c>
-      <c r="W19" s="36">
+      <c r="X19" s="36">
         <f t="shared" si="0"/>
         <v>500</v>
       </c>
-      <c r="X19" s="27">
+      <c r="Y19" s="27">
         <v>150</v>
       </c>
-      <c r="Y19" s="33" t="s">
+      <c r="Z19" s="33" t="s">
         <v>114</v>
       </c>
-      <c r="Z19" s="7">
+      <c r="AA19" s="7">
         <v>1</v>
       </c>
-      <c r="AA19" s="27">
+      <c r="AB19" s="27">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
         <v>111</v>
       </c>
@@ -10044,63 +10112,66 @@
       <c r="I20" s="7" t="s">
         <v>389</v>
       </c>
-      <c r="J20" s="7" t="s">
+      <c r="J20" s="7">
+        <v>2</v>
+      </c>
+      <c r="K20" s="7" t="s">
         <v>305</v>
       </c>
-      <c r="K20" s="7" t="s">
+      <c r="L20" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="L20" s="7" t="s">
+      <c r="M20" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="M20" s="7" t="s">
+      <c r="N20" s="7" t="s">
         <v>87</v>
-      </c>
-      <c r="N20" s="7" t="s">
-        <v>3</v>
       </c>
       <c r="O20" s="7" t="s">
         <v>3</v>
       </c>
       <c r="P20" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q20" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="Q20" s="27" t="s">
+      <c r="R20" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="R20" s="27" t="s">
+      <c r="S20" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="S20" s="31">
+      <c r="T20" s="31">
         <v>2</v>
       </c>
-      <c r="T20" s="31">
+      <c r="U20" s="31">
         <v>-2</v>
       </c>
-      <c r="U20" s="35">
+      <c r="V20" s="35">
         <v>15650</v>
       </c>
-      <c r="V20" s="35">
+      <c r="W20" s="35">
         <v>22300</v>
       </c>
-      <c r="W20" s="36">
+      <c r="X20" s="36">
         <f t="shared" si="0"/>
         <v>6650</v>
       </c>
-      <c r="X20" s="27">
+      <c r="Y20" s="27">
         <v>150</v>
       </c>
-      <c r="Y20" s="7" t="s">
+      <c r="Z20" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="Z20" s="7">
+      <c r="AA20" s="7">
         <v>33</v>
       </c>
-      <c r="AA20" s="27">
+      <c r="AB20" s="27">
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
         <v>111</v>
       </c>
@@ -10128,63 +10199,66 @@
       <c r="I21" s="7" t="s">
         <v>390</v>
       </c>
-      <c r="J21" s="7" t="s">
+      <c r="J21" s="7">
+        <v>1</v>
+      </c>
+      <c r="K21" s="7" t="s">
         <v>306</v>
       </c>
-      <c r="K21" s="7" t="s">
+      <c r="L21" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="L21" s="7" t="s">
+      <c r="M21" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="M21" s="7" t="s">
+      <c r="N21" s="7" t="s">
         <v>87</v>
-      </c>
-      <c r="N21" s="7" t="s">
-        <v>3</v>
       </c>
       <c r="O21" s="7" t="s">
         <v>3</v>
       </c>
       <c r="P21" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q21" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="Q21" s="27" t="s">
+      <c r="R21" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="R21" s="27" t="s">
+      <c r="S21" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="S21" s="31">
+      <c r="T21" s="31">
         <v>0</v>
       </c>
-      <c r="T21" s="31">
+      <c r="U21" s="31">
         <v>-2</v>
       </c>
-      <c r="U21" s="35">
+      <c r="V21" s="35">
         <v>18000</v>
       </c>
-      <c r="V21" s="35">
+      <c r="W21" s="35">
         <v>18500</v>
       </c>
-      <c r="W21" s="36">
+      <c r="X21" s="36">
         <f t="shared" si="0"/>
         <v>500</v>
       </c>
-      <c r="X21" s="27">
+      <c r="Y21" s="27">
         <v>150</v>
       </c>
-      <c r="Y21" s="33" t="s">
+      <c r="Z21" s="33" t="s">
         <v>114</v>
       </c>
-      <c r="Z21" s="7">
+      <c r="AA21" s="7">
         <v>1</v>
       </c>
-      <c r="AA21" s="27">
+      <c r="AB21" s="27">
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
         <v>111</v>
       </c>
@@ -10212,63 +10286,66 @@
       <c r="I22" s="7" t="s">
         <v>390</v>
       </c>
-      <c r="J22" s="7" t="s">
+      <c r="J22" s="7">
+        <v>2</v>
+      </c>
+      <c r="K22" s="7" t="s">
         <v>306</v>
       </c>
-      <c r="K22" s="7" t="s">
+      <c r="L22" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="L22" s="7" t="s">
+      <c r="M22" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="M22" s="7" t="s">
+      <c r="N22" s="7" t="s">
         <v>87</v>
-      </c>
-      <c r="N22" s="7" t="s">
-        <v>3</v>
       </c>
       <c r="O22" s="7" t="s">
         <v>3</v>
       </c>
       <c r="P22" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q22" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="Q22" s="27" t="s">
+      <c r="R22" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="R22" s="27" t="s">
+      <c r="S22" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="S22" s="31">
+      <c r="T22" s="31">
         <v>2</v>
       </c>
-      <c r="T22" s="31">
+      <c r="U22" s="31">
         <v>-2</v>
       </c>
-      <c r="U22" s="35">
+      <c r="V22" s="35">
         <v>15650</v>
       </c>
-      <c r="V22" s="35">
+      <c r="W22" s="35">
         <v>22300</v>
       </c>
-      <c r="W22" s="36">
+      <c r="X22" s="36">
         <f t="shared" si="0"/>
         <v>6650</v>
       </c>
-      <c r="X22" s="27">
+      <c r="Y22" s="27">
         <v>150</v>
       </c>
-      <c r="Y22" s="7" t="s">
+      <c r="Z22" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="Z22" s="7">
+      <c r="AA22" s="7">
         <v>33</v>
       </c>
-      <c r="AA22" s="27">
+      <c r="AB22" s="27">
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
         <v>111</v>
       </c>
@@ -10296,63 +10373,66 @@
       <c r="I23" s="7" t="s">
         <v>391</v>
       </c>
-      <c r="J23" s="7" t="s">
+      <c r="J23" s="7">
+        <v>2</v>
+      </c>
+      <c r="K23" s="7" t="s">
         <v>307</v>
       </c>
-      <c r="K23" s="7" t="s">
+      <c r="L23" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="L23" s="7" t="s">
+      <c r="M23" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="M23" s="7" t="s">
+      <c r="N23" s="7" t="s">
         <v>87</v>
-      </c>
-      <c r="N23" s="7" t="s">
-        <v>3</v>
       </c>
       <c r="O23" s="7" t="s">
         <v>3</v>
       </c>
       <c r="P23" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q23" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="Q23" s="27" t="s">
+      <c r="R23" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="R23" s="27" t="s">
+      <c r="S23" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="S23" s="31">
+      <c r="T23" s="31">
         <v>0</v>
       </c>
-      <c r="T23" s="31">
+      <c r="U23" s="31">
         <v>-2</v>
       </c>
-      <c r="U23" s="35">
+      <c r="V23" s="35">
         <v>15650</v>
       </c>
-      <c r="V23" s="35">
+      <c r="W23" s="35">
         <v>25000</v>
       </c>
-      <c r="W23" s="36">
+      <c r="X23" s="36">
         <f t="shared" si="0"/>
         <v>9350</v>
       </c>
-      <c r="X23" s="27">
+      <c r="Y23" s="27">
         <v>150</v>
       </c>
-      <c r="Y23" s="7" t="s">
+      <c r="Z23" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="Z23" s="7">
+      <c r="AA23" s="7">
         <v>33</v>
       </c>
-      <c r="AA23" s="27">
+      <c r="AB23" s="27">
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
         <v>111</v>
       </c>
@@ -10380,130 +10460,133 @@
       <c r="I24" s="7" t="s">
         <v>392</v>
       </c>
-      <c r="J24" s="7" t="s">
+      <c r="J24" s="7">
+        <v>2</v>
+      </c>
+      <c r="K24" s="7" t="s">
         <v>308</v>
       </c>
-      <c r="K24" s="7" t="s">
+      <c r="L24" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="L24" s="7" t="s">
+      <c r="M24" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="M24" s="7" t="s">
+      <c r="N24" s="7" t="s">
         <v>87</v>
-      </c>
-      <c r="N24" s="7" t="s">
-        <v>3</v>
       </c>
       <c r="O24" s="7" t="s">
         <v>3</v>
       </c>
       <c r="P24" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q24" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="Q24" s="27" t="s">
+      <c r="R24" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="R24" s="27" t="s">
+      <c r="S24" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="S24" s="31">
+      <c r="T24" s="31">
         <v>0</v>
       </c>
-      <c r="T24" s="31">
+      <c r="U24" s="31">
         <v>-2</v>
       </c>
-      <c r="U24" s="35">
+      <c r="V24" s="35">
         <v>15650</v>
       </c>
-      <c r="V24" s="35">
+      <c r="W24" s="35">
         <v>26500</v>
       </c>
-      <c r="W24" s="36">
+      <c r="X24" s="36">
         <f t="shared" si="0"/>
         <v>10850</v>
       </c>
-      <c r="X24" s="27">
+      <c r="Y24" s="27">
         <v>150</v>
       </c>
-      <c r="Y24" s="7" t="s">
+      <c r="Z24" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="Z24" s="7">
+      <c r="AA24" s="7">
         <v>33</v>
       </c>
-      <c r="AA24" s="27">
+      <c r="AB24" s="27">
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="W31" s="36"/>
-    </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="W32" s="36"/>
-    </row>
-    <row r="33" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W33" s="36"/>
-    </row>
-    <row r="34" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W34" s="36"/>
-    </row>
-    <row r="35" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W35" s="36"/>
-    </row>
-    <row r="36" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W36" s="36"/>
-    </row>
-    <row r="37" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W37" s="36"/>
-    </row>
-    <row r="38" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W38" s="36"/>
-    </row>
-    <row r="39" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W39" s="36"/>
-    </row>
-    <row r="40" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W40" s="36"/>
-    </row>
-    <row r="41" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W41" s="36"/>
-    </row>
-    <row r="42" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W42" s="36"/>
-    </row>
-    <row r="43" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W43" s="36"/>
-    </row>
-    <row r="44" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W44" s="36"/>
-    </row>
-    <row r="45" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W45" s="36"/>
-    </row>
-    <row r="46" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W46" s="36"/>
-    </row>
-    <row r="47" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W47" s="36"/>
-    </row>
-    <row r="48" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W48" s="36"/>
-    </row>
-    <row r="49" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W49" s="36"/>
-    </row>
-    <row r="50" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W50" s="36"/>
-    </row>
-    <row r="51" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W51" s="36"/>
-    </row>
-    <row r="52" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W52" s="36"/>
-    </row>
-    <row r="53" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W53" s="36"/>
+    <row r="31" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="X31" s="36"/>
+    </row>
+    <row r="32" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="X32" s="36"/>
+    </row>
+    <row r="33" spans="24:24" x14ac:dyDescent="0.2">
+      <c r="X33" s="36"/>
+    </row>
+    <row r="34" spans="24:24" x14ac:dyDescent="0.2">
+      <c r="X34" s="36"/>
+    </row>
+    <row r="35" spans="24:24" x14ac:dyDescent="0.2">
+      <c r="X35" s="36"/>
+    </row>
+    <row r="36" spans="24:24" x14ac:dyDescent="0.2">
+      <c r="X36" s="36"/>
+    </row>
+    <row r="37" spans="24:24" x14ac:dyDescent="0.2">
+      <c r="X37" s="36"/>
+    </row>
+    <row r="38" spans="24:24" x14ac:dyDescent="0.2">
+      <c r="X38" s="36"/>
+    </row>
+    <row r="39" spans="24:24" x14ac:dyDescent="0.2">
+      <c r="X39" s="36"/>
+    </row>
+    <row r="40" spans="24:24" x14ac:dyDescent="0.2">
+      <c r="X40" s="36"/>
+    </row>
+    <row r="41" spans="24:24" x14ac:dyDescent="0.2">
+      <c r="X41" s="36"/>
+    </row>
+    <row r="42" spans="24:24" x14ac:dyDescent="0.2">
+      <c r="X42" s="36"/>
+    </row>
+    <row r="43" spans="24:24" x14ac:dyDescent="0.2">
+      <c r="X43" s="36"/>
+    </row>
+    <row r="44" spans="24:24" x14ac:dyDescent="0.2">
+      <c r="X44" s="36"/>
+    </row>
+    <row r="45" spans="24:24" x14ac:dyDescent="0.2">
+      <c r="X45" s="36"/>
+    </row>
+    <row r="46" spans="24:24" x14ac:dyDescent="0.2">
+      <c r="X46" s="36"/>
+    </row>
+    <row r="47" spans="24:24" x14ac:dyDescent="0.2">
+      <c r="X47" s="36"/>
+    </row>
+    <row r="48" spans="24:24" x14ac:dyDescent="0.2">
+      <c r="X48" s="36"/>
+    </row>
+    <row r="49" spans="24:24" x14ac:dyDescent="0.2">
+      <c r="X49" s="36"/>
+    </row>
+    <row r="50" spans="24:24" x14ac:dyDescent="0.2">
+      <c r="X50" s="36"/>
+    </row>
+    <row r="51" spans="24:24" x14ac:dyDescent="0.2">
+      <c r="X51" s="36"/>
+    </row>
+    <row r="52" spans="24:24" x14ac:dyDescent="0.2">
+      <c r="X52" s="36"/>
+    </row>
+    <row r="53" spans="24:24" x14ac:dyDescent="0.2">
+      <c r="X53" s="36"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10512,6 +10595,443 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AA5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G38" sqref="G38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="8" max="8" width="38.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q1" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="R1" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="S1" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="T1" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="U1" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="V1" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="W1" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="X1" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="Y1" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="Z1" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="AA1" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="C2" s="27">
+        <v>134</v>
+      </c>
+      <c r="D2" s="11">
+        <v>42564</v>
+      </c>
+      <c r="E2" s="27">
+        <v>28</v>
+      </c>
+      <c r="F2" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>375</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>292</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="O2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="P2" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q2" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="R2" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="S2" s="31">
+        <v>3</v>
+      </c>
+      <c r="T2" s="31">
+        <v>-2</v>
+      </c>
+      <c r="U2" s="35">
+        <v>17200</v>
+      </c>
+      <c r="V2" s="35">
+        <v>21000</v>
+      </c>
+      <c r="W2" s="36">
+        <f t="shared" ref="W2:W5" si="0">V2-U2</f>
+        <v>3800</v>
+      </c>
+      <c r="X2" s="27">
+        <v>150</v>
+      </c>
+      <c r="Y2" s="33" t="s">
+        <v>114</v>
+      </c>
+      <c r="Z2" s="7">
+        <v>1</v>
+      </c>
+      <c r="AA2" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="C3" s="27">
+        <v>135</v>
+      </c>
+      <c r="D3" s="11">
+        <v>42566</v>
+      </c>
+      <c r="E3" s="27">
+        <v>28</v>
+      </c>
+      <c r="F3" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>376</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="O3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="P3" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q3" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="R3" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="S3" s="31">
+        <v>3</v>
+      </c>
+      <c r="T3" s="31">
+        <v>-1</v>
+      </c>
+      <c r="U3" s="35">
+        <v>17200</v>
+      </c>
+      <c r="V3" s="35">
+        <v>21500</v>
+      </c>
+      <c r="W3" s="36">
+        <f t="shared" si="0"/>
+        <v>4300</v>
+      </c>
+      <c r="X3" s="27">
+        <v>150</v>
+      </c>
+      <c r="Y3" s="33" t="s">
+        <v>114</v>
+      </c>
+      <c r="Z3" s="7">
+        <v>1</v>
+      </c>
+      <c r="AA3" s="27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="C4" s="27">
+        <v>139</v>
+      </c>
+      <c r="D4" s="11">
+        <v>42601</v>
+      </c>
+      <c r="E4" s="27">
+        <v>28</v>
+      </c>
+      <c r="F4" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>383</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>299</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="N4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="O4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="P4" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q4" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="R4" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="S4" s="31">
+        <v>4</v>
+      </c>
+      <c r="T4" s="31">
+        <v>-1</v>
+      </c>
+      <c r="U4" s="35">
+        <v>18000</v>
+      </c>
+      <c r="V4" s="35">
+        <v>23800</v>
+      </c>
+      <c r="W4" s="36">
+        <f t="shared" si="0"/>
+        <v>5800</v>
+      </c>
+      <c r="X4" s="27">
+        <v>150</v>
+      </c>
+      <c r="Y4" s="33" t="s">
+        <v>114</v>
+      </c>
+      <c r="Z4" s="7">
+        <v>1</v>
+      </c>
+      <c r="AA4" s="27">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="C5" s="27">
+        <v>140</v>
+      </c>
+      <c r="D5" s="11">
+        <v>42625</v>
+      </c>
+      <c r="E5" s="27">
+        <v>28</v>
+      </c>
+      <c r="F5" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>303</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="L5" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="N5" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="O5" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="P5" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q5" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="R5" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="S5" s="31">
+        <v>2</v>
+      </c>
+      <c r="T5" s="31">
+        <v>2</v>
+      </c>
+      <c r="U5" s="35">
+        <v>18000</v>
+      </c>
+      <c r="V5" s="35">
+        <v>25500</v>
+      </c>
+      <c r="W5" s="36">
+        <f t="shared" si="0"/>
+        <v>7500</v>
+      </c>
+      <c r="X5" s="27">
+        <v>150</v>
+      </c>
+      <c r="Y5" s="33" t="s">
+        <v>114</v>
+      </c>
+      <c r="Z5" s="7">
+        <v>1</v>
+      </c>
+      <c r="AA5" s="27">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
@@ -11831,7 +12351,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>

</xml_diff>

<commit_message>
Updated plotting, saving to individual session files instead of one single file,
</commit_message>
<xml_diff>
--- a/config/SFN_NHP_Coordinates_All.xlsx
+++ b/config/SFN_NHP_Coordinates_All.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1400" yWindow="1260" windowWidth="50860" windowHeight="25500" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="5680" yWindow="560" windowWidth="47640" windowHeight="25440" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Br" sheetId="2" r:id="rId1"/>
@@ -1320,12 +1320,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1532,7 +1550,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1650,6 +1668,57 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -8411,8 +8480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="K34" sqref="K34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9215,89 +9284,89 @@
       </c>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="47" t="s">
         <v>111</v>
       </c>
-      <c r="B10" s="25" t="s">
+      <c r="B10" s="48" t="s">
         <v>112</v>
       </c>
-      <c r="C10" s="27">
+      <c r="C10" s="49">
         <v>139</v>
       </c>
-      <c r="D10" s="11">
+      <c r="D10" s="50">
         <v>42601</v>
       </c>
-      <c r="E10" s="27">
+      <c r="E10" s="49">
         <v>28</v>
       </c>
-      <c r="F10" s="27" t="s">
+      <c r="F10" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="27" t="s">
+      <c r="G10" s="49" t="s">
         <v>113</v>
       </c>
-      <c r="H10" s="7" t="s">
+      <c r="H10" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="I10" s="7" t="s">
+      <c r="I10" s="47" t="s">
         <v>383</v>
       </c>
-      <c r="J10" s="7">
+      <c r="J10" s="47">
         <v>1</v>
       </c>
-      <c r="K10" s="7" t="s">
+      <c r="K10" s="47" t="s">
         <v>299</v>
       </c>
-      <c r="L10" s="7" t="s">
+      <c r="L10" s="47" t="s">
         <v>121</v>
       </c>
-      <c r="M10" s="7" t="s">
+      <c r="M10" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="N10" s="7" t="s">
+      <c r="N10" s="47" t="s">
         <v>87</v>
       </c>
-      <c r="O10" s="7" t="s">
+      <c r="O10" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="P10" s="7" t="s">
+      <c r="P10" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="Q10" s="7" t="s">
+      <c r="Q10" s="47" t="s">
         <v>36</v>
       </c>
-      <c r="R10" s="27" t="s">
+      <c r="R10" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="S10" s="27" t="s">
+      <c r="S10" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="T10" s="31">
+      <c r="T10" s="51">
         <v>4</v>
       </c>
-      <c r="U10" s="31">
+      <c r="U10" s="51">
         <v>-1</v>
       </c>
-      <c r="V10" s="35">
+      <c r="V10" s="49">
         <v>18000</v>
       </c>
-      <c r="W10" s="35">
+      <c r="W10" s="49">
         <v>23800</v>
       </c>
-      <c r="X10" s="36">
+      <c r="X10" s="47">
         <f t="shared" si="0"/>
         <v>5800</v>
       </c>
-      <c r="Y10" s="27">
+      <c r="Y10" s="49">
         <v>150</v>
       </c>
-      <c r="Z10" s="33" t="s">
+      <c r="Z10" s="52" t="s">
         <v>114</v>
       </c>
-      <c r="AA10" s="7">
+      <c r="AA10" s="47">
         <v>1</v>
       </c>
-      <c r="AB10" s="27">
+      <c r="AB10" s="49">
         <v>12</v>
       </c>
     </row>
@@ -9650,350 +9719,350 @@
       </c>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="41" t="s">
         <v>111</v>
       </c>
-      <c r="B15" s="25" t="s">
+      <c r="B15" s="45" t="s">
         <v>112</v>
       </c>
-      <c r="C15" s="27">
+      <c r="C15" s="42">
         <v>140</v>
       </c>
-      <c r="D15" s="11">
+      <c r="D15" s="46">
         <v>42625</v>
       </c>
-      <c r="E15" s="27">
+      <c r="E15" s="42">
         <v>28</v>
       </c>
-      <c r="F15" s="27" t="s">
+      <c r="F15" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="G15" s="27" t="s">
+      <c r="G15" s="42" t="s">
         <v>113</v>
       </c>
-      <c r="H15" s="7" t="s">
+      <c r="H15" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="I15" s="7" t="s">
+      <c r="I15" s="41" t="s">
         <v>387</v>
       </c>
-      <c r="J15" s="7">
+      <c r="J15" s="41">
         <v>1</v>
       </c>
-      <c r="K15" s="7" t="s">
+      <c r="K15" s="41" t="s">
         <v>303</v>
       </c>
-      <c r="L15" s="7" t="s">
+      <c r="L15" s="41" t="s">
         <v>121</v>
       </c>
-      <c r="M15" s="7" t="s">
+      <c r="M15" s="41" t="s">
         <v>49</v>
       </c>
-      <c r="N15" s="7" t="s">
+      <c r="N15" s="41" t="s">
         <v>87</v>
       </c>
-      <c r="O15" s="7" t="s">
+      <c r="O15" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="P15" s="7" t="s">
+      <c r="P15" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="Q15" s="7" t="s">
+      <c r="Q15" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="R15" s="27" t="s">
+      <c r="R15" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="S15" s="27" t="s">
+      <c r="S15" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="T15" s="31">
+      <c r="T15" s="43">
         <v>2</v>
       </c>
-      <c r="U15" s="31">
+      <c r="U15" s="43">
         <v>2</v>
       </c>
-      <c r="V15" s="35">
+      <c r="V15" s="42">
         <v>18000</v>
       </c>
-      <c r="W15" s="35">
+      <c r="W15" s="42">
         <v>25500</v>
       </c>
-      <c r="X15" s="36">
+      <c r="X15" s="41">
         <f t="shared" si="0"/>
         <v>7500</v>
       </c>
-      <c r="Y15" s="27">
+      <c r="Y15" s="42">
         <v>150</v>
       </c>
-      <c r="Z15" s="33" t="s">
+      <c r="Z15" s="44" t="s">
         <v>114</v>
       </c>
-      <c r="AA15" s="7">
+      <c r="AA15" s="41">
         <v>1</v>
       </c>
-      <c r="AB15" s="27">
+      <c r="AB15" s="42">
         <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="41" t="s">
         <v>111</v>
       </c>
-      <c r="B16" s="25" t="s">
+      <c r="B16" s="45" t="s">
         <v>112</v>
       </c>
-      <c r="C16" s="27">
+      <c r="C16" s="42">
         <v>140</v>
       </c>
-      <c r="D16" s="11">
+      <c r="D16" s="46">
         <v>42625</v>
       </c>
-      <c r="E16" s="27">
+      <c r="E16" s="42">
         <v>28</v>
       </c>
-      <c r="F16" s="27" t="s">
+      <c r="F16" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="G16" s="27" t="s">
+      <c r="G16" s="42" t="s">
         <v>113</v>
       </c>
-      <c r="H16" s="7" t="s">
+      <c r="H16" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="I16" s="7" t="s">
+      <c r="I16" s="41" t="s">
         <v>387</v>
       </c>
-      <c r="J16" s="7">
+      <c r="J16" s="41">
         <v>2</v>
       </c>
-      <c r="K16" s="7" t="s">
+      <c r="K16" s="41" t="s">
         <v>303</v>
       </c>
-      <c r="L16" s="7" t="s">
+      <c r="L16" s="41" t="s">
         <v>121</v>
       </c>
-      <c r="M16" s="7" t="s">
+      <c r="M16" s="41" t="s">
         <v>49</v>
       </c>
-      <c r="N16" s="7" t="s">
+      <c r="N16" s="41" t="s">
         <v>87</v>
       </c>
-      <c r="O16" s="7" t="s">
+      <c r="O16" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="P16" s="7" t="s">
+      <c r="P16" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="Q16" s="7" t="s">
+      <c r="Q16" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="R16" s="27" t="s">
+      <c r="R16" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="S16" s="27" t="s">
+      <c r="S16" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="T16" s="31">
+      <c r="T16" s="43">
         <v>2</v>
       </c>
-      <c r="U16" s="31">
+      <c r="U16" s="43">
         <v>-1</v>
       </c>
-      <c r="V16" s="35">
+      <c r="V16" s="42">
         <v>15650</v>
       </c>
-      <c r="W16" s="35">
+      <c r="W16" s="42">
         <v>21500</v>
       </c>
-      <c r="X16" s="36">
+      <c r="X16" s="41">
         <f t="shared" si="0"/>
         <v>5850</v>
       </c>
-      <c r="Y16" s="27">
+      <c r="Y16" s="42">
         <v>150</v>
       </c>
-      <c r="Z16" s="7" t="s">
+      <c r="Z16" s="41" t="s">
         <v>115</v>
       </c>
-      <c r="AA16" s="7">
+      <c r="AA16" s="41">
         <v>33</v>
       </c>
-      <c r="AB16" s="27">
+      <c r="AB16" s="42">
         <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="47" t="s">
         <v>111</v>
       </c>
-      <c r="B17" s="25" t="s">
+      <c r="B17" s="48" t="s">
         <v>112</v>
       </c>
-      <c r="C17" s="27">
+      <c r="C17" s="49">
         <v>141</v>
       </c>
-      <c r="D17" s="11">
+      <c r="D17" s="50">
         <v>42634</v>
       </c>
-      <c r="E17" s="27">
+      <c r="E17" s="49">
         <v>28</v>
       </c>
-      <c r="F17" s="27" t="s">
+      <c r="F17" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="G17" s="27" t="s">
+      <c r="G17" s="49" t="s">
         <v>113</v>
       </c>
-      <c r="H17" s="7" t="s">
+      <c r="H17" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="I17" s="7" t="s">
+      <c r="I17" s="47" t="s">
         <v>388</v>
       </c>
-      <c r="J17" s="7">
+      <c r="J17" s="47">
         <v>1</v>
       </c>
-      <c r="K17" s="7" t="s">
+      <c r="K17" s="47" t="s">
         <v>304</v>
       </c>
-      <c r="L17" s="7" t="s">
+      <c r="L17" s="47" t="s">
         <v>121</v>
       </c>
-      <c r="M17" s="7" t="s">
+      <c r="M17" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="N17" s="7" t="s">
+      <c r="N17" s="47" t="s">
         <v>87</v>
       </c>
-      <c r="O17" s="7" t="s">
+      <c r="O17" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="P17" s="7" t="s">
+      <c r="P17" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="Q17" s="7" t="s">
+      <c r="Q17" s="47" t="s">
         <v>36</v>
       </c>
-      <c r="R17" s="27" t="s">
+      <c r="R17" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="S17" s="27" t="s">
+      <c r="S17" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="T17" s="31">
+      <c r="T17" s="51">
         <v>0</v>
       </c>
-      <c r="U17" s="31">
+      <c r="U17" s="51">
         <v>0</v>
       </c>
-      <c r="V17" s="35">
+      <c r="V17" s="49">
         <v>18000</v>
       </c>
-      <c r="W17" s="35">
+      <c r="W17" s="49">
         <v>19500</v>
       </c>
-      <c r="X17" s="36">
+      <c r="X17" s="47">
         <f t="shared" si="0"/>
         <v>1500</v>
       </c>
-      <c r="Y17" s="27">
+      <c r="Y17" s="49">
         <v>150</v>
       </c>
-      <c r="Z17" s="33" t="s">
+      <c r="Z17" s="52" t="s">
         <v>114</v>
       </c>
-      <c r="AA17" s="7">
+      <c r="AA17" s="47">
         <v>1</v>
       </c>
-      <c r="AB17" s="27">
+      <c r="AB17" s="49">
         <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="47" t="s">
         <v>111</v>
       </c>
-      <c r="B18" s="25" t="s">
+      <c r="B18" s="48" t="s">
         <v>112</v>
       </c>
-      <c r="C18" s="27">
+      <c r="C18" s="49">
         <v>141</v>
       </c>
-      <c r="D18" s="11">
+      <c r="D18" s="50">
         <v>42634</v>
       </c>
-      <c r="E18" s="27">
+      <c r="E18" s="49">
         <v>28</v>
       </c>
-      <c r="F18" s="27" t="s">
+      <c r="F18" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="G18" s="27" t="s">
+      <c r="G18" s="49" t="s">
         <v>113</v>
       </c>
-      <c r="H18" s="7" t="s">
+      <c r="H18" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="I18" s="7" t="s">
+      <c r="I18" s="47" t="s">
         <v>388</v>
       </c>
-      <c r="J18" s="7">
+      <c r="J18" s="47">
         <v>2</v>
       </c>
-      <c r="K18" s="7" t="s">
+      <c r="K18" s="47" t="s">
         <v>304</v>
       </c>
-      <c r="L18" s="7" t="s">
+      <c r="L18" s="47" t="s">
         <v>121</v>
       </c>
-      <c r="M18" s="7" t="s">
+      <c r="M18" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="N18" s="7" t="s">
+      <c r="N18" s="47" t="s">
         <v>87</v>
       </c>
-      <c r="O18" s="7" t="s">
+      <c r="O18" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="P18" s="7" t="s">
+      <c r="P18" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="Q18" s="7" t="s">
+      <c r="Q18" s="47" t="s">
         <v>36</v>
       </c>
-      <c r="R18" s="27" t="s">
+      <c r="R18" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="S18" s="27" t="s">
+      <c r="S18" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="T18" s="31">
+      <c r="T18" s="51">
         <v>2</v>
       </c>
-      <c r="U18" s="31">
+      <c r="U18" s="51">
         <v>-1</v>
       </c>
-      <c r="V18" s="35">
+      <c r="V18" s="49">
         <v>15650</v>
       </c>
-      <c r="W18" s="35">
+      <c r="W18" s="49">
         <v>24000</v>
       </c>
-      <c r="X18" s="36">
+      <c r="X18" s="47">
         <f t="shared" si="0"/>
         <v>8350</v>
       </c>
-      <c r="Y18" s="27">
+      <c r="Y18" s="49">
         <v>150</v>
       </c>
-      <c r="Z18" s="7" t="s">
+      <c r="Z18" s="47" t="s">
         <v>115</v>
       </c>
-      <c r="AA18" s="7">
+      <c r="AA18" s="47">
         <v>33</v>
       </c>
-      <c r="AB18" s="27">
+      <c r="AB18" s="49">
         <v>9</v>
       </c>
     </row>
@@ -10346,89 +10415,89 @@
       </c>
     </row>
     <row r="23" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="53" t="s">
         <v>111</v>
       </c>
-      <c r="B23" s="25" t="s">
+      <c r="B23" s="54" t="s">
         <v>112</v>
       </c>
-      <c r="C23" s="27">
+      <c r="C23" s="55">
         <v>142</v>
       </c>
-      <c r="D23" s="11">
+      <c r="D23" s="56">
         <v>42646</v>
       </c>
-      <c r="E23" s="27">
+      <c r="E23" s="55">
         <v>28</v>
       </c>
-      <c r="F23" s="27" t="s">
+      <c r="F23" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="G23" s="27" t="s">
+      <c r="G23" s="55" t="s">
         <v>113</v>
       </c>
-      <c r="H23" s="7" t="s">
+      <c r="H23" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="I23" s="7" t="s">
+      <c r="I23" s="53" t="s">
         <v>391</v>
       </c>
-      <c r="J23" s="7">
+      <c r="J23" s="53">
         <v>2</v>
       </c>
-      <c r="K23" s="7" t="s">
+      <c r="K23" s="53" t="s">
         <v>307</v>
       </c>
-      <c r="L23" s="7" t="s">
+      <c r="L23" s="53" t="s">
         <v>121</v>
       </c>
-      <c r="M23" s="7" t="s">
+      <c r="M23" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="N23" s="7" t="s">
+      <c r="N23" s="53" t="s">
         <v>87</v>
       </c>
-      <c r="O23" s="7" t="s">
+      <c r="O23" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="P23" s="7" t="s">
+      <c r="P23" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="Q23" s="7" t="s">
+      <c r="Q23" s="53" t="s">
         <v>36</v>
       </c>
-      <c r="R23" s="27" t="s">
+      <c r="R23" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="S23" s="27" t="s">
+      <c r="S23" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="T23" s="31">
+      <c r="T23" s="57">
         <v>0</v>
       </c>
-      <c r="U23" s="31">
+      <c r="U23" s="57">
         <v>-2</v>
       </c>
-      <c r="V23" s="35">
+      <c r="V23" s="55">
         <v>15650</v>
       </c>
-      <c r="W23" s="35">
+      <c r="W23" s="55">
         <v>25000</v>
       </c>
-      <c r="X23" s="36">
+      <c r="X23" s="53">
         <f t="shared" si="0"/>
         <v>9350</v>
       </c>
-      <c r="Y23" s="27">
+      <c r="Y23" s="55">
         <v>150</v>
       </c>
-      <c r="Z23" s="7" t="s">
+      <c r="Z23" s="53" t="s">
         <v>115</v>
       </c>
-      <c r="AA23" s="7">
+      <c r="AA23" s="53">
         <v>33</v>
       </c>
-      <c r="AB23" s="27">
+      <c r="AB23" s="55">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated spreadsheet for preferred direction, quality of session, notes exception: jo
</commit_message>
<xml_diff>
--- a/config/SFN_NHP_Coordinates_All.xlsx
+++ b/config/SFN_NHP_Coordinates_All.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/subravcr/Projects/lab-schall/schalllab-spatial/config/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elseyjg/temp/schalllab-spatial/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5680" yWindow="560" windowWidth="47640" windowHeight="25440" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Br" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1676" uniqueCount="394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1843" uniqueCount="424">
   <si>
     <t>a3</t>
   </si>
@@ -1215,6 +1215,96 @@
   </si>
   <si>
     <t>probeNo</t>
+  </si>
+  <si>
+    <t>preferredDirection</t>
+  </si>
+  <si>
+    <t>qualityOfSession</t>
+  </si>
+  <si>
+    <t>qualityOfSession_explained</t>
+  </si>
+  <si>
+    <t>good clustering, edge cutoff, missing channel</t>
+  </si>
+  <si>
+    <t>great clustering</t>
+  </si>
+  <si>
+    <t>excellent clustering and activity</t>
+  </si>
+  <si>
+    <t>good clustering</t>
+  </si>
+  <si>
+    <t>edge cutoff, missing channels</t>
+  </si>
+  <si>
+    <t>good clustering, edge cutoff</t>
+  </si>
+  <si>
+    <t>good clustering, edge cutoff, missing channels</t>
+  </si>
+  <si>
+    <t>some clustering, edge cutoff, missing channels</t>
+  </si>
+  <si>
+    <t>few channels, edge cutoff</t>
+  </si>
+  <si>
+    <t>one missing channel, edge cutoff</t>
+  </si>
+  <si>
+    <t>edge cutoff</t>
+  </si>
+  <si>
+    <t>edge cutoff, entire array clustered</t>
+  </si>
+  <si>
+    <t>edge cutoff, missing channel</t>
+  </si>
+  <si>
+    <t>low clustering</t>
+  </si>
+  <si>
+    <t>missing channel, good clustering</t>
+  </si>
+  <si>
+    <t>few clusters</t>
+  </si>
+  <si>
+    <t>missing channels, some clustering</t>
+  </si>
+  <si>
+    <t>some clustering</t>
+  </si>
+  <si>
+    <t>edge cutoff, some clustering</t>
+  </si>
+  <si>
+    <t>few channels, no clustering</t>
+  </si>
+  <si>
+    <t>few channels, low clustering</t>
+  </si>
+  <si>
+    <t>low clustering, few channels</t>
+  </si>
+  <si>
+    <t>high clustering, few channels</t>
+  </si>
+  <si>
+    <t>no clustering</t>
+  </si>
+  <si>
+    <t>low clustering, edge cutoff</t>
+  </si>
+  <si>
+    <t>high clustering, edge cutoff</t>
+  </si>
+  <si>
+    <t>no clustering, missing channels</t>
   </si>
 </sst>
 </file>
@@ -2193,10 +2283,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Z23"/>
+  <dimension ref="A1:AC23"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD12"/>
+    <sheetView topLeftCell="X1" workbookViewId="0">
+      <selection activeCell="AA1" sqref="AA1:AC1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2217,9 +2307,11 @@
     <col min="22" max="23" width="18.83203125" customWidth="1"/>
     <col min="24" max="24" width="89.33203125" customWidth="1"/>
     <col min="25" max="26" width="26" customWidth="1"/>
+    <col min="27" max="28" width="48" style="1" customWidth="1"/>
+    <col min="29" max="29" width="71" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:29" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>74</v>
       </c>
@@ -2298,8 +2390,17 @@
       <c r="Z1" s="6" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA1" s="6" t="s">
+        <v>394</v>
+      </c>
+      <c r="AB1" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="AC1" s="6" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>100</v>
       </c>
@@ -2381,8 +2482,17 @@
       <c r="Z2" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB2" s="1">
+        <v>3</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>100</v>
       </c>
@@ -2464,8 +2574,17 @@
       <c r="Z3" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA3" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB3" s="1">
+        <v>2</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>100</v>
       </c>
@@ -2547,8 +2666,17 @@
       <c r="Z4" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA4" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB4" s="1">
+        <v>3</v>
+      </c>
+      <c r="AC4" s="1" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>100</v>
       </c>
@@ -2630,8 +2758,17 @@
       <c r="Z5" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA5" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB5" s="1">
+        <v>4</v>
+      </c>
+      <c r="AC5" s="1" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>100</v>
       </c>
@@ -2713,8 +2850,17 @@
       <c r="Z6" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA6" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB6" s="1">
+        <v>4</v>
+      </c>
+      <c r="AC6" s="1" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>100</v>
       </c>
@@ -2796,8 +2942,17 @@
       <c r="Z7" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA7" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB7" s="1">
+        <v>4</v>
+      </c>
+      <c r="AC7" s="1" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>100</v>
       </c>
@@ -2879,8 +3034,17 @@
       <c r="Z8" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA8" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB8" s="1">
+        <v>3</v>
+      </c>
+      <c r="AC8" s="1" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>100</v>
       </c>
@@ -2962,8 +3126,17 @@
       <c r="Z9" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA9" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB9" s="1">
+        <v>2</v>
+      </c>
+      <c r="AC9" s="1" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>100</v>
       </c>
@@ -3045,8 +3218,17 @@
       <c r="Z10" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA10" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB10" s="1">
+        <v>4</v>
+      </c>
+      <c r="AC10" s="1" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>100</v>
       </c>
@@ -3128,8 +3310,17 @@
       <c r="Z11" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA11" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB11" s="1">
+        <v>2</v>
+      </c>
+      <c r="AC11" s="1" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>100</v>
       </c>
@@ -3211,8 +3402,17 @@
       <c r="Z12" s="1">
         <v>9</v>
       </c>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA12" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB12" s="1">
+        <v>3</v>
+      </c>
+      <c r="AC12" s="1" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>100</v>
       </c>
@@ -3294,8 +3494,17 @@
       <c r="Z13" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA13" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB13" s="1">
+        <v>2</v>
+      </c>
+      <c r="AC13" s="1" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>100</v>
       </c>
@@ -3377,8 +3586,17 @@
       <c r="Z14" s="1">
         <v>11</v>
       </c>
-    </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA14" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB14" s="1">
+        <v>3</v>
+      </c>
+      <c r="AC14" s="1" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>100</v>
       </c>
@@ -3460,8 +3678,17 @@
       <c r="Z15" s="1">
         <v>12</v>
       </c>
-    </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA15" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB15" s="1">
+        <v>3</v>
+      </c>
+      <c r="AC15" s="1" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>100</v>
       </c>
@@ -3543,8 +3770,17 @@
       <c r="Z16" s="1">
         <v>13</v>
       </c>
-    </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA16" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB16" s="1">
+        <v>4</v>
+      </c>
+      <c r="AC16" s="1" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="17" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>100</v>
       </c>
@@ -3626,8 +3862,17 @@
       <c r="Z17" s="1">
         <v>14</v>
       </c>
-    </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA17" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB17" s="1">
+        <v>4</v>
+      </c>
+      <c r="AC17" s="1" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="18" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>100</v>
       </c>
@@ -3709,8 +3954,17 @@
       <c r="Z18" s="1">
         <v>11</v>
       </c>
-    </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA18" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB18" s="1">
+        <v>3</v>
+      </c>
+      <c r="AC18" s="1" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="19" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>100</v>
       </c>
@@ -3792,8 +4046,17 @@
       <c r="Z19" s="1">
         <v>15</v>
       </c>
-    </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA19" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB19" s="1">
+        <v>4</v>
+      </c>
+      <c r="AC19" s="1" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="20" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>100</v>
       </c>
@@ -3875,8 +4138,17 @@
       <c r="Z20" s="1">
         <v>16</v>
       </c>
-    </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA20" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB20" s="1">
+        <v>4</v>
+      </c>
+      <c r="AC20" s="1" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="21" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>100</v>
       </c>
@@ -3958,8 +4230,17 @@
       <c r="Z21" s="1">
         <v>17</v>
       </c>
-    </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA21" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB21" s="1">
+        <v>4</v>
+      </c>
+      <c r="AC21" s="1" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="22" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>100</v>
       </c>
@@ -4041,8 +4322,17 @@
       <c r="Z22" s="1">
         <v>18</v>
       </c>
-    </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA22" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB22" s="1">
+        <v>4</v>
+      </c>
+      <c r="AC22" s="1" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="23" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>100</v>
       </c>
@@ -4145,7 +4435,7 @@
   </sheetPr>
   <dimension ref="A1:Z20"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
       <selection activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
@@ -5825,10 +6115,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AA88"/>
+  <dimension ref="A1:AC88"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AA10" sqref="AA10:AA13"/>
+    <sheetView topLeftCell="W1" workbookViewId="0">
+      <selection activeCell="AA1" sqref="AA1:AC1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5855,11 +6145,13 @@
     <col min="24" max="24" width="106.6640625" style="1" customWidth="1"/>
     <col min="25" max="25" width="29.5" style="10" customWidth="1"/>
     <col min="26" max="26" width="18.1640625" style="1" customWidth="1"/>
-    <col min="27" max="27" width="27.1640625" style="1" customWidth="1"/>
-    <col min="28" max="16384" width="10.83203125" style="1"/>
+    <col min="27" max="27" width="37.5" style="1" customWidth="1"/>
+    <col min="28" max="28" width="48" style="1" customWidth="1"/>
+    <col min="29" max="29" width="71" style="1" customWidth="1"/>
+    <col min="30" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:29" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>74</v>
       </c>
@@ -5938,8 +6230,17 @@
       <c r="Z1" s="6" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AA1" s="6" t="s">
+        <v>394</v>
+      </c>
+      <c r="AB1" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="AC1" s="6" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
         <v>111</v>
       </c>
@@ -6021,8 +6322,17 @@
       <c r="Z2" s="19">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AA2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB2" s="1">
+        <v>4</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A3" s="19" t="s">
         <v>111</v>
       </c>
@@ -6104,8 +6414,17 @@
       <c r="Z3" s="19">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AA3" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB3" s="1">
+        <v>4</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A4" s="19" t="s">
         <v>111</v>
       </c>
@@ -6187,8 +6506,17 @@
       <c r="Z4" s="19">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AA4" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB4" s="1">
+        <v>4</v>
+      </c>
+      <c r="AC4" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A5" s="19" t="s">
         <v>111</v>
       </c>
@@ -6270,8 +6598,17 @@
       <c r="Z5" s="19">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AA5" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB5" s="1">
+        <v>2</v>
+      </c>
+      <c r="AC5" s="1" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A6" s="19" t="s">
         <v>111</v>
       </c>
@@ -6353,8 +6690,17 @@
       <c r="Z6" s="19">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AA6" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB6" s="1">
+        <v>4</v>
+      </c>
+      <c r="AC6" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A7" s="19" t="s">
         <v>111</v>
       </c>
@@ -6436,8 +6782,17 @@
       <c r="Z7" s="19">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AA7" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB7" s="1">
+        <v>4</v>
+      </c>
+      <c r="AC7" s="1" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A8" s="19" t="s">
         <v>111</v>
       </c>
@@ -6519,8 +6874,17 @@
       <c r="Z8" s="19">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AA8" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB8" s="1">
+        <v>2</v>
+      </c>
+      <c r="AC8" s="1" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A9" s="19" t="s">
         <v>111</v>
       </c>
@@ -6602,8 +6966,17 @@
       <c r="Z9" s="19">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AA9" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB9" s="1">
+        <v>4</v>
+      </c>
+      <c r="AC9" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A10" s="19" t="s">
         <v>111</v>
       </c>
@@ -6685,9 +7058,17 @@
       <c r="Z10" s="19">
         <v>6</v>
       </c>
-      <c r="AA10" s="7"/>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AA10" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB10" s="1">
+        <v>4</v>
+      </c>
+      <c r="AC10" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A11" s="19" t="s">
         <v>111</v>
       </c>
@@ -6769,9 +7150,17 @@
       <c r="Z11" s="19">
         <v>7</v>
       </c>
-      <c r="AA11" s="7"/>
-    </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AA11" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB11" s="1">
+        <v>4</v>
+      </c>
+      <c r="AC11" s="7" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A12" s="19" t="s">
         <v>111</v>
       </c>
@@ -6853,9 +7242,17 @@
       <c r="Z12" s="19">
         <v>8</v>
       </c>
-      <c r="AA12" s="7"/>
-    </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AA12" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB12" s="7">
+        <v>4</v>
+      </c>
+      <c r="AC12" s="7" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A13" s="19" t="s">
         <v>111</v>
       </c>
@@ -6937,9 +7334,17 @@
       <c r="Z13" s="19">
         <v>9</v>
       </c>
-      <c r="AA13" s="7"/>
-    </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AA13" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB13" s="1">
+        <v>4</v>
+      </c>
+      <c r="AC13" s="7" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A14" s="19"/>
       <c r="B14" s="25"/>
       <c r="C14" s="27"/>
@@ -6967,7 +7372,7 @@
       <c r="Y14" s="32"/>
       <c r="Z14" s="27"/>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A15" s="19"/>
       <c r="B15" s="25"/>
       <c r="C15" s="27"/>
@@ -6995,7 +7400,7 @@
       <c r="Y15" s="32"/>
       <c r="Z15" s="27"/>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A16" s="19"/>
       <c r="B16" s="25"/>
       <c r="C16" s="27"/>
@@ -8478,10 +8883,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB53"/>
+  <dimension ref="A1:AE53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView topLeftCell="Z1" workbookViewId="0">
+      <selection activeCell="AC1" sqref="AC1:AE1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8499,9 +8904,12 @@
     <col min="25" max="25" width="16.1640625" customWidth="1"/>
     <col min="26" max="26" width="105.5" customWidth="1"/>
     <col min="27" max="28" width="30" customWidth="1"/>
+    <col min="29" max="29" width="37.5" style="1" customWidth="1"/>
+    <col min="30" max="30" width="48" style="1" customWidth="1"/>
+    <col min="31" max="31" width="71" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:31" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>74</v>
       </c>
@@ -8586,8 +8994,17 @@
       <c r="AB1" s="6" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC1" s="6" t="s">
+        <v>394</v>
+      </c>
+      <c r="AD1" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="AE1" s="6" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>111</v>
       </c>
@@ -8673,8 +9090,17 @@
       <c r="AB2" s="27">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AD2" s="1">
+        <v>4</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>111</v>
       </c>
@@ -8760,8 +9186,17 @@
       <c r="AB3" s="27">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC3" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AD3" s="1">
+        <v>4</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>111</v>
       </c>
@@ -8848,7 +9283,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>111</v>
       </c>
@@ -8934,8 +9369,17 @@
       <c r="AB5" s="27">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC5" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AD5" s="1">
+        <v>4</v>
+      </c>
+      <c r="AE5" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>111</v>
       </c>
@@ -9021,8 +9465,17 @@
       <c r="AB6" s="27">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC6" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AD6" s="1">
+        <v>4</v>
+      </c>
+      <c r="AE6" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>111</v>
       </c>
@@ -9108,8 +9561,17 @@
       <c r="AB7" s="27">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC7" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AD7" s="1">
+        <v>4</v>
+      </c>
+      <c r="AE7" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>111</v>
       </c>
@@ -9195,8 +9657,17 @@
       <c r="AB8" s="27">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC8" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AD8" s="1">
+        <v>4</v>
+      </c>
+      <c r="AE8" s="1" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>111</v>
       </c>
@@ -9282,8 +9753,17 @@
       <c r="AB9" s="27">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC9" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AD9" s="7">
+        <v>4</v>
+      </c>
+      <c r="AE9" s="1" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A10" s="47" t="s">
         <v>111</v>
       </c>
@@ -9370,7 +9850,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>111</v>
       </c>
@@ -9456,8 +9936,17 @@
       <c r="AB11" s="27">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC11" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AD11" s="7">
+        <v>4</v>
+      </c>
+      <c r="AE11" s="1" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>111</v>
       </c>
@@ -9543,8 +10032,17 @@
       <c r="AB12" s="27">
         <v>13</v>
       </c>
-    </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC12" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AD12" s="1">
+        <v>4</v>
+      </c>
+      <c r="AE12" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>111</v>
       </c>
@@ -9630,8 +10128,17 @@
       <c r="AB13" s="27">
         <v>14</v>
       </c>
-    </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC13" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AD13" s="1">
+        <v>4</v>
+      </c>
+      <c r="AE13" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="14" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>111</v>
       </c>
@@ -9718,7 +10225,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A15" s="41" t="s">
         <v>111</v>
       </c>
@@ -9805,7 +10312,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A16" s="41" t="s">
         <v>111</v>
       </c>
@@ -9892,7 +10399,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A17" s="47" t="s">
         <v>111</v>
       </c>
@@ -9978,8 +10485,17 @@
       <c r="AB17" s="49">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC17" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AD17" s="7">
+        <v>4</v>
+      </c>
+      <c r="AE17" s="1" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="18" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A18" s="47" t="s">
         <v>111</v>
       </c>
@@ -10065,8 +10581,17 @@
       <c r="AB18" s="49">
         <v>9</v>
       </c>
-    </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC18" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AD18" s="7">
+        <v>4</v>
+      </c>
+      <c r="AE18" s="1" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="19" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>111</v>
       </c>
@@ -10152,8 +10677,17 @@
       <c r="AB19" s="27">
         <v>16</v>
       </c>
-    </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC19" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AD19" s="7">
+        <v>4</v>
+      </c>
+      <c r="AE19" s="1" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="20" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
         <v>111</v>
       </c>
@@ -10239,8 +10773,17 @@
       <c r="AB20" s="27">
         <v>10</v>
       </c>
-    </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC20" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AD20" s="7">
+        <v>4</v>
+      </c>
+      <c r="AE20" s="1" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="21" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
         <v>111</v>
       </c>
@@ -10326,8 +10869,17 @@
       <c r="AB21" s="27">
         <v>16</v>
       </c>
-    </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC21" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD21" s="7">
+        <v>4</v>
+      </c>
+      <c r="AE21" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="22" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
         <v>111</v>
       </c>
@@ -10413,8 +10965,17 @@
       <c r="AB22" s="27">
         <v>10</v>
       </c>
-    </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC22" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AD22" s="7">
+        <v>4</v>
+      </c>
+      <c r="AE22" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="23" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A23" s="53" t="s">
         <v>111</v>
       </c>
@@ -10500,8 +11061,17 @@
       <c r="AB23" s="55">
         <v>16</v>
       </c>
-    </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC23" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AD23" s="7">
+        <v>4</v>
+      </c>
+      <c r="AE23" s="7" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="24" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
         <v>111</v>
       </c>
@@ -10587,11 +11157,20 @@
       <c r="AB24" s="27">
         <v>16</v>
       </c>
-    </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC24" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AD24" s="7">
+        <v>4</v>
+      </c>
+      <c r="AE24" s="7" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="31" spans="1:31" x14ac:dyDescent="0.2">
       <c r="X31" s="36"/>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:31" x14ac:dyDescent="0.2">
       <c r="X32" s="36"/>
     </row>
     <row r="33" spans="24:24" x14ac:dyDescent="0.2">
@@ -11105,10 +11684,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AB37"/>
+  <dimension ref="A1:AC37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView topLeftCell="W1" workbookViewId="0">
+      <selection activeCell="AA1" sqref="AA1:AC1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11134,10 +11713,13 @@
     <col min="24" max="24" width="24.1640625" style="19" customWidth="1"/>
     <col min="25" max="25" width="71.5" style="19" customWidth="1"/>
     <col min="26" max="26" width="24.33203125" style="19" customWidth="1"/>
-    <col min="27" max="16384" width="10.83203125" style="19"/>
+    <col min="27" max="27" width="37.5" style="1" customWidth="1"/>
+    <col min="28" max="28" width="48" style="1" customWidth="1"/>
+    <col min="29" max="29" width="71" style="1" customWidth="1"/>
+    <col min="30" max="16384" width="10.83203125" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:29" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>74</v>
       </c>
@@ -11216,9 +11798,17 @@
       <c r="Z1" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="AA1" s="6"/>
-    </row>
-    <row r="2" spans="1:28" ht="17" x14ac:dyDescent="0.2">
+      <c r="AA1" s="6" t="s">
+        <v>394</v>
+      </c>
+      <c r="AB1" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="AC1" s="6" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
         <v>109</v>
       </c>
@@ -11300,10 +11890,17 @@
       <c r="Z2" s="15">
         <v>1</v>
       </c>
-      <c r="AA2" s="15"/>
-      <c r="AB2" s="15"/>
-    </row>
-    <row r="3" spans="1:28" ht="17" x14ac:dyDescent="0.2">
+      <c r="AA2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB2" s="1">
+        <v>3</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="19" t="s">
         <v>109</v>
       </c>
@@ -11385,10 +11982,17 @@
       <c r="Z3" s="15">
         <v>1</v>
       </c>
-      <c r="AA3" s="15"/>
-      <c r="AB3" s="15"/>
-    </row>
-    <row r="4" spans="1:28" ht="17" x14ac:dyDescent="0.2">
+      <c r="AA3" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB3" s="1">
+        <v>2</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="19" t="s">
         <v>109</v>
       </c>
@@ -11470,10 +12074,17 @@
       <c r="Z4" s="15">
         <v>1</v>
       </c>
-      <c r="AA4" s="15"/>
-      <c r="AB4" s="15"/>
-    </row>
-    <row r="5" spans="1:28" ht="17" x14ac:dyDescent="0.2">
+      <c r="AA4" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB4" s="1">
+        <v>2</v>
+      </c>
+      <c r="AC4" s="1" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="19" t="s">
         <v>109</v>
       </c>
@@ -11555,10 +12166,17 @@
       <c r="Z5" s="15">
         <v>1</v>
       </c>
-      <c r="AA5" s="15"/>
-      <c r="AB5" s="15"/>
-    </row>
-    <row r="6" spans="1:28" ht="17" x14ac:dyDescent="0.2">
+      <c r="AA5" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB5" s="1">
+        <v>2</v>
+      </c>
+      <c r="AC5" s="1" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="19" t="s">
         <v>109</v>
       </c>
@@ -11640,10 +12258,17 @@
       <c r="Z6" s="15">
         <v>1</v>
       </c>
-      <c r="AA6" s="15"/>
-      <c r="AB6" s="15"/>
-    </row>
-    <row r="7" spans="1:28" ht="17" x14ac:dyDescent="0.2">
+      <c r="AA6" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB6" s="1">
+        <v>3</v>
+      </c>
+      <c r="AC6" s="1" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="19" t="s">
         <v>109</v>
       </c>
@@ -11725,10 +12350,17 @@
       <c r="Z7" s="15">
         <v>1</v>
       </c>
-      <c r="AA7" s="15"/>
-      <c r="AB7" s="15"/>
-    </row>
-    <row r="8" spans="1:28" ht="17" x14ac:dyDescent="0.2">
+      <c r="AA7" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB7" s="1">
+        <v>4</v>
+      </c>
+      <c r="AC7" s="1" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="19" t="s">
         <v>109</v>
       </c>
@@ -11810,10 +12442,17 @@
       <c r="Z8" s="15">
         <v>1</v>
       </c>
-      <c r="AA8" s="15"/>
-      <c r="AB8" s="15"/>
-    </row>
-    <row r="9" spans="1:28" ht="17" x14ac:dyDescent="0.2">
+      <c r="AA8" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB8" s="1">
+        <v>2</v>
+      </c>
+      <c r="AC8" s="1" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="19" t="s">
         <v>109</v>
       </c>
@@ -11895,10 +12534,17 @@
       <c r="Z9" s="15">
         <v>1</v>
       </c>
-      <c r="AA9" s="15"/>
-      <c r="AB9" s="15"/>
-    </row>
-    <row r="10" spans="1:28" ht="17" x14ac:dyDescent="0.2">
+      <c r="AA9" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB9" s="7">
+        <v>3</v>
+      </c>
+      <c r="AC9" s="1" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="19" t="s">
         <v>109</v>
       </c>
@@ -11980,10 +12626,17 @@
       <c r="Z10" s="15">
         <v>1</v>
       </c>
-      <c r="AA10" s="15"/>
-      <c r="AB10" s="15"/>
-    </row>
-    <row r="11" spans="1:28" ht="17" x14ac:dyDescent="0.2">
+      <c r="AA10" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB10" s="1">
+        <v>4</v>
+      </c>
+      <c r="AC10" s="1" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="19" t="s">
         <v>109</v>
       </c>
@@ -12065,10 +12718,17 @@
       <c r="Z11" s="15">
         <v>1</v>
       </c>
-      <c r="AA11" s="15"/>
-      <c r="AB11" s="15"/>
-    </row>
-    <row r="12" spans="1:28" ht="17" x14ac:dyDescent="0.2">
+      <c r="AA11" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB11" s="7">
+        <v>3</v>
+      </c>
+      <c r="AC11" s="1" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="19" t="s">
         <v>109</v>
       </c>
@@ -12150,10 +12810,17 @@
       <c r="Z12" s="15">
         <v>1</v>
       </c>
-      <c r="AA12" s="15"/>
-      <c r="AB12" s="15"/>
-    </row>
-    <row r="13" spans="1:28" ht="17" x14ac:dyDescent="0.2">
+      <c r="AA12" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB12" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC12" s="1" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="19" t="s">
         <v>109</v>
       </c>
@@ -12235,10 +12902,17 @@
       <c r="Z13" s="15">
         <v>1</v>
       </c>
-      <c r="AA13" s="15"/>
-      <c r="AB13" s="15"/>
-    </row>
-    <row r="14" spans="1:28" ht="17" x14ac:dyDescent="0.2">
+      <c r="AA13" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB13" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC13" s="1" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="19" t="s">
         <v>109</v>
       </c>
@@ -12320,82 +12994,101 @@
       <c r="Z14" s="15">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AA14" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB14" s="1">
+        <v>3</v>
+      </c>
+      <c r="AC14" s="1" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.2">
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
       <c r="W15" s="1"/>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.2">
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
       <c r="W16" s="1"/>
     </row>
-    <row r="17" spans="15:21" x14ac:dyDescent="0.2">
+    <row r="17" spans="15:29" x14ac:dyDescent="0.2">
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
-    </row>
-    <row r="18" spans="15:21" x14ac:dyDescent="0.2">
+      <c r="AB17" s="7"/>
+    </row>
+    <row r="18" spans="15:29" x14ac:dyDescent="0.2">
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
-    </row>
-    <row r="19" spans="15:21" ht="17" x14ac:dyDescent="0.2">
+      <c r="AB18" s="7"/>
+    </row>
+    <row r="19" spans="15:29" ht="17" x14ac:dyDescent="0.2">
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
       <c r="U19" s="15"/>
-    </row>
-    <row r="20" spans="15:21" ht="17" x14ac:dyDescent="0.2">
+      <c r="AB19" s="7"/>
+    </row>
+    <row r="20" spans="15:29" ht="17" x14ac:dyDescent="0.2">
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
       <c r="U20" s="15"/>
-    </row>
-    <row r="21" spans="15:21" ht="17" x14ac:dyDescent="0.2">
+      <c r="AB20" s="7"/>
+    </row>
+    <row r="21" spans="15:29" ht="17" x14ac:dyDescent="0.2">
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
       <c r="U21" s="15"/>
-    </row>
-    <row r="22" spans="15:21" ht="17" x14ac:dyDescent="0.2">
+      <c r="AB21" s="7"/>
+    </row>
+    <row r="22" spans="15:29" ht="17" x14ac:dyDescent="0.2">
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
       <c r="U22" s="15"/>
-    </row>
-    <row r="23" spans="15:21" ht="17" x14ac:dyDescent="0.2">
+      <c r="AB22" s="7"/>
+    </row>
+    <row r="23" spans="15:29" ht="17" x14ac:dyDescent="0.2">
       <c r="P23" s="17"/>
       <c r="U23" s="15"/>
-    </row>
-    <row r="24" spans="15:21" ht="17" x14ac:dyDescent="0.2">
+      <c r="AB23" s="7"/>
+      <c r="AC23" s="7"/>
+    </row>
+    <row r="24" spans="15:29" ht="17" x14ac:dyDescent="0.2">
       <c r="P24" s="17"/>
       <c r="U24" s="15"/>
-    </row>
-    <row r="25" spans="15:21" ht="17" x14ac:dyDescent="0.2">
+      <c r="AB24" s="7"/>
+      <c r="AC24" s="7"/>
+    </row>
+    <row r="25" spans="15:29" ht="17" x14ac:dyDescent="0.2">
       <c r="P25" s="17"/>
       <c r="U25" s="15"/>
     </row>
-    <row r="26" spans="15:21" ht="17" x14ac:dyDescent="0.2">
+    <row r="26" spans="15:29" ht="17" x14ac:dyDescent="0.2">
       <c r="P26" s="17"/>
       <c r="U26" s="15"/>
     </row>
-    <row r="27" spans="15:21" ht="17" x14ac:dyDescent="0.2">
+    <row r="27" spans="15:29" ht="17" x14ac:dyDescent="0.2">
       <c r="P27" s="17"/>
       <c r="U27" s="15"/>
     </row>
-    <row r="28" spans="15:21" ht="17" x14ac:dyDescent="0.2">
+    <row r="28" spans="15:29" ht="17" x14ac:dyDescent="0.2">
       <c r="P28" s="17"/>
       <c r="U28" s="17"/>
     </row>
-    <row r="29" spans="15:21" ht="17" x14ac:dyDescent="0.2">
+    <row r="29" spans="15:29" ht="17" x14ac:dyDescent="0.2">
       <c r="P29" s="17"/>
       <c r="U29" s="17"/>
     </row>
-    <row r="30" spans="15:21" ht="17" x14ac:dyDescent="0.2">
+    <row r="30" spans="15:29" ht="17" x14ac:dyDescent="0.2">
       <c r="P30" s="17"/>
       <c r="U30" s="17"/>
     </row>
-    <row r="31" spans="15:21" ht="17" x14ac:dyDescent="0.2">
+    <row r="31" spans="15:29" ht="17" x14ac:dyDescent="0.2">
       <c r="P31" s="17"/>
       <c r="U31" s="17"/>
     </row>
-    <row r="32" spans="15:21" ht="17" x14ac:dyDescent="0.2">
+    <row r="32" spans="15:29" ht="17" x14ac:dyDescent="0.2">
       <c r="P32" s="17"/>
     </row>
     <row r="33" spans="16:16" ht="17" x14ac:dyDescent="0.2">
@@ -12425,10 +13118,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AA1048576"/>
+  <dimension ref="A1:AC1048576"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="Z4" sqref="Z4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12445,11 +13138,13 @@
     <col min="22" max="24" width="16.33203125" style="19" customWidth="1"/>
     <col min="25" max="25" width="70.1640625" style="19" customWidth="1"/>
     <col min="26" max="26" width="31.6640625" style="19" customWidth="1"/>
-    <col min="27" max="27" width="16.33203125" style="19" customWidth="1"/>
-    <col min="28" max="16384" width="10.83203125" style="19"/>
+    <col min="27" max="27" width="37.5" style="1" customWidth="1"/>
+    <col min="28" max="28" width="48" style="1" customWidth="1"/>
+    <col min="29" max="29" width="71" style="1" customWidth="1"/>
+    <col min="30" max="16384" width="10.83203125" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:29" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>74</v>
       </c>
@@ -12528,9 +13223,17 @@
       <c r="Z1" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="AA1" s="6"/>
-    </row>
-    <row r="2" spans="1:27" ht="17" x14ac:dyDescent="0.2">
+      <c r="AA1" s="6" t="s">
+        <v>394</v>
+      </c>
+      <c r="AB1" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="AC1" s="6" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
         <v>106</v>
       </c>
@@ -12612,9 +13315,17 @@
       <c r="Z2" s="18">
         <v>1</v>
       </c>
-      <c r="AA2" s="18"/>
-    </row>
-    <row r="3" spans="1:27" ht="17" x14ac:dyDescent="0.2">
+      <c r="AA2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB2" s="1">
+        <v>2</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
         <v>106</v>
       </c>
@@ -12696,9 +13407,17 @@
       <c r="Z3" s="18">
         <v>1</v>
       </c>
-      <c r="AA3" s="18"/>
-    </row>
-    <row r="4" spans="1:27" ht="17" x14ac:dyDescent="0.2">
+      <c r="AA3" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB3" s="1">
+        <v>2</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
         <v>106</v>
       </c>
@@ -12780,9 +13499,17 @@
       <c r="Z4" s="18">
         <v>1</v>
       </c>
-      <c r="AA4" s="18"/>
-    </row>
-    <row r="5" spans="1:27" ht="17" x14ac:dyDescent="0.2">
+      <c r="AA4" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC4" s="1" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
         <v>106</v>
       </c>
@@ -12864,9 +13591,17 @@
       <c r="Z5" s="18">
         <v>1</v>
       </c>
-      <c r="AA5" s="18"/>
-    </row>
-    <row r="6" spans="1:27" ht="17" x14ac:dyDescent="0.2">
+      <c r="AA5" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB5" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC5" s="1" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
         <v>106</v>
       </c>
@@ -12948,9 +13683,17 @@
       <c r="Z6" s="18">
         <v>1</v>
       </c>
-      <c r="AA6" s="18"/>
-    </row>
-    <row r="7" spans="1:27" ht="17" x14ac:dyDescent="0.2">
+      <c r="AA6" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB6" s="1">
+        <v>3</v>
+      </c>
+      <c r="AC6" s="1" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
         <v>106</v>
       </c>
@@ -13032,9 +13775,17 @@
       <c r="Z7" s="18">
         <v>1</v>
       </c>
-      <c r="AA7" s="18"/>
-    </row>
-    <row r="8" spans="1:27" ht="17" x14ac:dyDescent="0.2">
+      <c r="AA7" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB7" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC7" s="1" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="15" t="s">
         <v>106</v>
       </c>
@@ -13116,9 +13867,17 @@
       <c r="Z8" s="18">
         <v>1</v>
       </c>
-      <c r="AA8" s="18"/>
-    </row>
-    <row r="9" spans="1:27" ht="17" x14ac:dyDescent="0.2">
+      <c r="AA8" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB8" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC8" s="1" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
         <v>106</v>
       </c>
@@ -13200,9 +13959,17 @@
       <c r="Z9" s="18">
         <v>1</v>
       </c>
-      <c r="AA9" s="18"/>
-    </row>
-    <row r="10" spans="1:27" ht="17" x14ac:dyDescent="0.2">
+      <c r="AA9" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB9" s="7">
+        <v>3</v>
+      </c>
+      <c r="AC9" s="1" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="15" t="s">
         <v>106</v>
       </c>
@@ -13284,9 +14051,17 @@
       <c r="Z10" s="18">
         <v>1</v>
       </c>
-      <c r="AA10" s="18"/>
-    </row>
-    <row r="11" spans="1:27" ht="17" x14ac:dyDescent="0.2">
+      <c r="AA10" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB10" s="1">
+        <v>2</v>
+      </c>
+      <c r="AC10" s="1" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="15" t="s">
         <v>106</v>
       </c>
@@ -13368,9 +14143,17 @@
       <c r="Z11" s="18">
         <v>1</v>
       </c>
-      <c r="AA11" s="18"/>
-    </row>
-    <row r="12" spans="1:27" ht="17" x14ac:dyDescent="0.2">
+      <c r="AA11" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB11" s="7">
+        <v>3</v>
+      </c>
+      <c r="AC11" s="1" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="15" t="s">
         <v>106</v>
       </c>
@@ -13452,9 +14235,17 @@
       <c r="Z12" s="18">
         <v>1</v>
       </c>
-      <c r="AA12" s="18"/>
-    </row>
-    <row r="13" spans="1:27" ht="17" x14ac:dyDescent="0.2">
+      <c r="AA12" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB12" s="7">
+        <v>3</v>
+      </c>
+      <c r="AC12" s="1" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="s">
         <v>106</v>
       </c>
@@ -13536,108 +14327,126 @@
       <c r="Z13" s="18">
         <v>1</v>
       </c>
-      <c r="AA13" s="18"/>
-    </row>
-    <row r="14" spans="1:27" ht="17" x14ac:dyDescent="0.2">
+      <c r="AA13" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB13" s="7">
+        <v>3</v>
+      </c>
+      <c r="AC13" s="1" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" ht="17" x14ac:dyDescent="0.2">
       <c r="J14" s="18"/>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
       <c r="R14" s="18"/>
       <c r="W14" s="1"/>
     </row>
-    <row r="15" spans="1:27" ht="17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:29" ht="17" x14ac:dyDescent="0.2">
       <c r="J15" s="18"/>
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
       <c r="R15" s="18"/>
       <c r="W15" s="1"/>
     </row>
-    <row r="16" spans="1:27" ht="17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:29" ht="17" x14ac:dyDescent="0.2">
       <c r="J16" s="18"/>
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
       <c r="R16" s="17"/>
       <c r="W16" s="1"/>
     </row>
-    <row r="17" spans="15:23" ht="17" x14ac:dyDescent="0.2">
+    <row r="17" spans="15:29" ht="17" x14ac:dyDescent="0.2">
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
       <c r="R17" s="17"/>
       <c r="W17" s="1"/>
-    </row>
-    <row r="18" spans="15:23" ht="17" x14ac:dyDescent="0.2">
+      <c r="AB17" s="7"/>
+    </row>
+    <row r="18" spans="15:29" ht="17" x14ac:dyDescent="0.2">
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
       <c r="R18" s="17"/>
       <c r="U18" s="15"/>
       <c r="W18" s="1"/>
-    </row>
-    <row r="19" spans="15:23" ht="17" x14ac:dyDescent="0.2">
+      <c r="AB18" s="7"/>
+    </row>
+    <row r="19" spans="15:29" ht="17" x14ac:dyDescent="0.2">
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
       <c r="R19" s="17"/>
       <c r="U19" s="15"/>
       <c r="W19" s="1"/>
-    </row>
-    <row r="20" spans="15:23" ht="17" x14ac:dyDescent="0.2">
+      <c r="AB19" s="7"/>
+    </row>
+    <row r="20" spans="15:29" ht="17" x14ac:dyDescent="0.2">
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
       <c r="R20" s="17"/>
       <c r="U20" s="15"/>
       <c r="W20" s="1"/>
-    </row>
-    <row r="21" spans="15:23" ht="17" x14ac:dyDescent="0.2">
+      <c r="AB20" s="7"/>
+    </row>
+    <row r="21" spans="15:29" ht="17" x14ac:dyDescent="0.2">
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
       <c r="R21" s="17"/>
       <c r="U21" s="15"/>
       <c r="W21" s="1"/>
-    </row>
-    <row r="22" spans="15:23" ht="17" x14ac:dyDescent="0.2">
+      <c r="AB21" s="7"/>
+    </row>
+    <row r="22" spans="15:29" ht="17" x14ac:dyDescent="0.2">
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
       <c r="R22" s="17"/>
       <c r="U22" s="15"/>
       <c r="W22" s="1"/>
-    </row>
-    <row r="23" spans="15:23" ht="17" x14ac:dyDescent="0.2">
+      <c r="AB22" s="7"/>
+    </row>
+    <row r="23" spans="15:29" ht="17" x14ac:dyDescent="0.2">
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
       <c r="R23" s="17"/>
       <c r="U23" s="15"/>
       <c r="W23" s="1"/>
-    </row>
-    <row r="24" spans="15:23" ht="17" x14ac:dyDescent="0.2">
+      <c r="AB23" s="7"/>
+      <c r="AC23" s="7"/>
+    </row>
+    <row r="24" spans="15:29" ht="17" x14ac:dyDescent="0.2">
       <c r="R24" s="17"/>
       <c r="U24" s="15"/>
-    </row>
-    <row r="25" spans="15:23" ht="17" x14ac:dyDescent="0.2">
+      <c r="AB24" s="7"/>
+      <c r="AC24" s="7"/>
+    </row>
+    <row r="25" spans="15:29" ht="17" x14ac:dyDescent="0.2">
       <c r="R25" s="17"/>
       <c r="U25" s="15"/>
     </row>
-    <row r="26" spans="15:23" ht="17" x14ac:dyDescent="0.2">
+    <row r="26" spans="15:29" ht="17" x14ac:dyDescent="0.2">
       <c r="R26" s="17"/>
       <c r="U26" s="15"/>
     </row>
-    <row r="27" spans="15:23" ht="17" x14ac:dyDescent="0.2">
+    <row r="27" spans="15:29" ht="17" x14ac:dyDescent="0.2">
       <c r="R27" s="17"/>
       <c r="U27" s="15"/>
     </row>
-    <row r="28" spans="15:23" ht="17" x14ac:dyDescent="0.2">
+    <row r="28" spans="15:29" ht="17" x14ac:dyDescent="0.2">
       <c r="R28" s="17"/>
       <c r="U28" s="17"/>
     </row>
-    <row r="29" spans="15:23" ht="17" x14ac:dyDescent="0.2">
+    <row r="29" spans="15:29" ht="17" x14ac:dyDescent="0.2">
       <c r="R29" s="17"/>
       <c r="U29" s="17"/>
     </row>
-    <row r="30" spans="15:23" ht="17" x14ac:dyDescent="0.2">
+    <row r="30" spans="15:29" ht="17" x14ac:dyDescent="0.2">
       <c r="R30" s="17"/>
     </row>
-    <row r="31" spans="15:23" ht="17" x14ac:dyDescent="0.2">
+    <row r="31" spans="15:29" ht="17" x14ac:dyDescent="0.2">
       <c r="R31" s="17"/>
     </row>
-    <row r="32" spans="15:23" ht="17" x14ac:dyDescent="0.2">
+    <row r="32" spans="15:29" ht="17" x14ac:dyDescent="0.2">
       <c r="R32" s="17"/>
     </row>
     <row r="33" spans="18:18" ht="17" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
added jo session quality ratings
</commit_message>
<xml_diff>
--- a/config/SFN_NHP_Coordinates_All.xlsx
+++ b/config/SFN_NHP_Coordinates_All.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5220" yWindow="460" windowWidth="30860" windowHeight="19440" tabRatio="500"/>
+    <workbookView xWindow="5220" yWindow="460" windowWidth="30860" windowHeight="19440" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Br" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1843" uniqueCount="424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1904" uniqueCount="432">
   <si>
     <t>a3</t>
   </si>
@@ -1305,6 +1305,30 @@
   </si>
   <si>
     <t>no clustering, missing channels</t>
+  </si>
+  <si>
+    <t>great clustering, edge cutoff</t>
+  </si>
+  <si>
+    <t>few clusters, edge cutoff</t>
+  </si>
+  <si>
+    <t>few clusters, missing channels</t>
+  </si>
+  <si>
+    <t>good clustering, sparcely connected clusters</t>
+  </si>
+  <si>
+    <t>no clusters</t>
+  </si>
+  <si>
+    <t>one cluster with edge cutoff</t>
+  </si>
+  <si>
+    <t>one small cluster</t>
+  </si>
+  <si>
+    <t>few clusters, sparcely connected</t>
   </si>
 </sst>
 </file>
@@ -1445,8 +1469,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="193">
+  <cellStyleXfs count="195">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1812,7 +1838,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="193">
+  <cellStyles count="195">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1909,6 +1935,7 @@
     <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2005,6 +2032,7 @@
     <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2285,8 +2313,8 @@
   </sheetPr>
   <dimension ref="A1:AC23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
+    <sheetView topLeftCell="X1" workbookViewId="0">
+      <selection activeCell="AB9" sqref="AB9:AC9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4433,10 +4461,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Z20"/>
+  <dimension ref="A1:AD24"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="J36" sqref="J36"/>
+    <sheetView tabSelected="1" topLeftCell="Z1" workbookViewId="0">
+      <selection activeCell="AC21" sqref="AC21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4462,10 +4490,14 @@
     <col min="24" max="24" width="87.1640625" style="1" customWidth="1"/>
     <col min="25" max="25" width="31.83203125" style="1" customWidth="1"/>
     <col min="26" max="26" width="16.83203125" style="1" customWidth="1"/>
-    <col min="27" max="16384" width="10.83203125" style="1"/>
+    <col min="27" max="27" width="14" style="1" customWidth="1"/>
+    <col min="28" max="28" width="54.33203125" style="1" customWidth="1"/>
+    <col min="29" max="29" width="36.1640625" style="1" customWidth="1"/>
+    <col min="30" max="30" width="54.33203125" style="1" customWidth="1"/>
+    <col min="31" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:30" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>74</v>
       </c>
@@ -4544,8 +4576,20 @@
       <c r="Z1" s="6" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA1" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="AB1" s="6" t="s">
+        <v>394</v>
+      </c>
+      <c r="AC1" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="AD1" s="6" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>73</v>
       </c>
@@ -4626,8 +4670,20 @@
       <c r="Z2" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA2" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AC2" s="7">
+        <v>2</v>
+      </c>
+      <c r="AD2" s="7" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>73</v>
       </c>
@@ -4708,8 +4764,20 @@
       <c r="Z3" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA3" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AC3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD3" s="1" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>73</v>
       </c>
@@ -4790,8 +4858,20 @@
       <c r="Z4" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA4" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="AB4" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AC4" s="1">
+        <v>2</v>
+      </c>
+      <c r="AD4" s="1" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>73</v>
       </c>
@@ -4872,8 +4952,20 @@
       <c r="Z5" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA5" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="AB5" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AC5" s="1">
+        <v>4</v>
+      </c>
+      <c r="AD5" s="1" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>73</v>
       </c>
@@ -4954,8 +5046,20 @@
       <c r="Z6" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA6" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="AB6" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AC6" s="1">
+        <v>3</v>
+      </c>
+      <c r="AD6" s="1" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>73</v>
       </c>
@@ -5036,8 +5140,20 @@
       <c r="Z7" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA7" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="AB7" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AC7" s="1">
+        <v>2</v>
+      </c>
+      <c r="AD7" s="1" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>73</v>
       </c>
@@ -5118,8 +5234,20 @@
       <c r="Z8" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA8" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="AB8" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AC8" s="1">
+        <v>4</v>
+      </c>
+      <c r="AD8" s="1" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>73</v>
       </c>
@@ -5200,8 +5328,20 @@
       <c r="Z9" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA9" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="AB9" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AC9" s="7">
+        <v>2</v>
+      </c>
+      <c r="AD9" s="1" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>73</v>
       </c>
@@ -5282,8 +5422,20 @@
       <c r="Z10" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA10" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="AB10" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AC10" s="1">
+        <v>3</v>
+      </c>
+      <c r="AD10" s="1" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>73</v>
       </c>
@@ -5364,8 +5516,20 @@
       <c r="Z11" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA11" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="AB11" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AC11" s="7">
+        <v>2</v>
+      </c>
+      <c r="AD11" s="1" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>73</v>
       </c>
@@ -5446,8 +5610,20 @@
       <c r="Z12" s="1">
         <v>9</v>
       </c>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA12" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="AB12" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AC12" s="7">
+        <v>2</v>
+      </c>
+      <c r="AD12" s="1" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>73</v>
       </c>
@@ -5528,8 +5704,20 @@
       <c r="Z13" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA13" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="AB13" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AC13" s="7">
+        <v>4</v>
+      </c>
+      <c r="AD13" s="1" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>73</v>
       </c>
@@ -5610,8 +5798,20 @@
       <c r="Z14" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA14" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="AB14" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AC14" s="1">
+        <v>3</v>
+      </c>
+      <c r="AD14" s="1" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>73</v>
       </c>
@@ -5692,8 +5892,20 @@
       <c r="Z15" s="1">
         <v>11</v>
       </c>
-    </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA15" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="AB15" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AC15" s="1">
+        <v>4</v>
+      </c>
+      <c r="AD15" s="1" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>73</v>
       </c>
@@ -5774,8 +5986,20 @@
       <c r="Z16" s="1">
         <v>11</v>
       </c>
-    </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA16" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="AB16" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AC16" s="1">
+        <v>2</v>
+      </c>
+      <c r="AD16" s="1" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="17" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>73</v>
       </c>
@@ -5856,8 +6080,20 @@
       <c r="Z17" s="1">
         <v>9</v>
       </c>
-    </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA17" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="AB17" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AC17" s="7">
+        <v>1</v>
+      </c>
+      <c r="AD17" s="1" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="18" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>73</v>
       </c>
@@ -5938,8 +6174,20 @@
       <c r="Z18" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA18" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="AB18" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AC18" s="7">
+        <v>2</v>
+      </c>
+      <c r="AD18" s="1" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="19" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>73</v>
       </c>
@@ -6020,8 +6268,20 @@
       <c r="Z19" s="1">
         <v>9</v>
       </c>
-    </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA19" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="AB19" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AC19" s="7">
+        <v>3</v>
+      </c>
+      <c r="AD19" s="1" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="20" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>73</v>
       </c>
@@ -6102,6 +6362,32 @@
       <c r="Z20" s="1">
         <v>8</v>
       </c>
+      <c r="AA20" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="AB20" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AC20" s="7">
+        <v>1</v>
+      </c>
+      <c r="AD20" s="1" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="21" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AC21" s="7"/>
+    </row>
+    <row r="22" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AC22" s="7"/>
+    </row>
+    <row r="23" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AC23" s="7"/>
+      <c r="AD23" s="7"/>
+    </row>
+    <row r="24" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AC24" s="7"/>
+      <c r="AD24" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
@@ -8885,7 +9171,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE53"/>
   <sheetViews>
-    <sheetView topLeftCell="Z1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AB30" sqref="AB30"/>
     </sheetView>
   </sheetViews>
@@ -13120,8 +13406,8 @@
   </sheetPr>
   <dimension ref="A1:AC1048576"/>
   <sheetViews>
-    <sheetView topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView topLeftCell="Y1" workbookViewId="0">
+      <selection activeCell="AA1" sqref="AA1:AC1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
All code + excel updated (not for clust aggregation)
</commit_message>
<xml_diff>
--- a/config/SFN_NHP_Coordinates_All.xlsx
+++ b/config/SFN_NHP_Coordinates_All.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27011"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elseyjg/temp/schalllab-spatial/config/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/subravcr/Projects/lab-schall/schalllab-spatial/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5220" yWindow="460" windowWidth="30860" windowHeight="19440" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="5220" yWindow="460" windowWidth="30860" windowHeight="19440" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Br" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1904" uniqueCount="432">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1904" uniqueCount="436">
   <si>
     <t>a3</t>
   </si>
@@ -1166,54 +1166,12 @@
     <t>Users/Kaleb/dataProcessed/Init_SetUp-160715-150111/Channel*/chan*.mat</t>
   </si>
   <si>
-    <t>Users/Kaleb/dataProcessed/Init_SetUp-160802-144253/Channel*/chan*.mat</t>
-  </si>
-  <si>
-    <t>Users/Kaleb/dataProcessed/Init_SetUp-160711-151215/Channel*/chan*.mat</t>
-  </si>
-  <si>
-    <t>Users/Kaleb/dataProcessed/Init_SetUp-160808-152950/Channel*/chan*.mat</t>
-  </si>
-  <si>
-    <t>Users/Kaleb/dataProcessed/Init_SetUp-160811-145107/Channel*/chan*.mat</t>
-  </si>
-  <si>
-    <t>Users/Kaleb/dataProcessed/Init_SetUp-160812-150028/Channel*/chan*.mat</t>
-  </si>
-  <si>
-    <t>Users/Kaleb/dataProcessed/Init_SetUp-160816-145437/Channel*/chan*.mat</t>
-  </si>
-  <si>
     <t>Users/Kaleb/dataProcessed/Init_SetUp-160819-152223/Channel*/chan*.mat</t>
   </si>
   <si>
-    <t>Users/Kaleb/dataProcessed/Init_SetUp-160829-153146/Channel*/chan*.mat</t>
-  </si>
-  <si>
-    <t>Users/Kaleb/dataProcessed/Init_SetUp-160831-144727/Channel*/chan*.mat</t>
-  </si>
-  <si>
-    <t>Users/Kaleb/dataProcessed/Init_SetUp-160909-132302/Channel*/chan*.mat</t>
-  </si>
-  <si>
     <t>Users/Kaleb/dataProcessed/Init_SetUp-160912-135839/Channel*/chan*.mat</t>
   </si>
   <si>
-    <t>Users/Kaleb/dataProcessed/Init_SetUp-160921-141512/Channel*/chan*.mat</t>
-  </si>
-  <si>
-    <t>Users/Kaleb/dataProcessed/Init_SetUp-160926-134654/Channel*/chan*.mat</t>
-  </si>
-  <si>
-    <t>Users/Kaleb/dataProcessed/Init_SetUp-160928-132038/Channel*/chan*.mat</t>
-  </si>
-  <si>
-    <t>Users/Kaleb/dataProcessed/Init_SetUp-161003-134515/Channel*/chan*.mat</t>
-  </si>
-  <si>
-    <t>Users/Kaleb/dataProcessed/Init_SetUp-161005-134520/Channel*/chan*.mat</t>
-  </si>
-  <si>
     <t>probeNo</t>
   </si>
   <si>
@@ -1329,6 +1287,60 @@
   </si>
   <si>
     <t>few clusters, sparcely connected</t>
+  </si>
+  <si>
+    <t>Users/Kaleb/dataProcessed/Init_SetUp-160711-151215/Channel*/*MUA.mat</t>
+  </si>
+  <si>
+    <t>Users/Kaleb/dataProcessed/Init_SetUp-160713-144841/Channel*/*MUA.mat</t>
+  </si>
+  <si>
+    <t>Users/Kaleb/dataProcessed/Init_SetUp-160715-150111/Channel*/*MUA.mat</t>
+  </si>
+  <si>
+    <t>Users/Kaleb/dataProcessed/Init_SetUp-160802-144253/Channel*/*MUA.mat</t>
+  </si>
+  <si>
+    <t>Users/Kaleb/dataProcessed/Init_SetUp-160808-152950/Channel*/*MUA.mat</t>
+  </si>
+  <si>
+    <t>Users/Kaleb/dataProcessed/Init_SetUp-160811-145107/Channel*/*MUA.mat</t>
+  </si>
+  <si>
+    <t>Users/Kaleb/dataProcessed/Init_SetUp-160812-150028/Channel*/*MUA.mat</t>
+  </si>
+  <si>
+    <t>Users/Kaleb/dataProcessed/Init_SetUp-160816-145437/Channel*/*MUA.mat</t>
+  </si>
+  <si>
+    <t>Users/Kaleb/dataProcessed/Init_SetUp-160819-152223/Channel*/*MUA.mat</t>
+  </si>
+  <si>
+    <t>Users/Kaleb/dataProcessed/Init_SetUp-160829-153146/Channel*/*MUA.mat</t>
+  </si>
+  <si>
+    <t>Users/Kaleb/dataProcessed/Init_SetUp-160831-144727/Channel*/*MUA.mat</t>
+  </si>
+  <si>
+    <t>Users/Kaleb/dataProcessed/Init_SetUp-160909-132302/Channel*/*MUA.mat</t>
+  </si>
+  <si>
+    <t>Users/Kaleb/dataProcessed/Init_SetUp-160912-135839/Channel*/*MUA.mat</t>
+  </si>
+  <si>
+    <t>Users/Kaleb/dataProcessed/Init_SetUp-160921-141512/Channel*/*MUA.mat</t>
+  </si>
+  <si>
+    <t>Users/Kaleb/dataProcessed/Init_SetUp-160926-134654/Channel*/*MUA.mat</t>
+  </si>
+  <si>
+    <t>Users/Kaleb/dataProcessed/Init_SetUp-160928-132038/Channel*/*MUA.mat</t>
+  </si>
+  <si>
+    <t>Users/Kaleb/dataProcessed/Init_SetUp-161003-134515/Channel*/*MUA.mat</t>
+  </si>
+  <si>
+    <t>Users/Kaleb/dataProcessed/Init_SetUp-161005-134520/Channel*/*MUA.mat</t>
   </si>
 </sst>
 </file>
@@ -2419,13 +2431,13 @@
         <v>81</v>
       </c>
       <c r="AA1" s="6" t="s">
-        <v>394</v>
+        <v>380</v>
       </c>
       <c r="AB1" s="6" t="s">
-        <v>395</v>
+        <v>381</v>
       </c>
       <c r="AC1" s="6" t="s">
-        <v>396</v>
+        <v>382</v>
       </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.2">
@@ -2517,7 +2529,7 @@
         <v>3</v>
       </c>
       <c r="AC2" s="1" t="s">
-        <v>418</v>
+        <v>404</v>
       </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.2">
@@ -2609,7 +2621,7 @@
         <v>2</v>
       </c>
       <c r="AC3" s="1" t="s">
-        <v>419</v>
+        <v>405</v>
       </c>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.2">
@@ -2701,7 +2713,7 @@
         <v>3</v>
       </c>
       <c r="AC4" s="1" t="s">
-        <v>410</v>
+        <v>396</v>
       </c>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.2">
@@ -2793,7 +2805,7 @@
         <v>4</v>
       </c>
       <c r="AC5" s="1" t="s">
-        <v>420</v>
+        <v>406</v>
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.2">
@@ -2885,7 +2897,7 @@
         <v>4</v>
       </c>
       <c r="AC6" s="1" t="s">
-        <v>420</v>
+        <v>406</v>
       </c>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.2">
@@ -2977,7 +2989,7 @@
         <v>4</v>
       </c>
       <c r="AC7" s="1" t="s">
-        <v>420</v>
+        <v>406</v>
       </c>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.2">
@@ -3069,7 +3081,7 @@
         <v>3</v>
       </c>
       <c r="AC8" s="1" t="s">
-        <v>421</v>
+        <v>407</v>
       </c>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.2">
@@ -3161,7 +3173,7 @@
         <v>2</v>
       </c>
       <c r="AC9" s="1" t="s">
-        <v>422</v>
+        <v>408</v>
       </c>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.2">
@@ -3253,7 +3265,7 @@
         <v>4</v>
       </c>
       <c r="AC10" s="1" t="s">
-        <v>420</v>
+        <v>406</v>
       </c>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.2">
@@ -3345,7 +3357,7 @@
         <v>2</v>
       </c>
       <c r="AC11" s="1" t="s">
-        <v>422</v>
+        <v>408</v>
       </c>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.2">
@@ -3437,7 +3449,7 @@
         <v>3</v>
       </c>
       <c r="AC12" s="1" t="s">
-        <v>421</v>
+        <v>407</v>
       </c>
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.2">
@@ -3529,7 +3541,7 @@
         <v>2</v>
       </c>
       <c r="AC13" s="1" t="s">
-        <v>422</v>
+        <v>408</v>
       </c>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.2">
@@ -3621,7 +3633,7 @@
         <v>3</v>
       </c>
       <c r="AC14" s="1" t="s">
-        <v>421</v>
+        <v>407</v>
       </c>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.2">
@@ -3713,7 +3725,7 @@
         <v>3</v>
       </c>
       <c r="AC15" s="1" t="s">
-        <v>421</v>
+        <v>407</v>
       </c>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.2">
@@ -3805,7 +3817,7 @@
         <v>4</v>
       </c>
       <c r="AC16" s="1" t="s">
-        <v>421</v>
+        <v>407</v>
       </c>
     </row>
     <row r="17" spans="1:29" x14ac:dyDescent="0.2">
@@ -3897,7 +3909,7 @@
         <v>4</v>
       </c>
       <c r="AC17" s="1" t="s">
-        <v>420</v>
+        <v>406</v>
       </c>
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.2">
@@ -3989,7 +4001,7 @@
         <v>3</v>
       </c>
       <c r="AC18" s="1" t="s">
-        <v>421</v>
+        <v>407</v>
       </c>
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.2">
@@ -4081,7 +4093,7 @@
         <v>4</v>
       </c>
       <c r="AC19" s="1" t="s">
-        <v>420</v>
+        <v>406</v>
       </c>
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.2">
@@ -4173,7 +4185,7 @@
         <v>4</v>
       </c>
       <c r="AC20" s="1" t="s">
-        <v>423</v>
+        <v>409</v>
       </c>
     </row>
     <row r="21" spans="1:29" x14ac:dyDescent="0.2">
@@ -4265,7 +4277,7 @@
         <v>4</v>
       </c>
       <c r="AC21" s="1" t="s">
-        <v>420</v>
+        <v>406</v>
       </c>
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.2">
@@ -4357,7 +4369,7 @@
         <v>4</v>
       </c>
       <c r="AC22" s="1" t="s">
-        <v>420</v>
+        <v>406</v>
       </c>
     </row>
     <row r="23" spans="1:29" x14ac:dyDescent="0.2">
@@ -4463,7 +4475,7 @@
   </sheetPr>
   <dimension ref="A1:AD24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z1" workbookViewId="0">
+    <sheetView topLeftCell="Z1" workbookViewId="0">
       <selection activeCell="AC21" sqref="AC21"/>
     </sheetView>
   </sheetViews>
@@ -4580,13 +4592,13 @@
         <v>122</v>
       </c>
       <c r="AB1" s="6" t="s">
-        <v>394</v>
+        <v>380</v>
       </c>
       <c r="AC1" s="6" t="s">
-        <v>395</v>
+        <v>381</v>
       </c>
       <c r="AD1" s="6" t="s">
-        <v>396</v>
+        <v>382</v>
       </c>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.2">
@@ -4680,7 +4692,7 @@
         <v>2</v>
       </c>
       <c r="AD2" s="7" t="s">
-        <v>422</v>
+        <v>408</v>
       </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.2">
@@ -4774,7 +4786,7 @@
         <v>1</v>
       </c>
       <c r="AD3" s="1" t="s">
-        <v>424</v>
+        <v>410</v>
       </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.2">
@@ -4868,7 +4880,7 @@
         <v>2</v>
       </c>
       <c r="AD4" s="1" t="s">
-        <v>425</v>
+        <v>411</v>
       </c>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.2">
@@ -4962,7 +4974,7 @@
         <v>4</v>
       </c>
       <c r="AD5" s="1" t="s">
-        <v>426</v>
+        <v>412</v>
       </c>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.2">
@@ -5056,7 +5068,7 @@
         <v>3</v>
       </c>
       <c r="AD6" s="1" t="s">
-        <v>426</v>
+        <v>412</v>
       </c>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.2">
@@ -5150,7 +5162,7 @@
         <v>2</v>
       </c>
       <c r="AD7" s="1" t="s">
-        <v>402</v>
+        <v>388</v>
       </c>
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.2">
@@ -5244,7 +5256,7 @@
         <v>4</v>
       </c>
       <c r="AD8" s="1" t="s">
-        <v>425</v>
+        <v>411</v>
       </c>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.2">
@@ -5338,7 +5350,7 @@
         <v>2</v>
       </c>
       <c r="AD9" s="1" t="s">
-        <v>400</v>
+        <v>386</v>
       </c>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.2">
@@ -5432,7 +5444,7 @@
         <v>3</v>
       </c>
       <c r="AD10" s="1" t="s">
-        <v>412</v>
+        <v>398</v>
       </c>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.2">
@@ -5526,7 +5538,7 @@
         <v>2</v>
       </c>
       <c r="AD11" s="1" t="s">
-        <v>400</v>
+        <v>386</v>
       </c>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.2">
@@ -5620,7 +5632,7 @@
         <v>2</v>
       </c>
       <c r="AD12" s="1" t="s">
-        <v>427</v>
+        <v>413</v>
       </c>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.2">
@@ -5714,7 +5726,7 @@
         <v>4</v>
       </c>
       <c r="AD13" s="1" t="s">
-        <v>428</v>
+        <v>414</v>
       </c>
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.2">
@@ -5808,7 +5820,7 @@
         <v>3</v>
       </c>
       <c r="AD14" s="1" t="s">
-        <v>429</v>
+        <v>415</v>
       </c>
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.2">
@@ -5902,7 +5914,7 @@
         <v>4</v>
       </c>
       <c r="AD15" s="1" t="s">
-        <v>430</v>
+        <v>416</v>
       </c>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.2">
@@ -5996,7 +6008,7 @@
         <v>2</v>
       </c>
       <c r="AD16" s="1" t="s">
-        <v>402</v>
+        <v>388</v>
       </c>
     </row>
     <row r="17" spans="1:30" x14ac:dyDescent="0.2">
@@ -6090,7 +6102,7 @@
         <v>1</v>
       </c>
       <c r="AD17" s="1" t="s">
-        <v>398</v>
+        <v>384</v>
       </c>
     </row>
     <row r="18" spans="1:30" x14ac:dyDescent="0.2">
@@ -6184,7 +6196,7 @@
         <v>2</v>
       </c>
       <c r="AD18" s="1" t="s">
-        <v>412</v>
+        <v>398</v>
       </c>
     </row>
     <row r="19" spans="1:30" x14ac:dyDescent="0.2">
@@ -6278,7 +6290,7 @@
         <v>3</v>
       </c>
       <c r="AD19" s="1" t="s">
-        <v>431</v>
+        <v>417</v>
       </c>
     </row>
     <row r="20" spans="1:30" x14ac:dyDescent="0.2">
@@ -6372,7 +6384,7 @@
         <v>1</v>
       </c>
       <c r="AD20" s="1" t="s">
-        <v>424</v>
+        <v>410</v>
       </c>
     </row>
     <row r="21" spans="1:30" x14ac:dyDescent="0.2">
@@ -6517,13 +6529,13 @@
         <v>81</v>
       </c>
       <c r="AA1" s="6" t="s">
-        <v>394</v>
+        <v>380</v>
       </c>
       <c r="AB1" s="6" t="s">
-        <v>395</v>
+        <v>381</v>
       </c>
       <c r="AC1" s="6" t="s">
-        <v>396</v>
+        <v>382</v>
       </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.2">
@@ -6615,7 +6627,7 @@
         <v>4</v>
       </c>
       <c r="AC2" s="1" t="s">
-        <v>417</v>
+        <v>403</v>
       </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.2">
@@ -6707,7 +6719,7 @@
         <v>4</v>
       </c>
       <c r="AC3" s="1" t="s">
-        <v>417</v>
+        <v>403</v>
       </c>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.2">
@@ -6799,7 +6811,7 @@
         <v>4</v>
       </c>
       <c r="AC4" s="1" t="s">
-        <v>417</v>
+        <v>403</v>
       </c>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.2">
@@ -6891,7 +6903,7 @@
         <v>2</v>
       </c>
       <c r="AC5" s="1" t="s">
-        <v>407</v>
+        <v>393</v>
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.2">
@@ -6983,7 +6995,7 @@
         <v>4</v>
       </c>
       <c r="AC6" s="1" t="s">
-        <v>417</v>
+        <v>403</v>
       </c>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.2">
@@ -7075,7 +7087,7 @@
         <v>4</v>
       </c>
       <c r="AC7" s="1" t="s">
-        <v>405</v>
+        <v>391</v>
       </c>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.2">
@@ -7167,7 +7179,7 @@
         <v>2</v>
       </c>
       <c r="AC8" s="1" t="s">
-        <v>407</v>
+        <v>393</v>
       </c>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.2">
@@ -7259,7 +7271,7 @@
         <v>4</v>
       </c>
       <c r="AC9" s="1" t="s">
-        <v>417</v>
+        <v>403</v>
       </c>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.2">
@@ -7351,7 +7363,7 @@
         <v>4</v>
       </c>
       <c r="AC10" s="1" t="s">
-        <v>417</v>
+        <v>403</v>
       </c>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.2">
@@ -7443,7 +7455,7 @@
         <v>4</v>
       </c>
       <c r="AC11" s="7" t="s">
-        <v>417</v>
+        <v>403</v>
       </c>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.2">
@@ -7535,7 +7547,7 @@
         <v>4</v>
       </c>
       <c r="AC12" s="7" t="s">
-        <v>417</v>
+        <v>403</v>
       </c>
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.2">
@@ -7627,7 +7639,7 @@
         <v>4</v>
       </c>
       <c r="AC13" s="7" t="s">
-        <v>417</v>
+        <v>403</v>
       </c>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.2">
@@ -9171,8 +9183,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AB30" sqref="AB30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I44" sqref="I44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9224,7 +9236,7 @@
         <v>94</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>393</v>
+        <v>379</v>
       </c>
       <c r="K1" s="6" t="s">
         <v>93</v>
@@ -9281,13 +9293,13 @@
         <v>81</v>
       </c>
       <c r="AC1" s="6" t="s">
-        <v>394</v>
+        <v>380</v>
       </c>
       <c r="AD1" s="6" t="s">
-        <v>395</v>
+        <v>381</v>
       </c>
       <c r="AE1" s="6" t="s">
-        <v>396</v>
+        <v>382</v>
       </c>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.2">
@@ -9316,7 +9328,7 @@
         <v>16</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>378</v>
+        <v>418</v>
       </c>
       <c r="J2" s="7">
         <v>1</v>
@@ -9383,7 +9395,7 @@
         <v>4</v>
       </c>
       <c r="AE2" s="1" t="s">
-        <v>416</v>
+        <v>402</v>
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.2">
@@ -9412,7 +9424,7 @@
         <v>17</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>375</v>
+        <v>419</v>
       </c>
       <c r="J3" s="7">
         <v>1</v>
@@ -9479,7 +9491,7 @@
         <v>4</v>
       </c>
       <c r="AE3" s="1" t="s">
-        <v>417</v>
+        <v>403</v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.2">
@@ -9508,7 +9520,7 @@
         <v>18</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>376</v>
+        <v>420</v>
       </c>
       <c r="J4" s="7">
         <v>1</v>
@@ -9595,7 +9607,7 @@
         <v>19</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>377</v>
+        <v>421</v>
       </c>
       <c r="J5" s="7">
         <v>1</v>
@@ -9662,7 +9674,7 @@
         <v>4</v>
       </c>
       <c r="AE5" s="1" t="s">
-        <v>417</v>
+        <v>403</v>
       </c>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.2">
@@ -9691,7 +9703,7 @@
         <v>20</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>379</v>
+        <v>422</v>
       </c>
       <c r="J6" s="7">
         <v>1</v>
@@ -9758,7 +9770,7 @@
         <v>4</v>
       </c>
       <c r="AE6" s="1" t="s">
-        <v>417</v>
+        <v>403</v>
       </c>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.2">
@@ -9787,7 +9799,7 @@
         <v>21</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>380</v>
+        <v>423</v>
       </c>
       <c r="J7" s="7">
         <v>1</v>
@@ -9854,7 +9866,7 @@
         <v>4</v>
       </c>
       <c r="AE7" s="1" t="s">
-        <v>417</v>
+        <v>403</v>
       </c>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.2">
@@ -9883,7 +9895,7 @@
         <v>22</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>381</v>
+        <v>424</v>
       </c>
       <c r="J8" s="7">
         <v>1</v>
@@ -9950,7 +9962,7 @@
         <v>4</v>
       </c>
       <c r="AE8" s="1" t="s">
-        <v>416</v>
+        <v>402</v>
       </c>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.2">
@@ -9979,7 +9991,7 @@
         <v>24</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>382</v>
+        <v>425</v>
       </c>
       <c r="J9" s="7">
         <v>1</v>
@@ -10046,7 +10058,7 @@
         <v>4</v>
       </c>
       <c r="AE9" s="1" t="s">
-        <v>416</v>
+        <v>402</v>
       </c>
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.2">
@@ -10075,7 +10087,7 @@
         <v>25</v>
       </c>
       <c r="I10" s="47" t="s">
-        <v>383</v>
+        <v>426</v>
       </c>
       <c r="J10" s="47">
         <v>1</v>
@@ -10162,7 +10174,7 @@
         <v>26</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>384</v>
+        <v>427</v>
       </c>
       <c r="J11" s="7">
         <v>1</v>
@@ -10229,7 +10241,7 @@
         <v>4</v>
       </c>
       <c r="AE11" s="1" t="s">
-        <v>416</v>
+        <v>402</v>
       </c>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.2">
@@ -10258,7 +10270,7 @@
         <v>27</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>385</v>
+        <v>428</v>
       </c>
       <c r="J12" s="7">
         <v>1</v>
@@ -10325,7 +10337,7 @@
         <v>4</v>
       </c>
       <c r="AE12" s="1" t="s">
-        <v>417</v>
+        <v>403</v>
       </c>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.2">
@@ -10354,7 +10366,7 @@
         <v>28</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>386</v>
+        <v>429</v>
       </c>
       <c r="J13" s="7">
         <v>1</v>
@@ -10421,7 +10433,7 @@
         <v>4</v>
       </c>
       <c r="AE13" s="1" t="s">
-        <v>417</v>
+        <v>403</v>
       </c>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.2">
@@ -10450,7 +10462,7 @@
         <v>28</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>386</v>
+        <v>429</v>
       </c>
       <c r="J14" s="7">
         <v>2</v>
@@ -10537,7 +10549,7 @@
         <v>29</v>
       </c>
       <c r="I15" s="41" t="s">
-        <v>387</v>
+        <v>430</v>
       </c>
       <c r="J15" s="41">
         <v>1</v>
@@ -10624,7 +10636,7 @@
         <v>29</v>
       </c>
       <c r="I16" s="41" t="s">
-        <v>387</v>
+        <v>430</v>
       </c>
       <c r="J16" s="41">
         <v>2</v>
@@ -10711,7 +10723,7 @@
         <v>30</v>
       </c>
       <c r="I17" s="47" t="s">
-        <v>388</v>
+        <v>431</v>
       </c>
       <c r="J17" s="47">
         <v>1</v>
@@ -10778,7 +10790,7 @@
         <v>4</v>
       </c>
       <c r="AE17" s="1" t="s">
-        <v>416</v>
+        <v>402</v>
       </c>
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.2">
@@ -10807,7 +10819,7 @@
         <v>30</v>
       </c>
       <c r="I18" s="47" t="s">
-        <v>388</v>
+        <v>431</v>
       </c>
       <c r="J18" s="47">
         <v>2</v>
@@ -10874,7 +10886,7 @@
         <v>4</v>
       </c>
       <c r="AE18" s="1" t="s">
-        <v>416</v>
+        <v>402</v>
       </c>
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.2">
@@ -10903,7 +10915,7 @@
         <v>32</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>389</v>
+        <v>432</v>
       </c>
       <c r="J19" s="7">
         <v>1</v>
@@ -10970,7 +10982,7 @@
         <v>4</v>
       </c>
       <c r="AE19" s="1" t="s">
-        <v>416</v>
+        <v>402</v>
       </c>
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.2">
@@ -10999,7 +11011,7 @@
         <v>32</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>389</v>
+        <v>432</v>
       </c>
       <c r="J20" s="7">
         <v>2</v>
@@ -11066,7 +11078,7 @@
         <v>4</v>
       </c>
       <c r="AE20" s="1" t="s">
-        <v>416</v>
+        <v>402</v>
       </c>
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.2">
@@ -11095,7 +11107,7 @@
         <v>33</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>390</v>
+        <v>433</v>
       </c>
       <c r="J21" s="7">
         <v>1</v>
@@ -11162,7 +11174,7 @@
         <v>4</v>
       </c>
       <c r="AE21" s="1" t="s">
-        <v>417</v>
+        <v>403</v>
       </c>
     </row>
     <row r="22" spans="1:31" x14ac:dyDescent="0.2">
@@ -11191,7 +11203,7 @@
         <v>33</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>390</v>
+        <v>433</v>
       </c>
       <c r="J22" s="7">
         <v>2</v>
@@ -11258,7 +11270,7 @@
         <v>4</v>
       </c>
       <c r="AE22" s="1" t="s">
-        <v>417</v>
+        <v>403</v>
       </c>
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.2">
@@ -11287,7 +11299,7 @@
         <v>34</v>
       </c>
       <c r="I23" s="53" t="s">
-        <v>391</v>
+        <v>434</v>
       </c>
       <c r="J23" s="53">
         <v>2</v>
@@ -11354,7 +11366,7 @@
         <v>4</v>
       </c>
       <c r="AE23" s="7" t="s">
-        <v>416</v>
+        <v>402</v>
       </c>
     </row>
     <row r="24" spans="1:31" x14ac:dyDescent="0.2">
@@ -11383,7 +11395,7 @@
         <v>35</v>
       </c>
       <c r="I24" s="7" t="s">
-        <v>392</v>
+        <v>435</v>
       </c>
       <c r="J24" s="7">
         <v>2</v>
@@ -11450,7 +11462,7 @@
         <v>4</v>
       </c>
       <c r="AE24" s="7" t="s">
-        <v>416</v>
+        <v>402</v>
       </c>
     </row>
     <row r="31" spans="1:31" x14ac:dyDescent="0.2">
@@ -11818,7 +11830,7 @@
         <v>25</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>383</v>
+        <v>377</v>
       </c>
       <c r="J4" s="7" t="s">
         <v>299</v>
@@ -11902,7 +11914,7 @@
         <v>29</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>387</v>
+        <v>378</v>
       </c>
       <c r="J5" s="7" t="s">
         <v>303</v>
@@ -12085,13 +12097,13 @@
         <v>97</v>
       </c>
       <c r="AA1" s="6" t="s">
-        <v>394</v>
+        <v>380</v>
       </c>
       <c r="AB1" s="6" t="s">
-        <v>395</v>
+        <v>381</v>
       </c>
       <c r="AC1" s="6" t="s">
-        <v>396</v>
+        <v>382</v>
       </c>
     </row>
     <row r="2" spans="1:29" ht="17" x14ac:dyDescent="0.2">
@@ -12183,7 +12195,7 @@
         <v>3</v>
       </c>
       <c r="AC2" s="1" t="s">
-        <v>405</v>
+        <v>391</v>
       </c>
     </row>
     <row r="3" spans="1:29" ht="17" x14ac:dyDescent="0.2">
@@ -12275,7 +12287,7 @@
         <v>2</v>
       </c>
       <c r="AC3" s="1" t="s">
-        <v>406</v>
+        <v>392</v>
       </c>
     </row>
     <row r="4" spans="1:29" ht="17" x14ac:dyDescent="0.2">
@@ -12367,7 +12379,7 @@
         <v>2</v>
       </c>
       <c r="AC4" s="1" t="s">
-        <v>407</v>
+        <v>393</v>
       </c>
     </row>
     <row r="5" spans="1:29" ht="17" x14ac:dyDescent="0.2">
@@ -12459,7 +12471,7 @@
         <v>2</v>
       </c>
       <c r="AC5" s="1" t="s">
-        <v>408</v>
+        <v>394</v>
       </c>
     </row>
     <row r="6" spans="1:29" ht="17" x14ac:dyDescent="0.2">
@@ -12551,7 +12563,7 @@
         <v>3</v>
       </c>
       <c r="AC6" s="1" t="s">
-        <v>409</v>
+        <v>395</v>
       </c>
     </row>
     <row r="7" spans="1:29" ht="17" x14ac:dyDescent="0.2">
@@ -12643,7 +12655,7 @@
         <v>4</v>
       </c>
       <c r="AC7" s="1" t="s">
-        <v>410</v>
+        <v>396</v>
       </c>
     </row>
     <row r="8" spans="1:29" ht="17" x14ac:dyDescent="0.2">
@@ -12735,7 +12747,7 @@
         <v>2</v>
       </c>
       <c r="AC8" s="1" t="s">
-        <v>411</v>
+        <v>397</v>
       </c>
     </row>
     <row r="9" spans="1:29" ht="17" x14ac:dyDescent="0.2">
@@ -12827,7 +12839,7 @@
         <v>3</v>
       </c>
       <c r="AC9" s="1" t="s">
-        <v>412</v>
+        <v>398</v>
       </c>
     </row>
     <row r="10" spans="1:29" ht="17" x14ac:dyDescent="0.2">
@@ -12919,7 +12931,7 @@
         <v>4</v>
       </c>
       <c r="AC10" s="1" t="s">
-        <v>413</v>
+        <v>399</v>
       </c>
     </row>
     <row r="11" spans="1:29" ht="17" x14ac:dyDescent="0.2">
@@ -13011,7 +13023,7 @@
         <v>3</v>
       </c>
       <c r="AC11" s="1" t="s">
-        <v>414</v>
+        <v>400</v>
       </c>
     </row>
     <row r="12" spans="1:29" ht="17" x14ac:dyDescent="0.2">
@@ -13103,7 +13115,7 @@
         <v>1</v>
       </c>
       <c r="AC12" s="1" t="s">
-        <v>400</v>
+        <v>386</v>
       </c>
     </row>
     <row r="13" spans="1:29" ht="17" x14ac:dyDescent="0.2">
@@ -13195,7 +13207,7 @@
         <v>1</v>
       </c>
       <c r="AC13" s="1" t="s">
-        <v>400</v>
+        <v>386</v>
       </c>
     </row>
     <row r="14" spans="1:29" ht="17" x14ac:dyDescent="0.2">
@@ -13287,7 +13299,7 @@
         <v>3</v>
       </c>
       <c r="AC14" s="1" t="s">
-        <v>415</v>
+        <v>401</v>
       </c>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.2">
@@ -13510,13 +13522,13 @@
         <v>97</v>
       </c>
       <c r="AA1" s="6" t="s">
-        <v>394</v>
+        <v>380</v>
       </c>
       <c r="AB1" s="6" t="s">
-        <v>395</v>
+        <v>381</v>
       </c>
       <c r="AC1" s="6" t="s">
-        <v>396</v>
+        <v>382</v>
       </c>
     </row>
     <row r="2" spans="1:29" ht="17" x14ac:dyDescent="0.2">
@@ -13608,7 +13620,7 @@
         <v>2</v>
       </c>
       <c r="AC2" s="1" t="s">
-        <v>397</v>
+        <v>383</v>
       </c>
     </row>
     <row r="3" spans="1:29" ht="17" x14ac:dyDescent="0.2">
@@ -13700,7 +13712,7 @@
         <v>2</v>
       </c>
       <c r="AC3" s="1" t="s">
-        <v>397</v>
+        <v>383</v>
       </c>
     </row>
     <row r="4" spans="1:29" ht="17" x14ac:dyDescent="0.2">
@@ -13792,7 +13804,7 @@
         <v>1</v>
       </c>
       <c r="AC4" s="1" t="s">
-        <v>398</v>
+        <v>384</v>
       </c>
     </row>
     <row r="5" spans="1:29" ht="17" x14ac:dyDescent="0.2">
@@ -13884,7 +13896,7 @@
         <v>1</v>
       </c>
       <c r="AC5" s="1" t="s">
-        <v>399</v>
+        <v>385</v>
       </c>
     </row>
     <row r="6" spans="1:29" ht="17" x14ac:dyDescent="0.2">
@@ -13976,7 +13988,7 @@
         <v>3</v>
       </c>
       <c r="AC6" s="1" t="s">
-        <v>397</v>
+        <v>383</v>
       </c>
     </row>
     <row r="7" spans="1:29" ht="17" x14ac:dyDescent="0.2">
@@ -14068,7 +14080,7 @@
         <v>1</v>
       </c>
       <c r="AC7" s="1" t="s">
-        <v>398</v>
+        <v>384</v>
       </c>
     </row>
     <row r="8" spans="1:29" ht="17" x14ac:dyDescent="0.2">
@@ -14160,7 +14172,7 @@
         <v>1</v>
       </c>
       <c r="AC8" s="1" t="s">
-        <v>400</v>
+        <v>386</v>
       </c>
     </row>
     <row r="9" spans="1:29" ht="17" x14ac:dyDescent="0.2">
@@ -14252,7 +14264,7 @@
         <v>3</v>
       </c>
       <c r="AC9" s="1" t="s">
-        <v>401</v>
+        <v>387</v>
       </c>
     </row>
     <row r="10" spans="1:29" ht="17" x14ac:dyDescent="0.2">
@@ -14344,7 +14356,7 @@
         <v>2</v>
       </c>
       <c r="AC10" s="1" t="s">
-        <v>402</v>
+        <v>388</v>
       </c>
     </row>
     <row r="11" spans="1:29" ht="17" x14ac:dyDescent="0.2">
@@ -14436,7 +14448,7 @@
         <v>3</v>
       </c>
       <c r="AC11" s="1" t="s">
-        <v>403</v>
+        <v>389</v>
       </c>
     </row>
     <row r="12" spans="1:29" ht="17" x14ac:dyDescent="0.2">
@@ -14528,7 +14540,7 @@
         <v>3</v>
       </c>
       <c r="AC12" s="1" t="s">
-        <v>403</v>
+        <v>389</v>
       </c>
     </row>
     <row r="13" spans="1:29" ht="17" x14ac:dyDescent="0.2">
@@ -14620,7 +14632,7 @@
         <v>3</v>
       </c>
       <c r="AC13" s="1" t="s">
-        <v>404</v>
+        <v>390</v>
       </c>
     </row>
     <row r="14" spans="1:29" ht="17" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Updated for by position computation and taskType
</commit_message>
<xml_diff>
--- a/config/SFN_NHP_Coordinates_All.xlsx
+++ b/config/SFN_NHP_Coordinates_All.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27011"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elseyjg/temp/schalllab-spatial/config/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/subravcr/Projects/lab-schall/schalllab-spatial/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4240" yWindow="460" windowWidth="30860" windowHeight="19440" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="4240" yWindow="460" windowWidth="30860" windowHeight="19440" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Br" sheetId="2" r:id="rId1"/>
     <sheet name="Jo" sheetId="1" r:id="rId2"/>
     <sheet name="Da_WJ" sheetId="6" r:id="rId3"/>
     <sheet name="Da_K" sheetId="7" r:id="rId4"/>
-    <sheet name="TestDarwin" sheetId="8" r:id="rId5"/>
-    <sheet name="Ga" sheetId="4" r:id="rId6"/>
-    <sheet name="He" sheetId="5" r:id="rId7"/>
+    <sheet name="Ga" sheetId="4" r:id="rId5"/>
+    <sheet name="He" sheetId="5" r:id="rId6"/>
+    <sheet name="Test" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1890" uniqueCount="439">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1882" uniqueCount="435">
   <si>
     <t>a3</t>
   </si>
@@ -1143,18 +1143,6 @@
   </si>
   <si>
     <t>Users/Wolf/ephys_db/Helmholtz/2015-03-12a/DSP/DSP*/*MG*.mat</t>
-  </si>
-  <si>
-    <t>Users/Kaleb/dataProcessed/Init_SetUp-160713-144841/Channel*/chan*.mat</t>
-  </si>
-  <si>
-    <t>Users/Kaleb/dataProcessed/Init_SetUp-160715-150111/Channel*/chan*.mat</t>
-  </si>
-  <si>
-    <t>Users/Kaleb/dataProcessed/Init_SetUp-160819-152223/Channel*/chan*.mat</t>
-  </si>
-  <si>
-    <t>Users/Kaleb/dataProcessed/Init_SetUp-160912-135839/Channel*/chan*.mat</t>
   </si>
   <si>
     <t>probeNo</t>
@@ -2454,16 +2442,16 @@
         <v>80</v>
       </c>
       <c r="AA1" s="6" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="AB1" s="6" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="AC1" s="6" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="AD1" s="6" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.2">
@@ -2555,10 +2543,10 @@
         <v>3</v>
       </c>
       <c r="AC2" s="1" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="AD2" s="1" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.2">
@@ -2650,7 +2638,7 @@
         <v>2</v>
       </c>
       <c r="AC3" s="1" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.2">
@@ -2742,10 +2730,10 @@
         <v>3</v>
       </c>
       <c r="AC4" s="1" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="AD4" s="1" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.2">
@@ -2837,7 +2825,7 @@
         <v>4</v>
       </c>
       <c r="AC5" s="1" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.2">
@@ -2929,7 +2917,7 @@
         <v>4</v>
       </c>
       <c r="AC6" s="1" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.2">
@@ -3021,7 +3009,7 @@
         <v>4</v>
       </c>
       <c r="AC7" s="1" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.2">
@@ -3113,7 +3101,7 @@
         <v>3</v>
       </c>
       <c r="AC8" s="1" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.2">
@@ -3205,7 +3193,7 @@
         <v>2</v>
       </c>
       <c r="AC9" s="1" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.2">
@@ -3297,7 +3285,7 @@
         <v>4</v>
       </c>
       <c r="AC10" s="1" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.2">
@@ -3389,7 +3377,7 @@
         <v>2</v>
       </c>
       <c r="AC11" s="1" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.2">
@@ -3481,7 +3469,7 @@
         <v>2</v>
       </c>
       <c r="AC12" s="1" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.2">
@@ -3573,7 +3561,7 @@
         <v>1</v>
       </c>
       <c r="AC13" s="1" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.2">
@@ -3665,7 +3653,7 @@
         <v>3</v>
       </c>
       <c r="AC14" s="1" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.2">
@@ -3757,7 +3745,7 @@
         <v>3</v>
       </c>
       <c r="AC15" s="1" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.2">
@@ -3849,7 +3837,7 @@
         <v>4</v>
       </c>
       <c r="AC16" s="1" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
     </row>
     <row r="17" spans="1:30" x14ac:dyDescent="0.2">
@@ -3941,7 +3929,7 @@
         <v>3</v>
       </c>
       <c r="AC17" s="1" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="AD17"/>
     </row>
@@ -4034,7 +4022,7 @@
         <v>3</v>
       </c>
       <c r="AC18" s="1" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="AD18"/>
     </row>
@@ -4127,7 +4115,7 @@
         <v>4</v>
       </c>
       <c r="AC19" s="1" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="AD19"/>
     </row>
@@ -4220,7 +4208,7 @@
         <v>4</v>
       </c>
       <c r="AC20" s="1" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="AD20"/>
     </row>
@@ -4313,7 +4301,7 @@
         <v>4</v>
       </c>
       <c r="AC21" s="1" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="AD21"/>
     </row>
@@ -4406,7 +4394,7 @@
         <v>4</v>
       </c>
       <c r="AC22" s="1" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="AD22"/>
     </row>
@@ -4430,7 +4418,7 @@
   </sheetPr>
   <dimension ref="A1:AF24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AD19" sqref="AD19"/>
     </sheetView>
   </sheetViews>
@@ -4549,19 +4537,19 @@
         <v>120</v>
       </c>
       <c r="AB1" s="6" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="AC1" s="6" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="AD1" s="6" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="AE1" s="6" t="s">
+        <v>427</v>
+      </c>
+      <c r="AF1" s="6" t="s">
         <v>431</v>
-      </c>
-      <c r="AF1" s="6" t="s">
-        <v>435</v>
       </c>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.2">
@@ -4655,7 +4643,7 @@
         <v>2</v>
       </c>
       <c r="AD2" s="7" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.2">
@@ -4749,7 +4737,7 @@
         <v>1</v>
       </c>
       <c r="AD3" s="1" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.2">
@@ -4843,7 +4831,7 @@
         <v>2</v>
       </c>
       <c r="AD4" s="1" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.2">
@@ -4937,7 +4925,7 @@
         <v>4</v>
       </c>
       <c r="AD5" s="1" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.2">
@@ -5031,7 +5019,7 @@
         <v>3</v>
       </c>
       <c r="AD6" s="1" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.2">
@@ -5125,7 +5113,7 @@
         <v>2</v>
       </c>
       <c r="AD7" s="1" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.2">
@@ -5219,7 +5207,7 @@
         <v>3</v>
       </c>
       <c r="AD8" s="1" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.2">
@@ -5313,7 +5301,7 @@
         <v>2</v>
       </c>
       <c r="AD9" s="1" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.2">
@@ -5407,10 +5395,10 @@
         <v>3</v>
       </c>
       <c r="AD10" s="1" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="AE10" s="1" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.2">
@@ -5504,7 +5492,7 @@
         <v>2</v>
       </c>
       <c r="AD11" s="1" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.2">
@@ -5598,7 +5586,7 @@
         <v>3</v>
       </c>
       <c r="AD12" s="1" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.2">
@@ -5692,7 +5680,7 @@
         <v>4</v>
       </c>
       <c r="AD13" s="1" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.2">
@@ -5786,7 +5774,7 @@
         <v>3</v>
       </c>
       <c r="AD14" s="1" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.2">
@@ -5880,7 +5868,7 @@
         <v>4</v>
       </c>
       <c r="AD15" s="1" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.2">
@@ -5974,7 +5962,7 @@
         <v>2</v>
       </c>
       <c r="AD16" s="1" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.2">
@@ -6068,7 +6056,7 @@
         <v>1</v>
       </c>
       <c r="AD17" s="1" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="AE17"/>
     </row>
@@ -6163,7 +6151,7 @@
         <v>3</v>
       </c>
       <c r="AD18" s="1" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="AE18"/>
     </row>
@@ -6258,7 +6246,7 @@
         <v>3</v>
       </c>
       <c r="AD19" s="1" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="AE19"/>
     </row>
@@ -6353,7 +6341,7 @@
         <v>1</v>
       </c>
       <c r="AD20" s="1" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="AE20"/>
     </row>
@@ -6501,13 +6489,13 @@
         <v>80</v>
       </c>
       <c r="AA1" s="6" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="AB1" s="6" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="AC1" s="6" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.2">
@@ -6599,7 +6587,7 @@
         <v>4</v>
       </c>
       <c r="AC2" s="1" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.2">
@@ -6691,7 +6679,7 @@
         <v>4</v>
       </c>
       <c r="AC3" s="1" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.2">
@@ -6783,7 +6771,7 @@
         <v>4</v>
       </c>
       <c r="AC4" s="1" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.2">
@@ -6875,7 +6863,7 @@
         <v>2</v>
       </c>
       <c r="AC5" s="1" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.2">
@@ -6967,7 +6955,7 @@
         <v>4</v>
       </c>
       <c r="AC6" s="1" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.2">
@@ -7059,7 +7047,7 @@
         <v>4</v>
       </c>
       <c r="AC7" s="1" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.2">
@@ -7151,7 +7139,7 @@
         <v>2</v>
       </c>
       <c r="AC8" s="1" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.2">
@@ -7243,7 +7231,7 @@
         <v>4</v>
       </c>
       <c r="AC9" s="1" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.2">
@@ -7335,7 +7323,7 @@
         <v>4</v>
       </c>
       <c r="AC10" s="1" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.2">
@@ -7427,7 +7415,7 @@
         <v>4</v>
       </c>
       <c r="AC11" s="7" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.2">
@@ -7519,7 +7507,7 @@
         <v>4</v>
       </c>
       <c r="AC12" s="7" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.2">
@@ -7611,7 +7599,7 @@
         <v>4</v>
       </c>
       <c r="AC13" s="7" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.2">
@@ -9155,8 +9143,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE53"/>
   <sheetViews>
-    <sheetView topLeftCell="W1" workbookViewId="0">
-      <selection activeCell="I44" sqref="I44"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9208,7 +9196,7 @@
         <v>93</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="K1" s="6" t="s">
         <v>92</v>
@@ -9265,13 +9253,13 @@
         <v>80</v>
       </c>
       <c r="AC1" s="6" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="AD1" s="6" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="AE1" s="6" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.2">
@@ -9300,7 +9288,7 @@
         <v>15</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="J2" s="7">
         <v>1</v>
@@ -9367,7 +9355,7 @@
         <v>4</v>
       </c>
       <c r="AE2" s="1" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.2">
@@ -9396,7 +9384,7 @@
         <v>16</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="J3" s="7">
         <v>1</v>
@@ -9463,7 +9451,7 @@
         <v>4</v>
       </c>
       <c r="AE3" s="1" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.2">
@@ -9492,7 +9480,7 @@
         <v>17</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="J4" s="7">
         <v>1</v>
@@ -9579,7 +9567,7 @@
         <v>18</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="J5" s="7">
         <v>1</v>
@@ -9646,7 +9634,7 @@
         <v>4</v>
       </c>
       <c r="AE5" s="1" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.2">
@@ -9675,7 +9663,7 @@
         <v>19</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="J6" s="7">
         <v>1</v>
@@ -9742,7 +9730,7 @@
         <v>4</v>
       </c>
       <c r="AE6" s="1" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.2">
@@ -9771,7 +9759,7 @@
         <v>20</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="J7" s="7">
         <v>1</v>
@@ -9838,7 +9826,7 @@
         <v>4</v>
       </c>
       <c r="AE7" s="1" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.2">
@@ -9867,7 +9855,7 @@
         <v>21</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="J8" s="7">
         <v>1</v>
@@ -9934,7 +9922,7 @@
         <v>4</v>
       </c>
       <c r="AE8" s="1" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.2">
@@ -9963,7 +9951,7 @@
         <v>23</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="J9" s="7">
         <v>1</v>
@@ -10030,7 +10018,7 @@
         <v>4</v>
       </c>
       <c r="AE9" s="1" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.2">
@@ -10059,7 +10047,7 @@
         <v>24</v>
       </c>
       <c r="I10" s="47" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="J10" s="47">
         <v>1</v>
@@ -10146,7 +10134,7 @@
         <v>25</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="J11" s="7">
         <v>1</v>
@@ -10213,7 +10201,7 @@
         <v>4</v>
       </c>
       <c r="AE11" s="1" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.2">
@@ -10242,7 +10230,7 @@
         <v>26</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="J12" s="7">
         <v>1</v>
@@ -10309,7 +10297,7 @@
         <v>4</v>
       </c>
       <c r="AE12" s="1" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.2">
@@ -10338,7 +10326,7 @@
         <v>27</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="J13" s="7">
         <v>1</v>
@@ -10405,7 +10393,7 @@
         <v>4</v>
       </c>
       <c r="AE13" s="1" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.2">
@@ -10434,7 +10422,7 @@
         <v>27</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="J14" s="7">
         <v>2</v>
@@ -10521,7 +10509,7 @@
         <v>28</v>
       </c>
       <c r="I15" s="41" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="J15" s="41">
         <v>1</v>
@@ -10608,7 +10596,7 @@
         <v>28</v>
       </c>
       <c r="I16" s="41" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="J16" s="41">
         <v>2</v>
@@ -10695,7 +10683,7 @@
         <v>29</v>
       </c>
       <c r="I17" s="47" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="J17" s="47">
         <v>1</v>
@@ -10762,7 +10750,7 @@
         <v>4</v>
       </c>
       <c r="AE17" s="1" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.2">
@@ -10791,7 +10779,7 @@
         <v>29</v>
       </c>
       <c r="I18" s="47" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="J18" s="47">
         <v>2</v>
@@ -10858,7 +10846,7 @@
         <v>4</v>
       </c>
       <c r="AE18" s="1" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.2">
@@ -10887,7 +10875,7 @@
         <v>31</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="J19" s="7">
         <v>1</v>
@@ -10954,7 +10942,7 @@
         <v>4</v>
       </c>
       <c r="AE19" s="1" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.2">
@@ -10983,7 +10971,7 @@
         <v>31</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="J20" s="7">
         <v>2</v>
@@ -11050,7 +11038,7 @@
         <v>4</v>
       </c>
       <c r="AE20" s="1" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.2">
@@ -11079,7 +11067,7 @@
         <v>32</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="J21" s="7">
         <v>1</v>
@@ -11146,7 +11134,7 @@
         <v>4</v>
       </c>
       <c r="AE21" s="1" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="22" spans="1:31" x14ac:dyDescent="0.2">
@@ -11175,7 +11163,7 @@
         <v>32</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="J22" s="7">
         <v>2</v>
@@ -11242,7 +11230,7 @@
         <v>4</v>
       </c>
       <c r="AE22" s="1" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.2">
@@ -11271,7 +11259,7 @@
         <v>33</v>
       </c>
       <c r="I23" s="53" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="J23" s="53">
         <v>2</v>
@@ -11338,7 +11326,7 @@
         <v>4</v>
       </c>
       <c r="AE23" s="7" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
     </row>
     <row r="24" spans="1:31" x14ac:dyDescent="0.2">
@@ -11367,7 +11355,7 @@
         <v>34</v>
       </c>
       <c r="I24" s="7" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="J24" s="7">
         <v>2</v>
@@ -11434,7 +11422,7 @@
         <v>4</v>
       </c>
       <c r="AE24" s="7" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
     </row>
     <row r="31" spans="1:31" x14ac:dyDescent="0.2">
@@ -11513,443 +11501,6 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA5"/>
-  <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="8" max="8" width="38.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:27" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="N1" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="O1" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="P1" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="Q1" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="R1" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="S1" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="T1" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="U1" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="V1" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="W1" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="X1" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="Y1" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="Z1" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="AA1" s="6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="B2" s="25" t="s">
-        <v>110</v>
-      </c>
-      <c r="C2" s="27">
-        <v>134</v>
-      </c>
-      <c r="D2" s="11">
-        <v>42564</v>
-      </c>
-      <c r="E2" s="27">
-        <v>28</v>
-      </c>
-      <c r="F2" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="27" t="s">
-        <v>111</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>370</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>287</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="M2" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="N2" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="O2" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="P2" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q2" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="R2" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="S2" s="31">
-        <v>3</v>
-      </c>
-      <c r="T2" s="31">
-        <v>-2</v>
-      </c>
-      <c r="U2" s="35">
-        <v>17200</v>
-      </c>
-      <c r="V2" s="35">
-        <v>21000</v>
-      </c>
-      <c r="W2" s="36">
-        <f t="shared" ref="W2:W5" si="0">V2-U2</f>
-        <v>3800</v>
-      </c>
-      <c r="X2" s="27">
-        <v>150</v>
-      </c>
-      <c r="Y2" s="33" t="s">
-        <v>112</v>
-      </c>
-      <c r="Z2" s="7">
-        <v>1</v>
-      </c>
-      <c r="AA2" s="27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="B3" s="25" t="s">
-        <v>110</v>
-      </c>
-      <c r="C3" s="27">
-        <v>135</v>
-      </c>
-      <c r="D3" s="11">
-        <v>42566</v>
-      </c>
-      <c r="E3" s="27">
-        <v>28</v>
-      </c>
-      <c r="F3" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="27" t="s">
-        <v>111</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>371</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>288</v>
-      </c>
-      <c r="K3" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="L3" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="M3" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="N3" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="O3" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="P3" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q3" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="R3" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="S3" s="31">
-        <v>3</v>
-      </c>
-      <c r="T3" s="31">
-        <v>-1</v>
-      </c>
-      <c r="U3" s="35">
-        <v>17200</v>
-      </c>
-      <c r="V3" s="35">
-        <v>21500</v>
-      </c>
-      <c r="W3" s="36">
-        <f t="shared" si="0"/>
-        <v>4300</v>
-      </c>
-      <c r="X3" s="27">
-        <v>150</v>
-      </c>
-      <c r="Y3" s="33" t="s">
-        <v>112</v>
-      </c>
-      <c r="Z3" s="7">
-        <v>1</v>
-      </c>
-      <c r="AA3" s="27">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="B4" s="25" t="s">
-        <v>110</v>
-      </c>
-      <c r="C4" s="27">
-        <v>139</v>
-      </c>
-      <c r="D4" s="11">
-        <v>42601</v>
-      </c>
-      <c r="E4" s="27">
-        <v>28</v>
-      </c>
-      <c r="F4" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="27" t="s">
-        <v>111</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>372</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>294</v>
-      </c>
-      <c r="K4" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="L4" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="M4" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="N4" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="O4" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="P4" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q4" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="R4" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="S4" s="31">
-        <v>4</v>
-      </c>
-      <c r="T4" s="31">
-        <v>-1</v>
-      </c>
-      <c r="U4" s="35">
-        <v>18000</v>
-      </c>
-      <c r="V4" s="35">
-        <v>23800</v>
-      </c>
-      <c r="W4" s="36">
-        <f t="shared" si="0"/>
-        <v>5800</v>
-      </c>
-      <c r="X4" s="27">
-        <v>150</v>
-      </c>
-      <c r="Y4" s="33" t="s">
-        <v>112</v>
-      </c>
-      <c r="Z4" s="7">
-        <v>1</v>
-      </c>
-      <c r="AA4" s="27">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="B5" s="25" t="s">
-        <v>110</v>
-      </c>
-      <c r="C5" s="27">
-        <v>140</v>
-      </c>
-      <c r="D5" s="11">
-        <v>42625</v>
-      </c>
-      <c r="E5" s="27">
-        <v>28</v>
-      </c>
-      <c r="F5" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="27" t="s">
-        <v>111</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>373</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>298</v>
-      </c>
-      <c r="K5" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="L5" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="M5" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="N5" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="O5" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="P5" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q5" s="27" t="s">
-        <v>4</v>
-      </c>
-      <c r="R5" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="S5" s="31">
-        <v>2</v>
-      </c>
-      <c r="T5" s="31">
-        <v>2</v>
-      </c>
-      <c r="U5" s="35">
-        <v>18000</v>
-      </c>
-      <c r="V5" s="35">
-        <v>25500</v>
-      </c>
-      <c r="W5" s="36">
-        <f t="shared" si="0"/>
-        <v>7500</v>
-      </c>
-      <c r="X5" s="27">
-        <v>150</v>
-      </c>
-      <c r="Y5" s="33" t="s">
-        <v>112</v>
-      </c>
-      <c r="Z5" s="7">
-        <v>1</v>
-      </c>
-      <c r="AA5" s="27">
-        <v>14</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
@@ -12071,19 +11622,19 @@
         <v>96</v>
       </c>
       <c r="AA1" s="6" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="AB1" s="6" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="AC1" s="6" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="AD1" s="6" t="s">
+        <v>427</v>
+      </c>
+      <c r="AE1" s="4" t="s">
         <v>431</v>
-      </c>
-      <c r="AE1" s="4" t="s">
-        <v>435</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="17" x14ac:dyDescent="0.2">
@@ -12175,7 +11726,7 @@
         <v>2</v>
       </c>
       <c r="AC2" s="1" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
     </row>
     <row r="3" spans="1:31" ht="17" x14ac:dyDescent="0.2">
@@ -12267,7 +11818,7 @@
         <v>1</v>
       </c>
       <c r="AC3" s="1" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
     </row>
     <row r="4" spans="1:31" ht="17" x14ac:dyDescent="0.2">
@@ -12359,7 +11910,7 @@
         <v>2</v>
       </c>
       <c r="AC4" s="1" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
     </row>
     <row r="5" spans="1:31" ht="17" x14ac:dyDescent="0.2">
@@ -12451,7 +12002,7 @@
         <v>1</v>
       </c>
       <c r="AC5" s="1" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
     </row>
     <row r="6" spans="1:31" ht="17" x14ac:dyDescent="0.2">
@@ -12543,7 +12094,7 @@
         <v>2</v>
       </c>
       <c r="AC6" s="1" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
     </row>
     <row r="7" spans="1:31" ht="17" x14ac:dyDescent="0.2">
@@ -12635,7 +12186,7 @@
         <v>3</v>
       </c>
       <c r="AC7" s="1" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
     </row>
     <row r="8" spans="1:31" ht="17" x14ac:dyDescent="0.2">
@@ -12727,7 +12278,7 @@
         <v>2</v>
       </c>
       <c r="AC8" s="1" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
     </row>
     <row r="9" spans="1:31" ht="17" x14ac:dyDescent="0.2">
@@ -12819,10 +12370,10 @@
         <v>3</v>
       </c>
       <c r="AC9" s="1" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="AE9" s="19" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
     </row>
     <row r="10" spans="1:31" ht="17" x14ac:dyDescent="0.2">
@@ -12914,7 +12465,7 @@
         <v>3</v>
       </c>
       <c r="AC10" s="1" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
     </row>
     <row r="11" spans="1:31" ht="17" x14ac:dyDescent="0.2">
@@ -13006,7 +12557,7 @@
         <v>3</v>
       </c>
       <c r="AC11" s="1" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
     </row>
     <row r="12" spans="1:31" ht="17" x14ac:dyDescent="0.2">
@@ -13098,7 +12649,7 @@
         <v>1</v>
       </c>
       <c r="AC12" s="1" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
     </row>
     <row r="13" spans="1:31" ht="17" x14ac:dyDescent="0.2">
@@ -13190,7 +12741,7 @@
         <v>1</v>
       </c>
       <c r="AC13" s="1" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
     </row>
     <row r="14" spans="1:31" ht="17" x14ac:dyDescent="0.2">
@@ -13282,10 +12833,10 @@
         <v>2</v>
       </c>
       <c r="AC14" s="1" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="AD14" s="1" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.2">
@@ -13403,7 +12954,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
@@ -13516,19 +13067,19 @@
         <v>96</v>
       </c>
       <c r="AA1" s="6" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="AB1" s="6" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="AC1" s="6" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="AD1" s="6" t="s">
+        <v>427</v>
+      </c>
+      <c r="AE1" s="6" t="s">
         <v>431</v>
-      </c>
-      <c r="AE1" s="6" t="s">
-        <v>435</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="17" x14ac:dyDescent="0.2">
@@ -13620,7 +13171,7 @@
         <v>2</v>
       </c>
       <c r="AC2" s="1" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
     </row>
     <row r="3" spans="1:31" ht="17" x14ac:dyDescent="0.2">
@@ -13712,7 +13263,7 @@
         <v>2</v>
       </c>
       <c r="AC3" s="1" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
     </row>
     <row r="4" spans="1:31" ht="17" x14ac:dyDescent="0.2">
@@ -13804,7 +13355,7 @@
         <v>1</v>
       </c>
       <c r="AC4" s="1" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
     </row>
     <row r="5" spans="1:31" ht="17" x14ac:dyDescent="0.2">
@@ -13896,7 +13447,7 @@
         <v>1</v>
       </c>
       <c r="AC5" s="1" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
     </row>
     <row r="6" spans="1:31" ht="17" x14ac:dyDescent="0.2">
@@ -13988,7 +13539,7 @@
         <v>2</v>
       </c>
       <c r="AC6" s="1" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
     </row>
     <row r="7" spans="1:31" ht="17" x14ac:dyDescent="0.2">
@@ -14080,7 +13631,7 @@
         <v>1</v>
       </c>
       <c r="AC7" s="1" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
     </row>
     <row r="8" spans="1:31" ht="17" x14ac:dyDescent="0.2">
@@ -14172,7 +13723,7 @@
         <v>1</v>
       </c>
       <c r="AC8" s="1" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
     </row>
     <row r="9" spans="1:31" ht="17" x14ac:dyDescent="0.2">
@@ -14264,7 +13815,7 @@
         <v>2</v>
       </c>
       <c r="AC9" s="1" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
     </row>
     <row r="10" spans="1:31" ht="17" x14ac:dyDescent="0.2">
@@ -14356,13 +13907,13 @@
         <v>2</v>
       </c>
       <c r="AC10" s="1" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="AD10" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="AE10" s="19" t="s">
         <v>433</v>
-      </c>
-      <c r="AE10" s="19" t="s">
-        <v>437</v>
       </c>
     </row>
     <row r="11" spans="1:31" ht="17" x14ac:dyDescent="0.2">
@@ -14454,7 +14005,7 @@
         <v>3</v>
       </c>
       <c r="AC11" s="1" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
     </row>
     <row r="12" spans="1:31" ht="17" x14ac:dyDescent="0.2">
@@ -14546,7 +14097,7 @@
         <v>3</v>
       </c>
       <c r="AC12" s="1" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
     </row>
     <row r="13" spans="1:31" ht="17" x14ac:dyDescent="0.2">
@@ -14638,7 +14189,7 @@
         <v>3</v>
       </c>
       <c r="AC13" s="1" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
     </row>
     <row r="14" spans="1:31" ht="17" x14ac:dyDescent="0.2">
@@ -14941,4 +14492,400 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="51" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AE4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G42" sqref="G42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="8" max="8" width="38.5" customWidth="1"/>
+    <col min="9" max="9" width="45.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:31" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>370</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q1" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="R1" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="S1" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="T1" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="U1" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="V1" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="W1" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="X1" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="Y1" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="Z1" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="AA1" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="AB1" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="AC1" s="6" t="s">
+        <v>371</v>
+      </c>
+      <c r="AD1" s="6" t="s">
+        <v>372</v>
+      </c>
+      <c r="AE1" s="6" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2" s="27">
+        <v>134</v>
+      </c>
+      <c r="D2" s="11">
+        <v>42562</v>
+      </c>
+      <c r="E2" s="27">
+        <v>28</v>
+      </c>
+      <c r="F2" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>409</v>
+      </c>
+      <c r="J2" s="7">
+        <v>1</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="O2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="P2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q2" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="R2" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="S2" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="T2" s="31">
+        <v>3</v>
+      </c>
+      <c r="U2" s="31">
+        <v>-2</v>
+      </c>
+      <c r="V2" s="35">
+        <v>17200</v>
+      </c>
+      <c r="W2" s="35">
+        <v>21000</v>
+      </c>
+      <c r="X2" s="36">
+        <f>W2-V2</f>
+        <v>3800</v>
+      </c>
+      <c r="Y2" s="27">
+        <v>150</v>
+      </c>
+      <c r="Z2" s="33" t="s">
+        <v>112</v>
+      </c>
+      <c r="AA2" s="7">
+        <v>1</v>
+      </c>
+      <c r="AB2" s="27">
+        <v>1</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD2" s="1">
+        <v>4</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="C3" s="27">
+        <v>134</v>
+      </c>
+      <c r="D3" s="11">
+        <v>42564</v>
+      </c>
+      <c r="E3" s="27">
+        <v>28</v>
+      </c>
+      <c r="F3" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>410</v>
+      </c>
+      <c r="J3" s="7">
+        <v>1</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>287</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="O3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="P3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q3" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="R3" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="S3" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="T3" s="31">
+        <v>3</v>
+      </c>
+      <c r="U3" s="31">
+        <v>-2</v>
+      </c>
+      <c r="V3" s="35">
+        <v>17200</v>
+      </c>
+      <c r="W3" s="35">
+        <v>21000</v>
+      </c>
+      <c r="X3" s="36">
+        <f t="shared" ref="X3:X4" si="0">W3-V3</f>
+        <v>3800</v>
+      </c>
+      <c r="Y3" s="27">
+        <v>150</v>
+      </c>
+      <c r="Z3" s="33" t="s">
+        <v>112</v>
+      </c>
+      <c r="AA3" s="7">
+        <v>1</v>
+      </c>
+      <c r="AB3" s="27">
+        <v>1</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD3" s="1">
+        <v>4</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="C4" s="27">
+        <v>135</v>
+      </c>
+      <c r="D4" s="11">
+        <v>42566</v>
+      </c>
+      <c r="E4" s="27">
+        <v>28</v>
+      </c>
+      <c r="F4" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>411</v>
+      </c>
+      <c r="J4" s="7">
+        <v>1</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>288</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="N4" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="O4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="P4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q4" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="R4" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="S4" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="T4" s="31">
+        <v>3</v>
+      </c>
+      <c r="U4" s="31">
+        <v>-1</v>
+      </c>
+      <c r="V4" s="35">
+        <v>17200</v>
+      </c>
+      <c r="W4" s="35">
+        <v>21500</v>
+      </c>
+      <c r="X4" s="36">
+        <f t="shared" si="0"/>
+        <v>4300</v>
+      </c>
+      <c r="Y4" s="27">
+        <v>150</v>
+      </c>
+      <c r="Z4" s="33" t="s">
+        <v>112</v>
+      </c>
+      <c r="AA4" s="7">
+        <v>1</v>
+      </c>
+      <c r="AB4" s="27">
+        <v>2</v>
+      </c>
+      <c r="AC4" s="1"/>
+      <c r="AD4" s="1"/>
+      <c r="AE4" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated files to process for TaskType by location.  dist calculation is separated out.
</commit_message>
<xml_diff>
--- a/config/SFN_NHP_Coordinates_All.xlsx
+++ b/config/SFN_NHP_Coordinates_All.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4240" yWindow="460" windowWidth="30860" windowHeight="19440" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="4240" yWindow="460" windowWidth="30860" windowHeight="19440" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Br" sheetId="2" r:id="rId1"/>
@@ -2334,8 +2334,8 @@
   </sheetPr>
   <dimension ref="A1:AD22"/>
   <sheetViews>
-    <sheetView topLeftCell="AA1" workbookViewId="0">
-      <selection activeCell="AD1" sqref="AD1:AD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6375,8 +6375,8 @@
   </sheetPr>
   <dimension ref="A1:AC88"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9143,8 +9143,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11507,8 +11507,8 @@
   </sheetPr>
   <dimension ref="A1:AE37"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="X9" sqref="X9"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12961,8 +12961,8 @@
   </sheetPr>
   <dimension ref="A1:AE1048576"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14498,14 +14498,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="8" max="8" width="38.5" customWidth="1"/>
-    <col min="9" max="9" width="45.1640625" customWidth="1"/>
+    <col min="9" max="9" width="79.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="17" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
reverted to working processSessions (attempt1)
</commit_message>
<xml_diff>
--- a/config/SFN_NHP_Coordinates_All.xlsx
+++ b/config/SFN_NHP_Coordinates_All.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27011"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elseyjg/temp/schalllab-spatial/config/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/subravcr/Projects/lab-schall/schalllab-spatial/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4240" yWindow="460" windowWidth="30860" windowHeight="19440" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="4240" yWindow="460" windowWidth="30860" windowHeight="19440" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Br" sheetId="2" r:id="rId1"/>
     <sheet name="Jo" sheetId="1" r:id="rId2"/>
     <sheet name="Da_WJ" sheetId="6" r:id="rId3"/>
     <sheet name="Da_K" sheetId="7" r:id="rId4"/>
-    <sheet name="TestDarwin" sheetId="8" r:id="rId5"/>
-    <sheet name="Ga" sheetId="4" r:id="rId6"/>
-    <sheet name="He" sheetId="5" r:id="rId7"/>
+    <sheet name="Ga" sheetId="4" r:id="rId5"/>
+    <sheet name="He" sheetId="5" r:id="rId6"/>
+    <sheet name="Test" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1890" uniqueCount="439">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1882" uniqueCount="435">
   <si>
     <t>a3</t>
   </si>
@@ -1143,18 +1143,6 @@
   </si>
   <si>
     <t>Users/Wolf/ephys_db/Helmholtz/2015-03-12a/DSP/DSP*/*MG*.mat</t>
-  </si>
-  <si>
-    <t>Users/Kaleb/dataProcessed/Init_SetUp-160713-144841/Channel*/chan*.mat</t>
-  </si>
-  <si>
-    <t>Users/Kaleb/dataProcessed/Init_SetUp-160715-150111/Channel*/chan*.mat</t>
-  </si>
-  <si>
-    <t>Users/Kaleb/dataProcessed/Init_SetUp-160819-152223/Channel*/chan*.mat</t>
-  </si>
-  <si>
-    <t>Users/Kaleb/dataProcessed/Init_SetUp-160912-135839/Channel*/chan*.mat</t>
   </si>
   <si>
     <t>probeNo</t>
@@ -2346,8 +2334,8 @@
   </sheetPr>
   <dimension ref="A1:AD22"/>
   <sheetViews>
-    <sheetView topLeftCell="AA1" workbookViewId="0">
-      <selection activeCell="AD1" sqref="AD1:AD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2454,16 +2442,16 @@
         <v>80</v>
       </c>
       <c r="AA1" s="6" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="AB1" s="6" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="AC1" s="6" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="AD1" s="6" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.2">
@@ -2555,10 +2543,10 @@
         <v>3</v>
       </c>
       <c r="AC2" s="1" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="AD2" s="1" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.2">
@@ -2650,7 +2638,7 @@
         <v>2</v>
       </c>
       <c r="AC3" s="1" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.2">
@@ -2742,10 +2730,10 @@
         <v>3</v>
       </c>
       <c r="AC4" s="1" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="AD4" s="1" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.2">
@@ -2837,7 +2825,7 @@
         <v>4</v>
       </c>
       <c r="AC5" s="1" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.2">
@@ -2929,7 +2917,7 @@
         <v>4</v>
       </c>
       <c r="AC6" s="1" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.2">
@@ -3021,7 +3009,7 @@
         <v>4</v>
       </c>
       <c r="AC7" s="1" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.2">
@@ -3113,7 +3101,7 @@
         <v>3</v>
       </c>
       <c r="AC8" s="1" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.2">
@@ -3205,7 +3193,7 @@
         <v>2</v>
       </c>
       <c r="AC9" s="1" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.2">
@@ -3297,7 +3285,7 @@
         <v>4</v>
       </c>
       <c r="AC10" s="1" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.2">
@@ -3389,7 +3377,7 @@
         <v>2</v>
       </c>
       <c r="AC11" s="1" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.2">
@@ -3481,7 +3469,7 @@
         <v>2</v>
       </c>
       <c r="AC12" s="1" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.2">
@@ -3573,7 +3561,7 @@
         <v>1</v>
       </c>
       <c r="AC13" s="1" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.2">
@@ -3665,7 +3653,7 @@
         <v>3</v>
       </c>
       <c r="AC14" s="1" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.2">
@@ -3757,7 +3745,7 @@
         <v>3</v>
       </c>
       <c r="AC15" s="1" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.2">
@@ -3849,7 +3837,7 @@
         <v>4</v>
       </c>
       <c r="AC16" s="1" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
     </row>
     <row r="17" spans="1:30" x14ac:dyDescent="0.2">
@@ -3941,7 +3929,7 @@
         <v>3</v>
       </c>
       <c r="AC17" s="1" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="AD17"/>
     </row>
@@ -4034,7 +4022,7 @@
         <v>3</v>
       </c>
       <c r="AC18" s="1" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="AD18"/>
     </row>
@@ -4127,7 +4115,7 @@
         <v>4</v>
       </c>
       <c r="AC19" s="1" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="AD19"/>
     </row>
@@ -4220,7 +4208,7 @@
         <v>4</v>
       </c>
       <c r="AC20" s="1" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="AD20"/>
     </row>
@@ -4313,7 +4301,7 @@
         <v>4</v>
       </c>
       <c r="AC21" s="1" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="AD21"/>
     </row>
@@ -4406,7 +4394,7 @@
         <v>4</v>
       </c>
       <c r="AC22" s="1" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="AD22"/>
     </row>
@@ -4430,7 +4418,7 @@
   </sheetPr>
   <dimension ref="A1:AF24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AD19" sqref="AD19"/>
     </sheetView>
   </sheetViews>
@@ -4549,19 +4537,19 @@
         <v>120</v>
       </c>
       <c r="AB1" s="6" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="AC1" s="6" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="AD1" s="6" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="AE1" s="6" t="s">
+        <v>427</v>
+      </c>
+      <c r="AF1" s="6" t="s">
         <v>431</v>
-      </c>
-      <c r="AF1" s="6" t="s">
-        <v>435</v>
       </c>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.2">
@@ -4655,7 +4643,7 @@
         <v>2</v>
       </c>
       <c r="AD2" s="7" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.2">
@@ -4749,7 +4737,7 @@
         <v>1</v>
       </c>
       <c r="AD3" s="1" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.2">
@@ -4843,7 +4831,7 @@
         <v>2</v>
       </c>
       <c r="AD4" s="1" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.2">
@@ -4937,7 +4925,7 @@
         <v>4</v>
       </c>
       <c r="AD5" s="1" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.2">
@@ -5031,7 +5019,7 @@
         <v>3</v>
       </c>
       <c r="AD6" s="1" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.2">
@@ -5125,7 +5113,7 @@
         <v>2</v>
       </c>
       <c r="AD7" s="1" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.2">
@@ -5219,7 +5207,7 @@
         <v>3</v>
       </c>
       <c r="AD8" s="1" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.2">
@@ -5313,7 +5301,7 @@
         <v>2</v>
       </c>
       <c r="AD9" s="1" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.2">
@@ -5407,10 +5395,10 @@
         <v>3</v>
       </c>
       <c r="AD10" s="1" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="AE10" s="1" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.2">
@@ -5504,7 +5492,7 @@
         <v>2</v>
       </c>
       <c r="AD11" s="1" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.2">
@@ -5598,7 +5586,7 @@
         <v>3</v>
       </c>
       <c r="AD12" s="1" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.2">
@@ -5692,7 +5680,7 @@
         <v>4</v>
       </c>
       <c r="AD13" s="1" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.2">
@@ -5786,7 +5774,7 @@
         <v>3</v>
       </c>
       <c r="AD14" s="1" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.2">
@@ -5880,7 +5868,7 @@
         <v>4</v>
       </c>
       <c r="AD15" s="1" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.2">
@@ -5974,7 +5962,7 @@
         <v>2</v>
       </c>
       <c r="AD16" s="1" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.2">
@@ -6068,7 +6056,7 @@
         <v>1</v>
       </c>
       <c r="AD17" s="1" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="AE17"/>
     </row>
@@ -6163,7 +6151,7 @@
         <v>3</v>
       </c>
       <c r="AD18" s="1" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="AE18"/>
     </row>
@@ -6258,7 +6246,7 @@
         <v>3</v>
       </c>
       <c r="AD19" s="1" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="AE19"/>
     </row>
@@ -6353,7 +6341,7 @@
         <v>1</v>
       </c>
       <c r="AD20" s="1" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="AE20"/>
     </row>
@@ -6387,8 +6375,8 @@
   </sheetPr>
   <dimension ref="A1:AC88"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6501,13 +6489,13 @@
         <v>80</v>
       </c>
       <c r="AA1" s="6" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="AB1" s="6" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="AC1" s="6" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.2">
@@ -6599,7 +6587,7 @@
         <v>4</v>
       </c>
       <c r="AC2" s="1" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.2">
@@ -6691,7 +6679,7 @@
         <v>4</v>
       </c>
       <c r="AC3" s="1" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.2">
@@ -6783,7 +6771,7 @@
         <v>4</v>
       </c>
       <c r="AC4" s="1" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.2">
@@ -6875,7 +6863,7 @@
         <v>2</v>
       </c>
       <c r="AC5" s="1" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.2">
@@ -6967,7 +6955,7 @@
         <v>4</v>
       </c>
       <c r="AC6" s="1" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.2">
@@ -7059,7 +7047,7 @@
         <v>4</v>
       </c>
       <c r="AC7" s="1" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.2">
@@ -7151,7 +7139,7 @@
         <v>2</v>
       </c>
       <c r="AC8" s="1" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.2">
@@ -7243,7 +7231,7 @@
         <v>4</v>
       </c>
       <c r="AC9" s="1" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.2">
@@ -7335,7 +7323,7 @@
         <v>4</v>
       </c>
       <c r="AC10" s="1" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.2">
@@ -7427,7 +7415,7 @@
         <v>4</v>
       </c>
       <c r="AC11" s="7" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.2">
@@ -7519,7 +7507,7 @@
         <v>4</v>
       </c>
       <c r="AC12" s="7" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.2">
@@ -7611,7 +7599,7 @@
         <v>4</v>
       </c>
       <c r="AC13" s="7" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.2">
@@ -9155,8 +9143,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE53"/>
   <sheetViews>
-    <sheetView topLeftCell="W1" workbookViewId="0">
-      <selection activeCell="I44" sqref="I44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9208,7 +9196,7 @@
         <v>93</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="K1" s="6" t="s">
         <v>92</v>
@@ -9265,13 +9253,13 @@
         <v>80</v>
       </c>
       <c r="AC1" s="6" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="AD1" s="6" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="AE1" s="6" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.2">
@@ -9300,7 +9288,7 @@
         <v>15</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="J2" s="7">
         <v>1</v>
@@ -9367,7 +9355,7 @@
         <v>4</v>
       </c>
       <c r="AE2" s="1" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.2">
@@ -9396,7 +9384,7 @@
         <v>16</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="J3" s="7">
         <v>1</v>
@@ -9463,7 +9451,7 @@
         <v>4</v>
       </c>
       <c r="AE3" s="1" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.2">
@@ -9492,7 +9480,7 @@
         <v>17</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="J4" s="7">
         <v>1</v>
@@ -9579,7 +9567,7 @@
         <v>18</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="J5" s="7">
         <v>1</v>
@@ -9646,7 +9634,7 @@
         <v>4</v>
       </c>
       <c r="AE5" s="1" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.2">
@@ -9675,7 +9663,7 @@
         <v>19</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="J6" s="7">
         <v>1</v>
@@ -9742,7 +9730,7 @@
         <v>4</v>
       </c>
       <c r="AE6" s="1" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.2">
@@ -9771,7 +9759,7 @@
         <v>20</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="J7" s="7">
         <v>1</v>
@@ -9838,7 +9826,7 @@
         <v>4</v>
       </c>
       <c r="AE7" s="1" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.2">
@@ -9867,7 +9855,7 @@
         <v>21</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="J8" s="7">
         <v>1</v>
@@ -9934,7 +9922,7 @@
         <v>4</v>
       </c>
       <c r="AE8" s="1" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.2">
@@ -9963,7 +9951,7 @@
         <v>23</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="J9" s="7">
         <v>1</v>
@@ -10030,7 +10018,7 @@
         <v>4</v>
       </c>
       <c r="AE9" s="1" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.2">
@@ -10059,7 +10047,7 @@
         <v>24</v>
       </c>
       <c r="I10" s="47" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="J10" s="47">
         <v>1</v>
@@ -10146,7 +10134,7 @@
         <v>25</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="J11" s="7">
         <v>1</v>
@@ -10213,7 +10201,7 @@
         <v>4</v>
       </c>
       <c r="AE11" s="1" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.2">
@@ -10242,7 +10230,7 @@
         <v>26</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="J12" s="7">
         <v>1</v>
@@ -10309,7 +10297,7 @@
         <v>4</v>
       </c>
       <c r="AE12" s="1" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.2">
@@ -10338,7 +10326,7 @@
         <v>27</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="J13" s="7">
         <v>1</v>
@@ -10405,7 +10393,7 @@
         <v>4</v>
       </c>
       <c r="AE13" s="1" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.2">
@@ -10434,7 +10422,7 @@
         <v>27</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="J14" s="7">
         <v>2</v>
@@ -10521,7 +10509,7 @@
         <v>28</v>
       </c>
       <c r="I15" s="41" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="J15" s="41">
         <v>1</v>
@@ -10608,7 +10596,7 @@
         <v>28</v>
       </c>
       <c r="I16" s="41" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="J16" s="41">
         <v>2</v>
@@ -10695,7 +10683,7 @@
         <v>29</v>
       </c>
       <c r="I17" s="47" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="J17" s="47">
         <v>1</v>
@@ -10762,7 +10750,7 @@
         <v>4</v>
       </c>
       <c r="AE17" s="1" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.2">
@@ -10791,7 +10779,7 @@
         <v>29</v>
       </c>
       <c r="I18" s="47" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="J18" s="47">
         <v>2</v>
@@ -10858,7 +10846,7 @@
         <v>4</v>
       </c>
       <c r="AE18" s="1" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.2">
@@ -10887,7 +10875,7 @@
         <v>31</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="J19" s="7">
         <v>1</v>
@@ -10954,7 +10942,7 @@
         <v>4</v>
       </c>
       <c r="AE19" s="1" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.2">
@@ -10983,7 +10971,7 @@
         <v>31</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="J20" s="7">
         <v>2</v>
@@ -11050,7 +11038,7 @@
         <v>4</v>
       </c>
       <c r="AE20" s="1" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.2">
@@ -11079,7 +11067,7 @@
         <v>32</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="J21" s="7">
         <v>1</v>
@@ -11146,7 +11134,7 @@
         <v>4</v>
       </c>
       <c r="AE21" s="1" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="22" spans="1:31" x14ac:dyDescent="0.2">
@@ -11175,7 +11163,7 @@
         <v>32</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="J22" s="7">
         <v>2</v>
@@ -11242,7 +11230,7 @@
         <v>4</v>
       </c>
       <c r="AE22" s="1" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.2">
@@ -11271,7 +11259,7 @@
         <v>33</v>
       </c>
       <c r="I23" s="53" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="J23" s="53">
         <v>2</v>
@@ -11338,7 +11326,7 @@
         <v>4</v>
       </c>
       <c r="AE23" s="7" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
     </row>
     <row r="24" spans="1:31" x14ac:dyDescent="0.2">
@@ -11367,7 +11355,7 @@
         <v>34</v>
       </c>
       <c r="I24" s="7" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="J24" s="7">
         <v>2</v>
@@ -11434,7 +11422,7 @@
         <v>4</v>
       </c>
       <c r="AE24" s="7" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
     </row>
     <row r="31" spans="1:31" x14ac:dyDescent="0.2">
@@ -11514,450 +11502,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA5"/>
-  <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="8" max="8" width="38.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:27" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="N1" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="O1" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="P1" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="Q1" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="R1" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="S1" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="T1" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="U1" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="V1" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="W1" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="X1" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="Y1" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="Z1" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="AA1" s="6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="B2" s="25" t="s">
-        <v>110</v>
-      </c>
-      <c r="C2" s="27">
-        <v>134</v>
-      </c>
-      <c r="D2" s="11">
-        <v>42564</v>
-      </c>
-      <c r="E2" s="27">
-        <v>28</v>
-      </c>
-      <c r="F2" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="27" t="s">
-        <v>111</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>370</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>287</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="M2" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="N2" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="O2" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="P2" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q2" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="R2" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="S2" s="31">
-        <v>3</v>
-      </c>
-      <c r="T2" s="31">
-        <v>-2</v>
-      </c>
-      <c r="U2" s="35">
-        <v>17200</v>
-      </c>
-      <c r="V2" s="35">
-        <v>21000</v>
-      </c>
-      <c r="W2" s="36">
-        <f t="shared" ref="W2:W5" si="0">V2-U2</f>
-        <v>3800</v>
-      </c>
-      <c r="X2" s="27">
-        <v>150</v>
-      </c>
-      <c r="Y2" s="33" t="s">
-        <v>112</v>
-      </c>
-      <c r="Z2" s="7">
-        <v>1</v>
-      </c>
-      <c r="AA2" s="27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="B3" s="25" t="s">
-        <v>110</v>
-      </c>
-      <c r="C3" s="27">
-        <v>135</v>
-      </c>
-      <c r="D3" s="11">
-        <v>42566</v>
-      </c>
-      <c r="E3" s="27">
-        <v>28</v>
-      </c>
-      <c r="F3" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="27" t="s">
-        <v>111</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>371</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>288</v>
-      </c>
-      <c r="K3" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="L3" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="M3" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="N3" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="O3" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="P3" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q3" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="R3" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="S3" s="31">
-        <v>3</v>
-      </c>
-      <c r="T3" s="31">
-        <v>-1</v>
-      </c>
-      <c r="U3" s="35">
-        <v>17200</v>
-      </c>
-      <c r="V3" s="35">
-        <v>21500</v>
-      </c>
-      <c r="W3" s="36">
-        <f t="shared" si="0"/>
-        <v>4300</v>
-      </c>
-      <c r="X3" s="27">
-        <v>150</v>
-      </c>
-      <c r="Y3" s="33" t="s">
-        <v>112</v>
-      </c>
-      <c r="Z3" s="7">
-        <v>1</v>
-      </c>
-      <c r="AA3" s="27">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="B4" s="25" t="s">
-        <v>110</v>
-      </c>
-      <c r="C4" s="27">
-        <v>139</v>
-      </c>
-      <c r="D4" s="11">
-        <v>42601</v>
-      </c>
-      <c r="E4" s="27">
-        <v>28</v>
-      </c>
-      <c r="F4" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="27" t="s">
-        <v>111</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>372</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>294</v>
-      </c>
-      <c r="K4" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="L4" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="M4" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="N4" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="O4" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="P4" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q4" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="R4" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="S4" s="31">
-        <v>4</v>
-      </c>
-      <c r="T4" s="31">
-        <v>-1</v>
-      </c>
-      <c r="U4" s="35">
-        <v>18000</v>
-      </c>
-      <c r="V4" s="35">
-        <v>23800</v>
-      </c>
-      <c r="W4" s="36">
-        <f t="shared" si="0"/>
-        <v>5800</v>
-      </c>
-      <c r="X4" s="27">
-        <v>150</v>
-      </c>
-      <c r="Y4" s="33" t="s">
-        <v>112</v>
-      </c>
-      <c r="Z4" s="7">
-        <v>1</v>
-      </c>
-      <c r="AA4" s="27">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="B5" s="25" t="s">
-        <v>110</v>
-      </c>
-      <c r="C5" s="27">
-        <v>140</v>
-      </c>
-      <c r="D5" s="11">
-        <v>42625</v>
-      </c>
-      <c r="E5" s="27">
-        <v>28</v>
-      </c>
-      <c r="F5" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="27" t="s">
-        <v>111</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>373</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>298</v>
-      </c>
-      <c r="K5" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="L5" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="M5" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="N5" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="O5" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="P5" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q5" s="27" t="s">
-        <v>4</v>
-      </c>
-      <c r="R5" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="S5" s="31">
-        <v>2</v>
-      </c>
-      <c r="T5" s="31">
-        <v>2</v>
-      </c>
-      <c r="U5" s="35">
-        <v>18000</v>
-      </c>
-      <c r="V5" s="35">
-        <v>25500</v>
-      </c>
-      <c r="W5" s="36">
-        <f t="shared" si="0"/>
-        <v>7500</v>
-      </c>
-      <c r="X5" s="27">
-        <v>150</v>
-      </c>
-      <c r="Y5" s="33" t="s">
-        <v>112</v>
-      </c>
-      <c r="Z5" s="7">
-        <v>1</v>
-      </c>
-      <c r="AA5" s="27">
-        <v>14</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AE37"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="X9" sqref="X9"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12071,19 +11622,19 @@
         <v>96</v>
       </c>
       <c r="AA1" s="6" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="AB1" s="6" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="AC1" s="6" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="AD1" s="6" t="s">
+        <v>427</v>
+      </c>
+      <c r="AE1" s="4" t="s">
         <v>431</v>
-      </c>
-      <c r="AE1" s="4" t="s">
-        <v>435</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="17" x14ac:dyDescent="0.2">
@@ -12175,7 +11726,7 @@
         <v>2</v>
       </c>
       <c r="AC2" s="1" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
     </row>
     <row r="3" spans="1:31" ht="17" x14ac:dyDescent="0.2">
@@ -12267,7 +11818,7 @@
         <v>1</v>
       </c>
       <c r="AC3" s="1" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
     </row>
     <row r="4" spans="1:31" ht="17" x14ac:dyDescent="0.2">
@@ -12359,7 +11910,7 @@
         <v>2</v>
       </c>
       <c r="AC4" s="1" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
     </row>
     <row r="5" spans="1:31" ht="17" x14ac:dyDescent="0.2">
@@ -12451,7 +12002,7 @@
         <v>1</v>
       </c>
       <c r="AC5" s="1" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
     </row>
     <row r="6" spans="1:31" ht="17" x14ac:dyDescent="0.2">
@@ -12543,7 +12094,7 @@
         <v>2</v>
       </c>
       <c r="AC6" s="1" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
     </row>
     <row r="7" spans="1:31" ht="17" x14ac:dyDescent="0.2">
@@ -12635,7 +12186,7 @@
         <v>3</v>
       </c>
       <c r="AC7" s="1" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
     </row>
     <row r="8" spans="1:31" ht="17" x14ac:dyDescent="0.2">
@@ -12727,7 +12278,7 @@
         <v>2</v>
       </c>
       <c r="AC8" s="1" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
     </row>
     <row r="9" spans="1:31" ht="17" x14ac:dyDescent="0.2">
@@ -12819,10 +12370,10 @@
         <v>3</v>
       </c>
       <c r="AC9" s="1" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="AE9" s="19" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
     </row>
     <row r="10" spans="1:31" ht="17" x14ac:dyDescent="0.2">
@@ -12914,7 +12465,7 @@
         <v>3</v>
       </c>
       <c r="AC10" s="1" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
     </row>
     <row r="11" spans="1:31" ht="17" x14ac:dyDescent="0.2">
@@ -13006,7 +12557,7 @@
         <v>3</v>
       </c>
       <c r="AC11" s="1" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
     </row>
     <row r="12" spans="1:31" ht="17" x14ac:dyDescent="0.2">
@@ -13098,7 +12649,7 @@
         <v>1</v>
       </c>
       <c r="AC12" s="1" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
     </row>
     <row r="13" spans="1:31" ht="17" x14ac:dyDescent="0.2">
@@ -13190,7 +12741,7 @@
         <v>1</v>
       </c>
       <c r="AC13" s="1" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
     </row>
     <row r="14" spans="1:31" ht="17" x14ac:dyDescent="0.2">
@@ -13282,10 +12833,10 @@
         <v>2</v>
       </c>
       <c r="AC14" s="1" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="AD14" s="1" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.2">
@@ -13403,15 +12954,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AE1048576"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13516,19 +13067,19 @@
         <v>96</v>
       </c>
       <c r="AA1" s="6" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="AB1" s="6" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="AC1" s="6" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="AD1" s="6" t="s">
+        <v>427</v>
+      </c>
+      <c r="AE1" s="6" t="s">
         <v>431</v>
-      </c>
-      <c r="AE1" s="6" t="s">
-        <v>435</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="17" x14ac:dyDescent="0.2">
@@ -13620,7 +13171,7 @@
         <v>2</v>
       </c>
       <c r="AC2" s="1" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
     </row>
     <row r="3" spans="1:31" ht="17" x14ac:dyDescent="0.2">
@@ -13712,7 +13263,7 @@
         <v>2</v>
       </c>
       <c r="AC3" s="1" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
     </row>
     <row r="4" spans="1:31" ht="17" x14ac:dyDescent="0.2">
@@ -13804,7 +13355,7 @@
         <v>1</v>
       </c>
       <c r="AC4" s="1" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
     </row>
     <row r="5" spans="1:31" ht="17" x14ac:dyDescent="0.2">
@@ -13896,7 +13447,7 @@
         <v>1</v>
       </c>
       <c r="AC5" s="1" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
     </row>
     <row r="6" spans="1:31" ht="17" x14ac:dyDescent="0.2">
@@ -13988,7 +13539,7 @@
         <v>2</v>
       </c>
       <c r="AC6" s="1" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
     </row>
     <row r="7" spans="1:31" ht="17" x14ac:dyDescent="0.2">
@@ -14080,7 +13631,7 @@
         <v>1</v>
       </c>
       <c r="AC7" s="1" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
     </row>
     <row r="8" spans="1:31" ht="17" x14ac:dyDescent="0.2">
@@ -14172,7 +13723,7 @@
         <v>1</v>
       </c>
       <c r="AC8" s="1" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
     </row>
     <row r="9" spans="1:31" ht="17" x14ac:dyDescent="0.2">
@@ -14264,7 +13815,7 @@
         <v>2</v>
       </c>
       <c r="AC9" s="1" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
     </row>
     <row r="10" spans="1:31" ht="17" x14ac:dyDescent="0.2">
@@ -14356,13 +13907,13 @@
         <v>2</v>
       </c>
       <c r="AC10" s="1" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="AD10" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="AE10" s="19" t="s">
         <v>433</v>
-      </c>
-      <c r="AE10" s="19" t="s">
-        <v>437</v>
       </c>
     </row>
     <row r="11" spans="1:31" ht="17" x14ac:dyDescent="0.2">
@@ -14454,7 +14005,7 @@
         <v>3</v>
       </c>
       <c r="AC11" s="1" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
     </row>
     <row r="12" spans="1:31" ht="17" x14ac:dyDescent="0.2">
@@ -14546,7 +14097,7 @@
         <v>3</v>
       </c>
       <c r="AC12" s="1" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
     </row>
     <row r="13" spans="1:31" ht="17" x14ac:dyDescent="0.2">
@@ -14638,7 +14189,7 @@
         <v>3</v>
       </c>
       <c r="AC13" s="1" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
     </row>
     <row r="14" spans="1:31" ht="17" x14ac:dyDescent="0.2">
@@ -14941,4 +14492,400 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="51" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AE4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G42" sqref="G42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="8" max="8" width="38.5" customWidth="1"/>
+    <col min="9" max="9" width="79.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:31" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>370</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q1" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="R1" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="S1" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="T1" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="U1" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="V1" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="W1" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="X1" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="Y1" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="Z1" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="AA1" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="AB1" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="AC1" s="6" t="s">
+        <v>371</v>
+      </c>
+      <c r="AD1" s="6" t="s">
+        <v>372</v>
+      </c>
+      <c r="AE1" s="6" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2" s="27">
+        <v>134</v>
+      </c>
+      <c r="D2" s="11">
+        <v>42562</v>
+      </c>
+      <c r="E2" s="27">
+        <v>28</v>
+      </c>
+      <c r="F2" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>409</v>
+      </c>
+      <c r="J2" s="7">
+        <v>1</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="O2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="P2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q2" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="R2" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="S2" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="T2" s="31">
+        <v>3</v>
+      </c>
+      <c r="U2" s="31">
+        <v>-2</v>
+      </c>
+      <c r="V2" s="35">
+        <v>17200</v>
+      </c>
+      <c r="W2" s="35">
+        <v>21000</v>
+      </c>
+      <c r="X2" s="36">
+        <f>W2-V2</f>
+        <v>3800</v>
+      </c>
+      <c r="Y2" s="27">
+        <v>150</v>
+      </c>
+      <c r="Z2" s="33" t="s">
+        <v>112</v>
+      </c>
+      <c r="AA2" s="7">
+        <v>1</v>
+      </c>
+      <c r="AB2" s="27">
+        <v>1</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD2" s="1">
+        <v>4</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="C3" s="27">
+        <v>134</v>
+      </c>
+      <c r="D3" s="11">
+        <v>42564</v>
+      </c>
+      <c r="E3" s="27">
+        <v>28</v>
+      </c>
+      <c r="F3" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>410</v>
+      </c>
+      <c r="J3" s="7">
+        <v>1</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>287</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="O3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="P3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q3" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="R3" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="S3" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="T3" s="31">
+        <v>3</v>
+      </c>
+      <c r="U3" s="31">
+        <v>-2</v>
+      </c>
+      <c r="V3" s="35">
+        <v>17200</v>
+      </c>
+      <c r="W3" s="35">
+        <v>21000</v>
+      </c>
+      <c r="X3" s="36">
+        <f t="shared" ref="X3:X4" si="0">W3-V3</f>
+        <v>3800</v>
+      </c>
+      <c r="Y3" s="27">
+        <v>150</v>
+      </c>
+      <c r="Z3" s="33" t="s">
+        <v>112</v>
+      </c>
+      <c r="AA3" s="7">
+        <v>1</v>
+      </c>
+      <c r="AB3" s="27">
+        <v>1</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD3" s="1">
+        <v>4</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="C4" s="27">
+        <v>135</v>
+      </c>
+      <c r="D4" s="11">
+        <v>42566</v>
+      </c>
+      <c r="E4" s="27">
+        <v>28</v>
+      </c>
+      <c r="F4" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>411</v>
+      </c>
+      <c r="J4" s="7">
+        <v>1</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>288</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="N4" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="O4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="P4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q4" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="R4" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="S4" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="T4" s="31">
+        <v>3</v>
+      </c>
+      <c r="U4" s="31">
+        <v>-1</v>
+      </c>
+      <c r="V4" s="35">
+        <v>17200</v>
+      </c>
+      <c r="W4" s="35">
+        <v>21500</v>
+      </c>
+      <c r="X4" s="36">
+        <f t="shared" si="0"/>
+        <v>4300</v>
+      </c>
+      <c r="Y4" s="27">
+        <v>150</v>
+      </c>
+      <c r="Z4" s="33" t="s">
+        <v>112</v>
+      </c>
+      <c r="AA4" s="7">
+        <v>1</v>
+      </c>
+      <c r="AB4" s="27">
+        <v>2</v>
+      </c>
+      <c r="AC4" s="1"/>
+      <c r="AD4" s="1"/>
+      <c r="AE4" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated to process different task types
</commit_message>
<xml_diff>
--- a/config/SFN_NHP_Coordinates_All.xlsx
+++ b/config/SFN_NHP_Coordinates_All.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4240" yWindow="460" windowWidth="30860" windowHeight="19440" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="5540" yWindow="7520" windowWidth="30860" windowHeight="19440" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Br" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1882" uniqueCount="435">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1919" uniqueCount="437">
   <si>
     <t>a3</t>
   </si>
@@ -1338,6 +1338,12 @@
   </si>
   <si>
     <t>16, 15, 14, 13, 12, 11, 10, 9</t>
+  </si>
+  <si>
+    <t>1, 2, 3, 4</t>
+  </si>
+  <si>
+    <t>1, 2, 3</t>
   </si>
 </sst>
 </file>
@@ -2334,8 +2340,8 @@
   </sheetPr>
   <dimension ref="A1:AD22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Z32" sqref="Z32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2533,8 +2539,8 @@
       <c r="Y2" s="1">
         <v>1</v>
       </c>
-      <c r="Z2" s="1">
-        <v>1</v>
+      <c r="Z2" s="1" t="s">
+        <v>436</v>
       </c>
       <c r="AA2" s="1" t="s">
         <v>82</v>
@@ -9144,7 +9150,7 @@
   <dimension ref="A1:AE53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+      <selection activeCell="Z32" sqref="Z32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9340,7 +9346,7 @@
         <v>150</v>
       </c>
       <c r="Z2" s="33" t="s">
-        <v>112</v>
+        <v>436</v>
       </c>
       <c r="AA2" s="7">
         <v>1</v>
@@ -14496,16 +14502,17 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE4"/>
+  <dimension ref="A1:AE6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G42" sqref="G42"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="Z32" sqref="Z32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="8" max="8" width="38.5" customWidth="1"/>
     <col min="9" max="9" width="79.83203125" customWidth="1"/>
+    <col min="26" max="26" width="108.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="17" x14ac:dyDescent="0.2">
@@ -14611,10 +14618,10 @@
         <v>110</v>
       </c>
       <c r="C2" s="27">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="D2" s="11">
-        <v>42562</v>
+        <v>42639</v>
       </c>
       <c r="E2" s="27">
         <v>28</v>
@@ -14626,16 +14633,16 @@
         <v>111</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>409</v>
+        <v>423</v>
       </c>
       <c r="J2" s="7">
         <v>1</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>286</v>
+        <v>300</v>
       </c>
       <c r="L2" s="7" t="s">
         <v>119</v>
@@ -14656,43 +14663,43 @@
         <v>35</v>
       </c>
       <c r="R2" s="27" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="S2" s="27" t="s">
         <v>1</v>
       </c>
       <c r="T2" s="31">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="U2" s="31">
         <v>-2</v>
       </c>
       <c r="V2" s="35">
-        <v>17200</v>
+        <v>18000</v>
       </c>
       <c r="W2" s="35">
-        <v>21000</v>
+        <v>18500</v>
       </c>
       <c r="X2" s="36">
-        <f>W2-V2</f>
-        <v>3800</v>
+        <f t="shared" ref="X2" si="0">W2-V2</f>
+        <v>500</v>
       </c>
       <c r="Y2" s="27">
         <v>150</v>
       </c>
       <c r="Z2" s="33" t="s">
-        <v>112</v>
+        <v>436</v>
       </c>
       <c r="AA2" s="7">
         <v>1</v>
       </c>
       <c r="AB2" s="27">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="AC2" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="AD2" s="1">
+      <c r="AD2" s="7">
         <v>4</v>
       </c>
       <c r="AE2" s="1" t="s">
@@ -14707,10 +14714,10 @@
         <v>110</v>
       </c>
       <c r="C3" s="27">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="D3" s="11">
-        <v>42564</v>
+        <v>42590</v>
       </c>
       <c r="E3" s="27">
         <v>28</v>
@@ -14722,16 +14729,16 @@
         <v>111</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>410</v>
+        <v>413</v>
       </c>
       <c r="J3" s="7">
         <v>1</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="L3" s="7" t="s">
         <v>119</v>
@@ -14752,38 +14759,38 @@
         <v>35</v>
       </c>
       <c r="R3" s="27" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="S3" s="27" t="s">
         <v>1</v>
       </c>
       <c r="T3" s="31">
-        <v>3</v>
-      </c>
-      <c r="U3" s="31">
+        <v>2</v>
+      </c>
+      <c r="U3" s="34">
         <v>-2</v>
       </c>
-      <c r="V3" s="35">
-        <v>17200</v>
-      </c>
-      <c r="W3" s="35">
-        <v>21000</v>
+      <c r="V3" s="36">
+        <v>18000</v>
+      </c>
+      <c r="W3" s="36">
+        <v>25000</v>
       </c>
       <c r="X3" s="36">
-        <f t="shared" ref="X3:X4" si="0">W3-V3</f>
-        <v>3800</v>
+        <f t="shared" ref="X3" si="1">W3-V3</f>
+        <v>7000</v>
       </c>
       <c r="Y3" s="27">
         <v>150</v>
       </c>
       <c r="Z3" s="33" t="s">
-        <v>112</v>
+        <v>435</v>
       </c>
       <c r="AA3" s="7">
         <v>1</v>
       </c>
       <c r="AB3" s="27">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="AC3" s="1" t="s">
         <v>82</v>
@@ -14803,10 +14810,10 @@
         <v>110</v>
       </c>
       <c r="C4" s="27">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D4" s="11">
-        <v>42566</v>
+        <v>42562</v>
       </c>
       <c r="E4" s="27">
         <v>28</v>
@@ -14818,16 +14825,16 @@
         <v>111</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="J4" s="7">
         <v>1</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="L4" s="7" t="s">
         <v>119</v>
@@ -14851,23 +14858,23 @@
         <v>0</v>
       </c>
       <c r="S4" s="27" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="T4" s="31">
         <v>3</v>
       </c>
       <c r="U4" s="31">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="V4" s="35">
         <v>17200</v>
       </c>
       <c r="W4" s="35">
-        <v>21500</v>
+        <v>21000</v>
       </c>
       <c r="X4" s="36">
-        <f t="shared" si="0"/>
-        <v>4300</v>
+        <f>W4-V4</f>
+        <v>3800</v>
       </c>
       <c r="Y4" s="27">
         <v>150</v>
@@ -14879,11 +14886,203 @@
         <v>1</v>
       </c>
       <c r="AB4" s="27">
+        <v>1</v>
+      </c>
+      <c r="AC4" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD4" s="1">
+        <v>4</v>
+      </c>
+      <c r="AE4" s="1" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="C5" s="27">
+        <v>134</v>
+      </c>
+      <c r="D5" s="11">
+        <v>42564</v>
+      </c>
+      <c r="E5" s="27">
+        <v>28</v>
+      </c>
+      <c r="F5" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>410</v>
+      </c>
+      <c r="J5" s="7">
+        <v>1</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>287</v>
+      </c>
+      <c r="L5" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="N5" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="O5" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="P5" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q5" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="R5" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="S5" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="T5" s="31">
+        <v>3</v>
+      </c>
+      <c r="U5" s="31">
+        <v>-2</v>
+      </c>
+      <c r="V5" s="35">
+        <v>17200</v>
+      </c>
+      <c r="W5" s="35">
+        <v>21000</v>
+      </c>
+      <c r="X5" s="36">
+        <f t="shared" ref="X5:X6" si="2">W5-V5</f>
+        <v>3800</v>
+      </c>
+      <c r="Y5" s="27">
+        <v>150</v>
+      </c>
+      <c r="Z5" s="33" t="s">
+        <v>112</v>
+      </c>
+      <c r="AA5" s="7">
+        <v>1</v>
+      </c>
+      <c r="AB5" s="27">
+        <v>1</v>
+      </c>
+      <c r="AC5" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD5" s="1">
+        <v>4</v>
+      </c>
+      <c r="AE5" s="1" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="C6" s="27">
+        <v>135</v>
+      </c>
+      <c r="D6" s="11">
+        <v>42566</v>
+      </c>
+      <c r="E6" s="27">
+        <v>28</v>
+      </c>
+      <c r="F6" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>411</v>
+      </c>
+      <c r="J6" s="7">
+        <v>1</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>288</v>
+      </c>
+      <c r="L6" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="M6" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="N6" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="O6" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="P6" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q6" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="R6" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="S6" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="T6" s="31">
+        <v>3</v>
+      </c>
+      <c r="U6" s="31">
+        <v>-1</v>
+      </c>
+      <c r="V6" s="35">
+        <v>17200</v>
+      </c>
+      <c r="W6" s="35">
+        <v>21500</v>
+      </c>
+      <c r="X6" s="36">
+        <f t="shared" si="2"/>
+        <v>4300</v>
+      </c>
+      <c r="Y6" s="27">
+        <v>150</v>
+      </c>
+      <c r="Z6" s="33" t="s">
+        <v>112</v>
+      </c>
+      <c r="AA6" s="7">
+        <v>1</v>
+      </c>
+      <c r="AB6" s="27">
         <v>2</v>
       </c>
-      <c r="AC4" s="1"/>
-      <c r="AD4" s="1"/>
-      <c r="AE4" s="1"/>
+      <c r="AC6" s="1"/>
+      <c r="AD6" s="1"/>
+      <c r="AE6" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated for processing darwinK
</commit_message>
<xml_diff>
--- a/config/SFN_NHP_Coordinates_All.xlsx
+++ b/config/SFN_NHP_Coordinates_All.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5540" yWindow="7520" windowWidth="30860" windowHeight="19440" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="-160" yWindow="9360" windowWidth="30860" windowHeight="19440" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Br" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1919" uniqueCount="437">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1918" uniqueCount="436">
   <si>
     <t>a3</t>
   </si>
@@ -1341,9 +1341,6 @@
   </si>
   <si>
     <t>1, 2, 3, 4</t>
-  </si>
-  <si>
-    <t>1, 2, 3</t>
   </si>
 </sst>
 </file>
@@ -2341,7 +2338,7 @@
   <dimension ref="A1:AD22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z32" sqref="Z32"/>
+      <selection activeCell="Z2" sqref="Z2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2539,8 +2536,8 @@
       <c r="Y2" s="1">
         <v>1</v>
       </c>
-      <c r="Z2" s="1" t="s">
-        <v>436</v>
+      <c r="Z2" s="1">
+        <v>2</v>
       </c>
       <c r="AA2" s="1" t="s">
         <v>82</v>
@@ -9149,8 +9146,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z32" sqref="Z32"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="Z2" sqref="Z2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9346,7 +9343,7 @@
         <v>150</v>
       </c>
       <c r="Z2" s="33" t="s">
-        <v>436</v>
+        <v>112</v>
       </c>
       <c r="AA2" s="7">
         <v>1</v>
@@ -14505,7 +14502,7 @@
   <dimension ref="A1:AE6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="Z32" sqref="Z32"/>
+      <selection activeCell="Z2" sqref="Z2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14688,7 +14685,7 @@
         <v>150</v>
       </c>
       <c r="Z2" s="33" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="AA2" s="7">
         <v>1</v>

</xml_diff>

<commit_message>
poster figs udated spreadsheet updated
</commit_message>
<xml_diff>
--- a/config/SFN_NHP_Coordinates_All.xlsx
+++ b/config/SFN_NHP_Coordinates_All.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4240" yWindow="460" windowWidth="30860" windowHeight="19440" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="38740" yWindow="460" windowWidth="37540" windowHeight="19440" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Br" sheetId="2" r:id="rId1"/>
@@ -1455,7 +1455,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1477,6 +1477,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1691,7 +1709,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1866,6 +1884,73 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="11" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="199">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2346,8 +2431,8 @@
   </sheetPr>
   <dimension ref="A1:AD22"/>
   <sheetViews>
-    <sheetView topLeftCell="AA1" workbookViewId="0">
-      <selection activeCell="AD1" sqref="AD1:AD1048576"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2368,8 +2453,8 @@
     <col min="22" max="23" width="18.83203125" customWidth="1"/>
     <col min="24" max="24" width="89.33203125" customWidth="1"/>
     <col min="25" max="26" width="26" customWidth="1"/>
-    <col min="27" max="27" width="48" style="1" customWidth="1"/>
-    <col min="28" max="28" width="35" style="1" customWidth="1"/>
+    <col min="27" max="27" width="27.6640625" style="1" customWidth="1"/>
+    <col min="28" max="28" width="20.6640625" style="1" customWidth="1"/>
     <col min="29" max="29" width="71" style="1" customWidth="1"/>
     <col min="30" max="30" width="88.6640625" style="1" customWidth="1"/>
   </cols>
@@ -2609,10 +2694,10 @@
         <f t="shared" ref="O3:O18" si="2">IF(N3="left", "right", "left")</f>
         <v>left</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="P3" s="60" t="s">
         <v>45</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="Q3" s="60" t="s">
         <v>46</v>
       </c>
       <c r="R3" s="8">
@@ -2701,10 +2786,10 @@
         <f t="shared" si="2"/>
         <v>left</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="P4" s="60" t="s">
         <v>45</v>
       </c>
-      <c r="Q4" s="1" t="s">
+      <c r="Q4" s="60" t="s">
         <v>46</v>
       </c>
       <c r="R4" s="8">
@@ -2888,10 +2973,10 @@
         <f t="shared" si="2"/>
         <v>right</v>
       </c>
-      <c r="P6" s="1" t="s">
+      <c r="P6" s="61" t="s">
         <v>51</v>
       </c>
-      <c r="Q6" s="1" t="s">
+      <c r="Q6" s="61" t="s">
         <v>50</v>
       </c>
       <c r="R6" s="8">
@@ -2980,10 +3065,10 @@
         <f t="shared" si="2"/>
         <v>right</v>
       </c>
-      <c r="P7" s="1" t="s">
+      <c r="P7" s="61" t="s">
         <v>51</v>
       </c>
-      <c r="Q7" s="1" t="s">
+      <c r="Q7" s="61" t="s">
         <v>50</v>
       </c>
       <c r="R7" s="8">
@@ -3300,97 +3385,98 @@
         <v>401</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:30" s="70" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="65" t="s">
         <v>99</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="56" t="s">
         <v>101</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="65">
         <v>216</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="66">
         <v>42473</v>
       </c>
-      <c r="E11" s="10">
+      <c r="E11" s="67">
         <v>29</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F11" s="65" t="s">
         <v>43</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="G11" s="65" t="s">
         <v>100</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="H11" s="65" t="s">
         <v>130</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="I11" s="65" t="s">
         <v>190</v>
       </c>
-      <c r="J11" s="39" t="s">
+      <c r="J11" s="65" t="s">
         <v>211</v>
       </c>
-      <c r="K11" s="1" t="s">
+      <c r="K11" s="65" t="s">
         <v>48</v>
       </c>
-      <c r="L11" s="1" t="s">
+      <c r="L11" s="65" t="s">
         <v>86</v>
       </c>
-      <c r="M11" s="1" t="s">
+      <c r="M11" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="N11" s="1" t="str">
+      <c r="N11" s="65" t="str">
         <f t="shared" si="1"/>
         <v>left</v>
       </c>
-      <c r="O11" s="1" t="str">
+      <c r="O11" s="65" t="str">
         <f t="shared" si="2"/>
         <v>right</v>
       </c>
-      <c r="P11" s="1" t="s">
+      <c r="P11" s="65" t="s">
         <v>47</v>
       </c>
-      <c r="Q11" s="1" t="s">
+      <c r="Q11" s="65" t="s">
         <v>55</v>
       </c>
-      <c r="R11" s="8">
+      <c r="R11" s="68">
         <v>-6</v>
       </c>
-      <c r="S11" s="8">
+      <c r="S11" s="68">
         <v>4</v>
       </c>
-      <c r="T11" s="1">
+      <c r="T11" s="65">
         <v>19000</v>
       </c>
-      <c r="U11" s="1">
+      <c r="U11" s="65">
         <v>22000</v>
       </c>
-      <c r="V11" s="1">
+      <c r="V11" s="65">
         <f t="shared" si="0"/>
         <v>3000</v>
       </c>
-      <c r="W11" s="1">
+      <c r="W11" s="65">
         <v>100</v>
       </c>
-      <c r="X11" s="7" t="s">
+      <c r="X11" s="53" t="s">
         <v>98</v>
       </c>
-      <c r="Y11" s="1">
+      <c r="Y11" s="65">
         <v>8</v>
       </c>
-      <c r="Z11" s="1">
+      <c r="Z11" s="65">
         <v>8</v>
       </c>
-      <c r="AA11" s="1" t="s">
+      <c r="AA11" s="65" t="s">
         <v>82</v>
       </c>
-      <c r="AB11" s="19">
+      <c r="AB11" s="69">
         <v>2</v>
       </c>
-      <c r="AC11" s="1" t="s">
+      <c r="AC11" s="65" t="s">
         <v>403</v>
       </c>
+      <c r="AD11" s="65"/>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
@@ -3532,10 +3618,10 @@
         <f t="shared" si="2"/>
         <v>right</v>
       </c>
-      <c r="P13" s="1" t="s">
+      <c r="P13" s="62" t="s">
         <v>52</v>
       </c>
-      <c r="Q13" s="1" t="s">
+      <c r="Q13" s="62" t="s">
         <v>58</v>
       </c>
       <c r="R13" s="8">
@@ -3808,10 +3894,10 @@
         <f t="shared" si="2"/>
         <v>right</v>
       </c>
-      <c r="P16" s="1" t="s">
+      <c r="P16" s="63" t="s">
         <v>52</v>
       </c>
-      <c r="Q16" s="1" t="s">
+      <c r="Q16" s="63" t="s">
         <v>55</v>
       </c>
       <c r="R16" s="8">
@@ -3900,10 +3986,10 @@
         <f t="shared" si="2"/>
         <v>right</v>
       </c>
-      <c r="P17" s="1" t="s">
+      <c r="P17" s="62" t="s">
         <v>52</v>
       </c>
-      <c r="Q17" s="1" t="s">
+      <c r="Q17" s="62" t="s">
         <v>58</v>
       </c>
       <c r="R17" s="8">
@@ -4365,10 +4451,10 @@
         <f t="shared" si="4"/>
         <v>right</v>
       </c>
-      <c r="P22" s="1" t="s">
+      <c r="P22" s="63" t="s">
         <v>52</v>
       </c>
-      <c r="Q22" s="1" t="s">
+      <c r="Q22" s="63" t="s">
         <v>55</v>
       </c>
       <c r="R22" s="8">
@@ -4430,8 +4516,8 @@
   </sheetPr>
   <dimension ref="A1:AF24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AD19" sqref="AD19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5034,99 +5120,100 @@
         <v>407</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:32" s="65" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="65" t="s">
         <v>72</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="53" t="s">
         <v>84</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="53">
         <v>33</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="66">
         <v>42669</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="65">
         <v>29</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="65" t="s">
         <v>43</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" s="65" t="s">
         <v>62</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="65" t="s">
         <v>147</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="I7" s="65" t="s">
         <v>229</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="J7" s="71" t="s">
         <v>248</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="K7" s="65" t="s">
         <v>48</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="L7" s="65" t="s">
         <v>86</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="M7" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="N7" s="1" t="str">
+      <c r="N7" s="65" t="str">
         <f t="shared" si="0"/>
         <v>left</v>
       </c>
-      <c r="O7" s="1" t="str">
+      <c r="O7" s="65" t="str">
         <f t="shared" si="1"/>
         <v>right</v>
       </c>
-      <c r="P7" s="1" t="s">
+      <c r="P7" s="65" t="s">
         <v>69</v>
       </c>
-      <c r="Q7" s="1" t="s">
+      <c r="Q7" s="65" t="s">
         <v>64</v>
       </c>
-      <c r="R7" s="8">
+      <c r="R7" s="68">
         <v>4.8</v>
       </c>
-      <c r="S7" s="8">
+      <c r="S7" s="68">
         <v>-4.7</v>
       </c>
-      <c r="T7" s="1">
+      <c r="T7" s="65">
         <v>20000</v>
       </c>
-      <c r="U7" s="1">
+      <c r="U7" s="65">
         <v>25500</v>
       </c>
-      <c r="V7" s="1">
+      <c r="V7" s="65">
         <v>5500</v>
       </c>
-      <c r="W7" s="1">
+      <c r="W7" s="65">
         <v>100</v>
       </c>
-      <c r="X7" s="7" t="s">
+      <c r="X7" s="53" t="s">
         <v>98</v>
       </c>
-      <c r="Y7" s="1">
+      <c r="Y7" s="65">
         <v>8</v>
       </c>
-      <c r="Z7" s="1">
+      <c r="Z7" s="65">
         <v>5</v>
       </c>
-      <c r="AA7" s="19" t="s">
+      <c r="AA7" s="69" t="s">
         <v>147</v>
       </c>
-      <c r="AB7" s="1" t="s">
+      <c r="AB7" s="65" t="s">
         <v>82</v>
       </c>
-      <c r="AC7" s="1">
+      <c r="AC7" s="65">
         <v>2</v>
       </c>
-      <c r="AD7" s="1" t="s">
+      <c r="AD7" s="65" t="s">
         <v>383</v>
       </c>
+      <c r="AF7" s="69"/>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
@@ -5977,7 +6064,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>72</v>
       </c>
@@ -6072,7 +6159,7 @@
       </c>
       <c r="AE17"/>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>72</v>
       </c>
@@ -6167,7 +6254,7 @@
       </c>
       <c r="AE18"/>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>72</v>
       </c>
@@ -6262,114 +6349,115 @@
       </c>
       <c r="AE19"/>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
+    <row r="20" spans="1:32" s="65" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="65" t="s">
         <v>72</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="53" t="s">
         <v>84</v>
       </c>
-      <c r="C20" s="7">
+      <c r="C20" s="53">
         <v>45</v>
       </c>
-      <c r="D20" s="3">
+      <c r="D20" s="66">
         <v>42754</v>
       </c>
-      <c r="E20" s="1">
+      <c r="E20" s="65">
         <v>29</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="F20" s="65" t="s">
         <v>43</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="G20" s="65" t="s">
         <v>62</v>
       </c>
-      <c r="H20" s="1" t="s">
+      <c r="H20" s="65" t="s">
         <v>160</v>
       </c>
-      <c r="I20" s="1" t="s">
+      <c r="I20" s="65" t="s">
         <v>242</v>
       </c>
-      <c r="J20" s="2" t="s">
+      <c r="J20" s="71" t="s">
         <v>261</v>
       </c>
-      <c r="K20" s="1" t="s">
+      <c r="K20" s="65" t="s">
         <v>48</v>
       </c>
-      <c r="L20" s="1" t="s">
+      <c r="L20" s="65" t="s">
         <v>86</v>
       </c>
-      <c r="M20" s="1" t="s">
+      <c r="M20" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="N20" s="1" t="str">
+      <c r="N20" s="65" t="str">
         <f t="shared" si="0"/>
         <v>left</v>
       </c>
-      <c r="O20" s="1" t="str">
+      <c r="O20" s="65" t="str">
         <f t="shared" si="1"/>
         <v>right</v>
       </c>
-      <c r="P20" s="1" t="s">
+      <c r="P20" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="Q20" s="1" t="s">
+      <c r="Q20" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="R20" s="8">
+      <c r="R20" s="68">
         <v>2</v>
       </c>
-      <c r="S20" s="8">
+      <c r="S20" s="68">
         <v>-3</v>
       </c>
-      <c r="T20" s="1">
+      <c r="T20" s="65">
         <v>20000</v>
       </c>
-      <c r="U20" s="1">
+      <c r="U20" s="65">
         <v>26000</v>
       </c>
-      <c r="V20" s="1">
+      <c r="V20" s="65">
         <v>6000</v>
       </c>
-      <c r="W20" s="1">
+      <c r="W20" s="65">
         <v>100</v>
       </c>
-      <c r="X20" s="7" t="s">
+      <c r="X20" s="53" t="s">
         <v>98</v>
       </c>
-      <c r="Y20" s="1">
+      <c r="Y20" s="65">
         <v>8</v>
       </c>
-      <c r="Z20" s="1">
+      <c r="Z20" s="65">
         <v>8</v>
       </c>
-      <c r="AA20" s="19" t="s">
+      <c r="AA20" s="69" t="s">
         <v>160</v>
       </c>
-      <c r="AB20" s="1" t="s">
+      <c r="AB20" s="65" t="s">
         <v>82</v>
       </c>
-      <c r="AC20" s="7">
+      <c r="AC20" s="53">
         <v>1</v>
       </c>
-      <c r="AD20" s="1" t="s">
+      <c r="AD20" s="65" t="s">
         <v>405</v>
       </c>
-      <c r="AE20"/>
-    </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="AE20" s="70"/>
+      <c r="AF20" s="69"/>
+    </row>
+    <row r="21" spans="1:32" x14ac:dyDescent="0.2">
       <c r="AC21" s="7"/>
       <c r="AE21"/>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:32" x14ac:dyDescent="0.2">
       <c r="AC22" s="7"/>
       <c r="AE22"/>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:32" x14ac:dyDescent="0.2">
       <c r="AC23" s="7"/>
       <c r="AD23" s="7"/>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:32" x14ac:dyDescent="0.2">
       <c r="AC24" s="7"/>
       <c r="AD24" s="7"/>
     </row>
@@ -6387,8 +6475,8 @@
   </sheetPr>
   <dimension ref="A1:AC88"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="W9" sqref="W9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6786,95 +6874,95 @@
         <v>398</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A5" s="19" t="s">
+    <row r="5" spans="1:29" s="65" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="69" t="s">
         <v>109</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="54" t="s">
         <v>110</v>
       </c>
-      <c r="C5" s="19">
+      <c r="C5" s="69">
         <v>129</v>
       </c>
-      <c r="D5" s="26">
+      <c r="D5" s="72">
         <v>42422</v>
       </c>
-      <c r="E5" s="19">
+      <c r="E5" s="69">
         <v>28</v>
       </c>
-      <c r="F5" s="27" t="s">
+      <c r="F5" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="19" t="s">
+      <c r="G5" s="69" t="s">
         <v>62</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="H5" s="53" t="s">
         <v>164</v>
       </c>
-      <c r="I5" s="19" t="s">
+      <c r="I5" s="69" t="s">
         <v>277</v>
       </c>
-      <c r="J5" s="19" t="s">
+      <c r="J5" s="69" t="s">
         <v>265</v>
       </c>
-      <c r="K5" s="19" t="s">
+      <c r="K5" s="69" t="s">
         <v>48</v>
       </c>
-      <c r="L5" s="19" t="s">
+      <c r="L5" s="69" t="s">
         <v>86</v>
       </c>
-      <c r="M5" s="19" t="s">
+      <c r="M5" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="N5" s="19" t="str">
+      <c r="N5" s="69" t="str">
         <f t="shared" si="0"/>
         <v>left</v>
       </c>
-      <c r="O5" s="19" t="str">
+      <c r="O5" s="69" t="str">
         <f t="shared" si="1"/>
         <v>right</v>
       </c>
-      <c r="P5" s="19" t="s">
+      <c r="P5" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="Q5" s="19" t="s">
+      <c r="Q5" s="69" t="s">
         <v>10</v>
       </c>
-      <c r="R5" s="28">
+      <c r="R5" s="73">
         <v>2</v>
       </c>
-      <c r="S5" s="28">
+      <c r="S5" s="73">
         <v>0</v>
       </c>
-      <c r="T5" s="38">
+      <c r="T5" s="69">
         <v>18000</v>
       </c>
-      <c r="U5" s="38">
+      <c r="U5" s="69">
         <v>24500</v>
       </c>
-      <c r="V5" s="38">
+      <c r="V5" s="69">
         <f t="shared" si="2"/>
         <v>6500</v>
       </c>
-      <c r="W5" s="19">
+      <c r="W5" s="69">
         <v>150</v>
       </c>
-      <c r="X5" s="29" t="s">
+      <c r="X5" s="74" t="s">
         <v>112</v>
       </c>
-      <c r="Y5" s="32">
+      <c r="Y5" s="75">
         <v>1</v>
       </c>
-      <c r="Z5" s="19">
+      <c r="Z5" s="69">
         <v>4</v>
       </c>
-      <c r="AA5" s="1" t="s">
+      <c r="AA5" s="65" t="s">
         <v>82</v>
       </c>
-      <c r="AB5" s="1">
+      <c r="AB5" s="65">
         <v>2</v>
       </c>
-      <c r="AC5" s="1" t="s">
+      <c r="AC5" s="65" t="s">
         <v>388</v>
       </c>
     </row>
@@ -7062,95 +7150,95 @@
         <v>386</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A8" s="19" t="s">
+    <row r="8" spans="1:29" s="65" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="69" t="s">
         <v>109</v>
       </c>
-      <c r="B8" s="25" t="s">
+      <c r="B8" s="54" t="s">
         <v>110</v>
       </c>
-      <c r="C8" s="19">
+      <c r="C8" s="69">
         <v>130</v>
       </c>
-      <c r="D8" s="26">
+      <c r="D8" s="72">
         <v>42426</v>
       </c>
-      <c r="E8" s="19">
+      <c r="E8" s="69">
         <v>28</v>
       </c>
-      <c r="F8" s="27" t="s">
+      <c r="F8" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="G8" s="19" t="s">
+      <c r="G8" s="69" t="s">
         <v>62</v>
       </c>
-      <c r="H8" s="7" t="s">
+      <c r="H8" s="53" t="s">
         <v>167</v>
       </c>
-      <c r="I8" s="19" t="s">
+      <c r="I8" s="69" t="s">
         <v>280</v>
       </c>
-      <c r="J8" s="19" t="s">
+      <c r="J8" s="69" t="s">
         <v>268</v>
       </c>
-      <c r="K8" s="19" t="s">
+      <c r="K8" s="69" t="s">
         <v>48</v>
       </c>
-      <c r="L8" s="19" t="s">
+      <c r="L8" s="69" t="s">
         <v>86</v>
       </c>
-      <c r="M8" s="19" t="s">
+      <c r="M8" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="N8" s="19" t="str">
+      <c r="N8" s="69" t="str">
         <f t="shared" ref="N8:N13" si="3">M8</f>
         <v>left</v>
       </c>
-      <c r="O8" s="19" t="str">
+      <c r="O8" s="69" t="str">
         <f t="shared" ref="O8:O13" si="4">IF(N8="left", "right", "left")</f>
         <v>right</v>
       </c>
-      <c r="P8" s="19" t="s">
+      <c r="P8" s="69" t="s">
         <v>11</v>
       </c>
-      <c r="Q8" s="19" t="s">
+      <c r="Q8" s="69" t="s">
         <v>10</v>
       </c>
-      <c r="R8" s="28">
+      <c r="R8" s="73">
         <v>1</v>
       </c>
-      <c r="S8" s="28">
+      <c r="S8" s="73">
         <v>0</v>
       </c>
-      <c r="T8" s="38">
+      <c r="T8" s="69">
         <v>18000</v>
       </c>
-      <c r="U8" s="38">
+      <c r="U8" s="69">
         <v>23200</v>
       </c>
-      <c r="V8" s="38">
+      <c r="V8" s="69">
         <f t="shared" si="2"/>
         <v>5200</v>
       </c>
-      <c r="W8" s="19">
+      <c r="W8" s="69">
         <v>150</v>
       </c>
-      <c r="X8" s="29" t="s">
+      <c r="X8" s="74" t="s">
         <v>112</v>
       </c>
-      <c r="Y8" s="32">
+      <c r="Y8" s="75">
         <v>1</v>
       </c>
-      <c r="Z8" s="19">
+      <c r="Z8" s="69">
         <v>5</v>
       </c>
-      <c r="AA8" s="1" t="s">
+      <c r="AA8" s="65" t="s">
         <v>82</v>
       </c>
-      <c r="AB8" s="1">
+      <c r="AB8" s="65">
         <v>2</v>
       </c>
-      <c r="AC8" s="1" t="s">
+      <c r="AC8" s="65" t="s">
         <v>388</v>
       </c>
     </row>
@@ -9155,7 +9243,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE53"/>
   <sheetViews>
-    <sheetView topLeftCell="W1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I44" sqref="I44"/>
     </sheetView>
   </sheetViews>
@@ -11956,8 +12044,8 @@
   </sheetPr>
   <dimension ref="A1:AE37"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="X9" sqref="X9"/>
+    <sheetView topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="AB14" activeCellId="3" sqref="AB4 AB6 AB8 AB14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12178,97 +12266,98 @@
         <v>386</v>
       </c>
     </row>
-    <row r="3" spans="1:31" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="19" t="s">
+    <row r="3" spans="1:31" s="69" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="69" t="s">
         <v>107</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="76" t="s">
         <v>108</v>
       </c>
-      <c r="C3" s="17">
+      <c r="C3" s="77">
         <v>60</v>
       </c>
-      <c r="D3" s="23">
+      <c r="D3" s="76">
         <v>41982</v>
       </c>
-      <c r="E3" s="17">
+      <c r="E3" s="77">
         <v>28</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F3" s="77" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="15" t="s">
+      <c r="G3" s="78" t="s">
         <v>62</v>
       </c>
-      <c r="H3" s="15" t="s">
+      <c r="H3" s="78" t="s">
         <v>174</v>
       </c>
-      <c r="I3" s="15" t="s">
+      <c r="I3" s="78" t="s">
         <v>305</v>
       </c>
-      <c r="J3" s="15" t="s">
+      <c r="J3" s="78" t="s">
         <v>308</v>
       </c>
-      <c r="K3" s="15" t="s">
+      <c r="K3" s="78" t="s">
         <v>36</v>
       </c>
-      <c r="L3" s="15" t="s">
+      <c r="L3" s="78" t="s">
         <v>44</v>
       </c>
-      <c r="M3" s="15" t="s">
+      <c r="M3" s="78" t="s">
         <v>86</v>
       </c>
-      <c r="N3" s="15" t="s">
+      <c r="N3" s="78" t="s">
         <v>35</v>
       </c>
-      <c r="O3" s="1" t="str">
+      <c r="O3" s="65" t="str">
         <f t="shared" ref="O3:O14" si="1">N3</f>
         <v>right</v>
       </c>
-      <c r="P3" s="1" t="str">
+      <c r="P3" s="65" t="str">
         <f t="shared" ref="P3:P14" si="2">IF(O3="left", "right", "left")</f>
         <v>left</v>
       </c>
-      <c r="Q3" s="15" t="s">
+      <c r="Q3" s="78" t="s">
         <v>11</v>
       </c>
-      <c r="R3" s="15" t="s">
+      <c r="R3" s="78" t="s">
         <v>10</v>
       </c>
-      <c r="S3" s="21">
+      <c r="S3" s="79">
         <v>1</v>
       </c>
-      <c r="T3" s="21">
+      <c r="T3" s="79">
         <v>0</v>
       </c>
-      <c r="U3" s="15">
+      <c r="U3" s="78">
         <v>2100</v>
       </c>
-      <c r="V3" s="15">
+      <c r="V3" s="78">
         <v>3751</v>
       </c>
-      <c r="W3" s="1">
+      <c r="W3" s="65">
         <f>V3-U3</f>
         <v>1651</v>
       </c>
-      <c r="X3" s="15">
+      <c r="X3" s="78">
         <v>150</v>
       </c>
-      <c r="Y3" s="33" t="s">
+      <c r="Y3" s="80" t="s">
         <v>115</v>
       </c>
-      <c r="Z3" s="15">
+      <c r="Z3" s="78">
         <v>1</v>
       </c>
-      <c r="AA3" s="1" t="s">
+      <c r="AA3" s="65" t="s">
         <v>82</v>
       </c>
-      <c r="AB3" s="1">
+      <c r="AB3" s="65">
         <v>1</v>
       </c>
-      <c r="AC3" s="1" t="s">
+      <c r="AC3" s="65" t="s">
         <v>387</v>
       </c>
+      <c r="AD3" s="65"/>
     </row>
     <row r="4" spans="1:31" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="19" t="s">
@@ -12362,97 +12451,98 @@
         <v>388</v>
       </c>
     </row>
-    <row r="5" spans="1:31" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="19" t="s">
+    <row r="5" spans="1:31" s="69" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="69" t="s">
         <v>107</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="76" t="s">
         <v>108</v>
       </c>
-      <c r="C5" s="17">
+      <c r="C5" s="77">
         <v>62</v>
       </c>
-      <c r="D5" s="23">
+      <c r="D5" s="76">
         <v>42009</v>
       </c>
-      <c r="E5" s="17">
+      <c r="E5" s="77">
         <v>28</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="F5" s="77" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="15" t="s">
+      <c r="G5" s="78" t="s">
         <v>62</v>
       </c>
-      <c r="H5" s="15" t="s">
+      <c r="H5" s="78" t="s">
         <v>356</v>
       </c>
-      <c r="I5" s="15" t="s">
+      <c r="I5" s="78" t="s">
         <v>357</v>
       </c>
-      <c r="J5" s="15" t="s">
+      <c r="J5" s="78" t="s">
         <v>310</v>
       </c>
-      <c r="K5" s="15" t="s">
+      <c r="K5" s="78" t="s">
         <v>36</v>
       </c>
-      <c r="L5" s="15" t="s">
+      <c r="L5" s="78" t="s">
         <v>44</v>
       </c>
-      <c r="M5" s="15" t="s">
+      <c r="M5" s="78" t="s">
         <v>86</v>
       </c>
-      <c r="N5" s="15" t="s">
+      <c r="N5" s="78" t="s">
         <v>35</v>
       </c>
-      <c r="O5" s="1" t="str">
+      <c r="O5" s="65" t="str">
         <f t="shared" si="1"/>
         <v>right</v>
       </c>
-      <c r="P5" s="1" t="str">
+      <c r="P5" s="65" t="str">
         <f t="shared" si="2"/>
         <v>left</v>
       </c>
-      <c r="Q5" s="15" t="s">
+      <c r="Q5" s="78" t="s">
         <v>11</v>
       </c>
-      <c r="R5" s="15" t="s">
+      <c r="R5" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="S5" s="21">
+      <c r="S5" s="79">
         <v>1</v>
       </c>
-      <c r="T5" s="21">
+      <c r="T5" s="79">
         <v>-1</v>
       </c>
-      <c r="U5" s="15">
+      <c r="U5" s="78">
         <v>4099</v>
       </c>
-      <c r="V5" s="15">
+      <c r="V5" s="78">
         <v>6005</v>
       </c>
-      <c r="W5" s="1">
+      <c r="W5" s="65">
         <f t="shared" ref="W5:W14" si="3">V5-U5</f>
         <v>1906</v>
       </c>
-      <c r="X5" s="15">
+      <c r="X5" s="78">
         <v>150</v>
       </c>
-      <c r="Y5" s="33" t="s">
+      <c r="Y5" s="80" t="s">
         <v>115</v>
       </c>
-      <c r="Z5" s="15">
+      <c r="Z5" s="78">
         <v>1</v>
       </c>
-      <c r="AA5" s="1" t="s">
+      <c r="AA5" s="65" t="s">
         <v>82</v>
       </c>
-      <c r="AB5" s="1">
+      <c r="AB5" s="65">
         <v>1</v>
       </c>
-      <c r="AC5" s="1" t="s">
+      <c r="AC5" s="65" t="s">
         <v>389</v>
       </c>
+      <c r="AD5" s="65"/>
     </row>
     <row r="6" spans="1:31" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="19" t="s">
@@ -13410,8 +13500,8 @@
   </sheetPr>
   <dimension ref="A1:AE1048576"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="AB9" sqref="H2:AB9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13950,10 +14040,10 @@
         <f t="shared" si="2"/>
         <v>left</v>
       </c>
-      <c r="Q6" s="15" t="s">
+      <c r="Q6" s="64" t="s">
         <v>41</v>
       </c>
-      <c r="R6" s="15" t="s">
+      <c r="R6" s="64" t="s">
         <v>9</v>
       </c>
       <c r="S6" s="21">
@@ -13991,97 +14081,98 @@
         <v>378</v>
       </c>
     </row>
-    <row r="7" spans="1:31" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="15" t="s">
+    <row r="7" spans="1:31" s="69" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="78" t="s">
         <v>104</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="81" t="s">
         <v>105</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="78">
         <v>35</v>
       </c>
-      <c r="D7" s="23">
+      <c r="D7" s="76">
         <v>41990</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E7" s="78">
         <v>28</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="F7" s="78" t="s">
         <v>2</v>
       </c>
-      <c r="G7" s="15" t="s">
+      <c r="G7" s="78" t="s">
         <v>62</v>
       </c>
-      <c r="H7" s="15" t="s">
+      <c r="H7" s="78" t="s">
         <v>181</v>
       </c>
-      <c r="I7" s="15" t="s">
+      <c r="I7" s="78" t="s">
         <v>325</v>
       </c>
-      <c r="J7" s="15" t="s">
+      <c r="J7" s="78" t="s">
         <v>331</v>
       </c>
-      <c r="K7" s="15" t="s">
+      <c r="K7" s="78" t="s">
         <v>36</v>
       </c>
-      <c r="L7" s="15" t="s">
+      <c r="L7" s="78" t="s">
         <v>44</v>
       </c>
-      <c r="M7" s="15" t="s">
+      <c r="M7" s="78" t="s">
         <v>86</v>
       </c>
-      <c r="N7" s="17" t="s">
+      <c r="N7" s="77" t="s">
         <v>35</v>
       </c>
-      <c r="O7" s="1" t="str">
+      <c r="O7" s="65" t="str">
         <f t="shared" si="1"/>
         <v>right</v>
       </c>
-      <c r="P7" s="1" t="str">
+      <c r="P7" s="65" t="str">
         <f t="shared" si="2"/>
         <v>left</v>
       </c>
-      <c r="Q7" s="15" t="s">
+      <c r="Q7" s="78" t="s">
         <v>40</v>
       </c>
-      <c r="R7" s="15" t="s">
+      <c r="R7" s="78" t="s">
         <v>9</v>
       </c>
-      <c r="S7" s="21">
+      <c r="S7" s="79">
         <v>-2</v>
       </c>
-      <c r="T7" s="21">
+      <c r="T7" s="79">
         <v>-2</v>
       </c>
-      <c r="U7" s="15">
+      <c r="U7" s="78">
         <v>2500</v>
       </c>
-      <c r="V7" s="15">
+      <c r="V7" s="78">
         <v>4503</v>
       </c>
-      <c r="W7" s="1">
+      <c r="W7" s="65">
         <f t="shared" si="3"/>
         <v>2003</v>
       </c>
-      <c r="X7" s="15">
+      <c r="X7" s="78">
         <v>150</v>
       </c>
-      <c r="Y7" s="33" t="s">
+      <c r="Y7" s="80" t="s">
         <v>115</v>
       </c>
-      <c r="Z7" s="18">
+      <c r="Z7" s="82">
         <v>1</v>
       </c>
-      <c r="AA7" s="1" t="s">
+      <c r="AA7" s="65" t="s">
         <v>82</v>
       </c>
-      <c r="AB7" s="1">
+      <c r="AB7" s="65">
         <v>1</v>
       </c>
-      <c r="AC7" s="1" t="s">
+      <c r="AC7" s="65" t="s">
         <v>379</v>
       </c>
+      <c r="AD7" s="65"/>
     </row>
     <row r="8" spans="1:31" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="15" t="s">
@@ -14134,10 +14225,10 @@
         <f t="shared" si="2"/>
         <v>left</v>
       </c>
-      <c r="Q8" s="15" t="s">
+      <c r="Q8" s="64" t="s">
         <v>41</v>
       </c>
-      <c r="R8" s="15" t="s">
+      <c r="R8" s="64" t="s">
         <v>9</v>
       </c>
       <c r="S8" s="21">
@@ -14226,10 +14317,10 @@
         <f t="shared" si="2"/>
         <v>left</v>
       </c>
-      <c r="Q9" s="15" t="s">
+      <c r="Q9" s="64" t="s">
         <v>41</v>
       </c>
-      <c r="R9" s="15" t="s">
+      <c r="R9" s="64" t="s">
         <v>9</v>
       </c>
       <c r="S9" s="21">

</xml_diff>